<commit_message>
Added all inputs to the xlsx, now generates a file with correct parameters, run_sim.py creates a simulation mode from the generated xlsx and runs it, plus creates an output folder with files
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c73fb9c84d8c23a4/00 Work/01 Cement Simulation/00 Python/CA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_36ABE5CF370C2A80F16EB01432D5BA90B9716B60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1F9047F-9BB5-471C-98F7-786741967AA6}"/>
+  <xr:revisionPtr revIDLastSave="440" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F1317BE-1138-4A5D-93A9-15E3DA4B1316}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="Store" sheetId="4" r:id="rId4"/>
     <sheet name="Move" sheetId="5" r:id="rId5"/>
     <sheet name="Deliver" sheetId="6" r:id="rId6"/>
+    <sheet name="Ship_Routes" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Deliver!$A$1:$D$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="97">
   <si>
     <t>Setting</t>
   </si>
@@ -208,6 +210,15 @@
     <t>Wagga</t>
   </si>
   <si>
+    <t>Clyde</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>FA_STORE</t>
+  </si>
+  <si>
     <t>Mean Production Rate (Tons/hr)</t>
   </si>
   <si>
@@ -220,6 +231,9 @@
     <t>Unplanned downtime %</t>
   </si>
   <si>
+    <t>Consumption %</t>
+  </si>
+  <si>
     <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 36, 37, 56, 57, 58, 64, 87, 91, 92, 93, 99, 100, 106, 107, 113, 114, 119, 120, 121, 127, 128, 129, 140, 141, 142, 147, 148, 154, 155, 156, 162, 163, 169, 170, 176, 177, 182, 183, 184, 189, 190, 191, 196, 197, 198, 203, 204, 205, 206, 223, 224, 225, 226, 231, 232, 233, 238, 239, 240, 245, 246, 247, 248, 252, 253, 254, 260, 261, 262, 263, 268, 269, 275, 276, 277, 282, 283, 289, 295, 296, 301, 302, 337, 345, 351, 352, 359, 360, 361, 362, 363, 364</t>
   </si>
   <si>
@@ -260,13 +274,77 @@
   </si>
   <si>
     <t>Demand per Location</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>GBFS_STORE</t>
+  </si>
+  <si>
+    <t>GBFS</t>
+  </si>
+  <si>
+    <t>SG_STORE</t>
+  </si>
+  <si>
+    <t>Tennyson</t>
+  </si>
+  <si>
+    <t>Chullora</t>
+  </si>
+  <si>
+    <t>Loc1</t>
+  </si>
+  <si>
+    <t>Loc2</t>
+  </si>
+  <si>
+    <t>Loc3</t>
+  </si>
+  <si>
+    <t>Loc4</t>
+  </si>
+  <si>
+    <t>Loc5</t>
+  </si>
+  <si>
+    <t>Glad</t>
+  </si>
+  <si>
+    <t>Bulw</t>
+  </si>
+  <si>
+    <t>Ports</t>
+  </si>
+  <si>
+    <t>Stops</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Vessel ID</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +357,19 @@
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -319,17 +410,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -718,10 +812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +925,7 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <f t="array" ref="A3">IF(ISNA(_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,_xlfn.MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
         <v>2</v>
       </c>
@@ -1484,7 +1578,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="3"/>
@@ -1602,9 +1696,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="array" ref="A17">IF(ISNA(_xlfn.XLOOKUP(P17,$P$2:P16,$A$2:A16)),IF(COUNTIFS($P$2:P17,P17)=1,IF(COUNTIFS($C$2:C16,C17)=0,1,_xlfn.MAXIFS($A$2:A16,$C$2:C16,C17)+1),A16),_xlfn.XLOOKUP(P17,$P$2:P16,$A$2:A16))</f>
-        <v>7</v>
+      <c r="A17" s="1">
+        <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -1848,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="K21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L21" t="s">
         <v>27</v>
@@ -1903,7 +1996,7 @@
         <v>33</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22" t="s">
         <v>27</v>
@@ -2091,9 +2184,8 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="array" ref="A26">IF(ISNA(_xlfn.XLOOKUP(P26,$P$2:P25,$A$2:A25)),IF(COUNTIFS($P$2:P26,P26)=1,IF(COUNTIFS($C$2:C25,C26)=0,1,_xlfn.MAXIFS($A$2:A25,$C$2:C25,C26)+1),A25),_xlfn.XLOOKUP(P26,$P$2:P25,$A$2:A25))</f>
-        <v>6</v>
+      <c r="A26" s="1">
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
@@ -2352,7 +2444,7 @@
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" si="3"/>
@@ -2536,47 +2628,44 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
         <v>24</v>
       </c>
       <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
         <v>23</v>
-      </c>
-      <c r="G34" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" t="s">
-        <v>25</v>
       </c>
       <c r="I34" t="s">
         <v>30</v>
       </c>
       <c r="J34" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ref="M34:M64" si="4">C34&amp;F34&amp;D34&amp;E34</f>
-        <v>Bulwer IslandMakeCM10CL</v>
+        <f t="shared" ref="M34:M67" si="4">C34&amp;F34&amp;D34&amp;E34</f>
+        <v>Bulwer IslandStoreCL_STORECL</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" ref="N34:N64" si="5">I34&amp;H34&amp;J34&amp;G34</f>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM10CL</v>
       </c>
       <c r="O34">
-        <f t="shared" ref="O34:O65" si="6">COUNTIFS(M:M,N34)</f>
+        <f t="shared" ref="O34:O64" si="6">COUNTIFS(M:M,N34)</f>
         <v>1</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" ref="P34:P64" si="7">C34&amp;F34&amp;G34</f>
-        <v>Bulwer IslandMakeGP</v>
+        <f t="shared" ref="P34:P67" si="7">C34&amp;F34&amp;G34</f>
+        <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2591,39 +2680,36 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
         <v>24</v>
       </c>
       <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" t="s">
         <v>23</v>
-      </c>
-      <c r="G35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" t="s">
-        <v>25</v>
       </c>
       <c r="I35" t="s">
         <v>30</v>
       </c>
       <c r="J35" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandMakeCM11CL</v>
+        <v>Bulwer IslandStoreCL_STORECL</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM11CL</v>
       </c>
       <c r="O35">
         <f t="shared" si="6"/>
@@ -2631,13 +2717,13 @@
       </c>
       <c r="P35" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandMakeGP</v>
+        <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="array" ref="A36">IF(ISNA(_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35)),IF(COUNTIFS($P$2:P36,P36)=1,IF(COUNTIFS($C$2:C35,C36)=0,1,_xlfn.MAXIFS($A$2:A35,$C$2:C35,C36)+1),A35),_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
@@ -2646,7 +2732,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
         <v>24</v>
@@ -2671,7 +2757,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORECL</v>
+        <v>Bulwer IslandStoreCL_STORE_ICL</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="5"/>
@@ -2689,7 +2775,7 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="array" ref="A37">IF(ISNA(_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36)),IF(COUNTIFS($P$2:P37,P37)=1,IF(COUNTIFS($C$2:C36,C37)=0,1,_xlfn.MAXIFS($A$2:A36,$C$2:C36,C37)+1),A36),_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
@@ -2698,7 +2784,7 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
         <v>24</v>
@@ -2723,7 +2809,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORECL</v>
+        <v>Bulwer IslandStoreCL_STORE_ICL</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="5"/>
@@ -2741,7 +2827,7 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="array" ref="A38">IF(ISNA(_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37)),IF(COUNTIFS($P$2:P38,P38)=1,IF(COUNTIFS($C$2:C37,C38)=0,1,_xlfn.MAXIFS($A$2:A37,$C$2:C37,C38)+1),A37),_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
@@ -2750,36 +2836,39 @@
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G38" t="s">
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I38" t="s">
         <v>30</v>
       </c>
       <c r="J38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>27</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM10CL</v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandDeliverTRUCKGP</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="O38">
         <f t="shared" si="6"/>
@@ -2787,7 +2876,7 @@
       </c>
       <c r="P38" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandStoreGP</v>
+        <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2802,36 +2891,39 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s">
         <v>24</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G39" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I39" t="s">
         <v>30</v>
       </c>
       <c r="J39" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>27</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORE_ICL</v>
+        <v>Bulwer IslandMakeCM11CL</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandMakeCM10CL</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="O39">
         <f t="shared" si="6"/>
@@ -2839,13 +2931,13 @@
       </c>
       <c r="P39" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandStoreCL</v>
+        <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="array" ref="A40">IF(ISNA(_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39)),IF(COUNTIFS($P$2:P40,P40)=1,IF(COUNTIFS($C$2:C39,C40)=0,1,_xlfn.MAXIFS($A$2:A39,$C$2:C39,C40)+1),A39),_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -2854,36 +2946,36 @@
         <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F40" t="s">
         <v>25</v>
       </c>
       <c r="G40" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I40" t="s">
         <v>30</v>
       </c>
       <c r="J40" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="K40">
         <v>2</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORE_ICL</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandMakeCM11CL</v>
+        <v>Bulwer IslandDeliverTRUCKGP</v>
       </c>
       <c r="O40">
         <f t="shared" si="6"/>
@@ -2891,7 +2983,7 @@
       </c>
       <c r="P40" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandStoreCL</v>
+        <v>Bulwer IslandStoreGP</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2955,52 +3047,52 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E42" t="s">
         <v>24</v>
       </c>
       <c r="F42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" t="s">
         <v>23</v>
-      </c>
-      <c r="G42" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" t="s">
-        <v>25</v>
       </c>
       <c r="I42" t="s">
         <v>38</v>
       </c>
       <c r="J42" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="K42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" t="s">
         <v>27</v>
       </c>
       <c r="M42" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaMakeVRMCL</v>
+        <v>Port KemblaStoreCL_STORE_ICL</v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>Port KemblaMakeVRMCL</v>
       </c>
       <c r="O42">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P42" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaMakeGP</v>
+        <v>Port KemblaStoreCL</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="array" ref="A43">IF(ISNA(_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42)),IF(COUNTIFS($P$2:P43,P43)=1,IF(COUNTIFS($C$2:C42,C43)=0,1,_xlfn.MAXIFS($A$2:A42,$C$2:C42,C43)+1),#REF!),_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42))</f>
+        <f t="array" ref="A43">IF(ISNA(_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42)),IF(COUNTIFS($P$2:P43,P43)=1,IF(COUNTIFS($C$2:C42,C43)=0,1,_xlfn.MAXIFS($A$2:A42,$C$2:C42,C43)+1),A42),_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42))</f>
         <v>2</v>
       </c>
       <c r="B43" t="s">
@@ -3010,39 +3102,39 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G43" t="s">
         <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I43" t="s">
         <v>38</v>
       </c>
       <c r="J43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L43" t="s">
         <v>27</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>Port KemblaMakeVRMCL</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaMoveTRAINGP</v>
+        <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="O43">
         <f t="shared" si="6"/>
@@ -3050,7 +3142,7 @@
       </c>
       <c r="P43" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaStoreGP</v>
+        <v>Port KemblaMakeGP</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3065,25 +3157,25 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F44" t="s">
         <v>25</v>
       </c>
       <c r="G44" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I44" t="s">
         <v>38</v>
       </c>
       <c r="J44" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -3093,25 +3185,25 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaStoreCL_STORE_ICL</v>
+        <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaMakeVRMCL</v>
+        <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="O44">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaStoreCL</v>
+        <v>Port KemblaStoreGP</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),#REF!),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
-        <v>2</v>
+        <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),A44),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -3270,7 +3362,7 @@
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="array" ref="A48">IF(ISNA(_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47)),IF(COUNTIFS($P$2:P48,P48)=1,IF(COUNTIFS($C$2:C47,C48)=0,1,_xlfn.MAXIFS($A$2:A47,$C$2:C47,C48)+1),A47),_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -3279,90 +3371,89 @@
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G48" t="s">
         <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="I48" t="s">
+        <v>55</v>
+      </c>
+      <c r="J48" t="s">
+        <v>33</v>
       </c>
       <c r="K48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M48" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaDeliverTRUCKGP</v>
+        <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N48" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="O48">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P48" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaDeliverGP</v>
+        <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="array" ref="A49">IF(ISNA(_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48)),IF(COUNTIFS($P$2:P49,P49)=1,IF(COUNTIFS($C$2:C48,C49)=0,1,_xlfn.MAXIFS($A$2:A48,$C$2:C48,C49)+1),A48),_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48))</f>
-        <v>1</v>
+      <c r="A49" s="1">
+        <v>4</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G49" t="s">
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>35</v>
-      </c>
-      <c r="I49" t="s">
-        <v>39</v>
-      </c>
-      <c r="J49" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="4"/>
-        <v>NewcastleStoreGP_STOREGP</v>
+        <v>Port KemblaDeliverTRUCKGP</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="5"/>
-        <v>NewcastleDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O49">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P49" t="str">
         <f t="shared" si="7"/>
-        <v>NewcastleStoreGP</v>
+        <v>Port KemblaDeliverGP</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3410,7 +3501,7 @@
       </c>
       <c r="O50">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P50" t="str">
         <f t="shared" si="7"/>
@@ -3466,53 +3557,59 @@
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="array" ref="A52">IF(ISNA(_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51)),IF(COUNTIFS($P$2:P52,P52)=1,IF(COUNTIFS($C$2:C51,C52)=0,1,_xlfn.MAXIFS($A$2:A51,$C$2:C51,C52)+1),A51),_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" t="s">
+        <v>35</v>
+      </c>
+      <c r="I52" t="s">
+        <v>46</v>
+      </c>
+      <c r="J52" t="s">
         <v>36</v>
       </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>35</v>
-      </c>
-      <c r="G52" t="s">
-        <v>19</v>
-      </c>
-      <c r="H52" t="s">
-        <v>22</v>
-      </c>
       <c r="K52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="4"/>
-        <v>NewcastleDeliverTRUCKGP</v>
+        <v>MelbourneStoreGP_STOREGP</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="O52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P52" t="str">
         <f t="shared" si="7"/>
-        <v>NewcastleDeliverGP</v>
+        <v>MelbourneStoreGP</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="array" ref="A53">IF(ISNA(_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52)),IF(COUNTIFS($P$2:P53,P53)=1,IF(COUNTIFS($C$2:C52,C53)=0,1,_xlfn.MAXIFS($A$2:A52,$C$2:C52,C53)+1),A52),_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
@@ -3521,96 +3618,96 @@
         <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G53" t="s">
         <v>19</v>
       </c>
       <c r="H53" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" t="s">
-        <v>46</v>
-      </c>
-      <c r="J53" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="4"/>
-        <v>MelbourneStoreGP_STOREGP</v>
+        <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="5"/>
-        <v>MelbourneDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O53">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P53" t="str">
         <f t="shared" si="7"/>
-        <v>MelbourneStoreGP</v>
+        <v>MelbourneDeliverGP</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="array" ref="A54">IF(ISNA(_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53)),IF(COUNTIFS($P$2:P54,P54)=1,IF(COUNTIFS($C$2:C53,C54)=0,1,_xlfn.MAXIFS($A$2:A53,$C$2:C53,C54)+1),A53),_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" t="s">
         <v>36</v>
       </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G54" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" t="s">
-        <v>22</v>
-      </c>
       <c r="K54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="4"/>
-        <v>MelbourneDeliverTRUCKGP</v>
+        <v>OsbornStoreGP_STOREGP</v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>OsbornDeliverTRUCKGP</v>
       </c>
       <c r="O54">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P54" t="str">
         <f t="shared" si="7"/>
-        <v>MelbourneDeliverGP</v>
+        <v>OsbornStoreGP</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="array" ref="A55">IF(ISNA(_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54)),IF(COUNTIFS($P$2:P55,P55)=1,IF(COUNTIFS($C$2:C54,C55)=0,1,_xlfn.MAXIFS($A$2:A54,$C$2:C54,C55)+1),A54),_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
@@ -3619,96 +3716,96 @@
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G55" t="s">
         <v>19</v>
       </c>
       <c r="H55" t="s">
-        <v>35</v>
-      </c>
-      <c r="I55" t="s">
-        <v>47</v>
-      </c>
-      <c r="J55" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M55" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornStoreGP_STOREGP</v>
+        <v>OsbornDeliverTRUCKGP</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="5"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O55">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P55" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornStoreGP</v>
+        <v>OsbornDeliverGP</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="array" ref="A56">IF(ISNA(_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55)),IF(COUNTIFS($P$2:P56,P56)=1,IF(COUNTIFS($C$2:C55,C56)=0,1,_xlfn.MAXIFS($A$2:A55,$C$2:C55,C56)+1),A55),_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" t="s">
+        <v>35</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" t="s">
         <v>36</v>
       </c>
-      <c r="E56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" t="s">
-        <v>35</v>
-      </c>
-      <c r="G56" t="s">
-        <v>19</v>
-      </c>
-      <c r="H56" t="s">
-        <v>22</v>
-      </c>
       <c r="K56">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M56" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>TownsvilleStoreGP_STOREGP</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="O56">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P56" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornDeliverGP</v>
+        <v>TownsvilleStoreGP</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="array" ref="A57">IF(ISNA(_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56)),IF(COUNTIFS($P$2:P57,P57)=1,IF(COUNTIFS($C$2:C56,C57)=0,1,_xlfn.MAXIFS($A$2:A56,$C$2:C56,C57)+1),A56),_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
@@ -3717,96 +3814,96 @@
         <v>37</v>
       </c>
       <c r="D57" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G57" t="s">
         <v>19</v>
       </c>
       <c r="H57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I57" t="s">
-        <v>37</v>
-      </c>
-      <c r="J57" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K57">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M57" t="str">
         <f t="shared" si="4"/>
-        <v>TownsvilleStoreGP_STOREGP</v>
+        <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="5"/>
-        <v>TownsvilleDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O57">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P57" t="str">
         <f t="shared" si="7"/>
-        <v>TownsvilleStoreGP</v>
+        <v>TownsvilleDeliverGP</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="array" ref="A58">IF(ISNA(_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57)),IF(COUNTIFS($P$2:P58,P58)=1,IF(COUNTIFS($C$2:C57,C58)=0,1,_xlfn.MAXIFS($A$2:A57,$C$2:C57,C58)+1),A57),_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I58" t="s">
+        <v>40</v>
+      </c>
+      <c r="J58" t="s">
         <v>36</v>
       </c>
-      <c r="E58" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" t="s">
-        <v>35</v>
-      </c>
-      <c r="G58" t="s">
-        <v>19</v>
-      </c>
-      <c r="H58" t="s">
-        <v>22</v>
-      </c>
       <c r="K58">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M58" t="str">
         <f t="shared" si="4"/>
-        <v>TownsvilleDeliverTRUCKGP</v>
+        <v>MackayStoreGP_STOREGP</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="O58">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P58" t="str">
         <f t="shared" si="7"/>
-        <v>TownsvilleDeliverGP</v>
+        <v>MackayStoreGP</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="array" ref="A59">IF(ISNA(_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58)),IF(COUNTIFS($P$2:P59,P59)=1,IF(COUNTIFS($C$2:C58,C59)=0,1,_xlfn.MAXIFS($A$2:A58,$C$2:C58,C59)+1),A58),_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
@@ -3815,96 +3912,96 @@
         <v>40</v>
       </c>
       <c r="D59" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G59" t="s">
         <v>19</v>
       </c>
       <c r="H59" t="s">
-        <v>35</v>
-      </c>
-      <c r="I59" t="s">
-        <v>40</v>
-      </c>
-      <c r="J59" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K59">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M59" t="str">
         <f t="shared" si="4"/>
-        <v>MackayStoreGP_STOREGP</v>
+        <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="5"/>
-        <v>MackayDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O59">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P59" t="str">
         <f t="shared" si="7"/>
-        <v>MackayStoreGP</v>
+        <v>MackayDeliverGP</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="array" ref="A60">IF(ISNA(_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59)),IF(COUNTIFS($P$2:P60,P60)=1,IF(COUNTIFS($C$2:C59,C60)=0,1,_xlfn.MAXIFS($A$2:A59,$C$2:C59,C60)+1),A59),_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" t="s">
+        <v>35</v>
+      </c>
+      <c r="I60" t="s">
+        <v>54</v>
+      </c>
+      <c r="J60" t="s">
         <v>36</v>
       </c>
-      <c r="E60" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" t="s">
-        <v>35</v>
-      </c>
-      <c r="G60" t="s">
-        <v>19</v>
-      </c>
-      <c r="H60" t="s">
-        <v>22</v>
-      </c>
       <c r="K60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M60" t="str">
         <f t="shared" si="4"/>
-        <v>MackayDeliverTRUCKGP</v>
+        <v>WaggaStoreGP_STOREGP</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="O60">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60" t="str">
         <f t="shared" si="7"/>
-        <v>MackayDeliverGP</v>
+        <v>WaggaStoreGP</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="array" ref="A61">IF(ISNA(_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60)),IF(COUNTIFS($P$2:P61,P61)=1,IF(COUNTIFS($C$2:C60,C61)=0,1,_xlfn.MAXIFS($A$2:A60,$C$2:C60,C61)+1),A60),_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
@@ -3913,96 +4010,96 @@
         <v>54</v>
       </c>
       <c r="D61" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G61" t="s">
         <v>19</v>
       </c>
       <c r="H61" t="s">
-        <v>35</v>
-      </c>
-      <c r="I61" t="s">
-        <v>54</v>
-      </c>
-      <c r="J61" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K61">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M61" t="str">
         <f t="shared" si="4"/>
-        <v>WaggaStoreGP_STOREGP</v>
+        <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="5"/>
-        <v>WaggaDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O61">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P61" t="str">
         <f t="shared" si="7"/>
-        <v>WaggaStoreGP</v>
+        <v>WaggaDeliverGP</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="array" ref="A62">IF(ISNA(_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61)),IF(COUNTIFS($P$2:P62,P62)=1,IF(COUNTIFS($C$2:C61,C62)=0,1,_xlfn.MAXIFS($A$2:A61,$C$2:C61,C62)+1),A61),_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" t="s">
+        <v>35</v>
+      </c>
+      <c r="I62" t="s">
+        <v>53</v>
+      </c>
+      <c r="J62" t="s">
         <v>36</v>
       </c>
-      <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
-        <v>35</v>
-      </c>
-      <c r="G62" t="s">
-        <v>19</v>
-      </c>
-      <c r="H62" t="s">
-        <v>22</v>
-      </c>
       <c r="K62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="4"/>
-        <v>WaggaDeliverTRUCKGP</v>
+        <v>AlburyStoreGP_STOREGP</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="O62">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P62" t="str">
         <f t="shared" si="7"/>
-        <v>WaggaDeliverGP</v>
+        <v>AlburyStoreGP</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="array" ref="A63">IF(ISNA(_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62)),IF(COUNTIFS($P$2:P63,P63)=1,IF(COUNTIFS($C$2:C62,C63)=0,1,_xlfn.MAXIFS($A$2:A62,$C$2:C62,C63)+1),A62),_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
@@ -4011,166 +4108,1417 @@
         <v>53</v>
       </c>
       <c r="D63" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G63" t="s">
         <v>19</v>
       </c>
       <c r="H63" t="s">
-        <v>35</v>
-      </c>
-      <c r="I63" t="s">
-        <v>53</v>
-      </c>
-      <c r="J63" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="K63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M63" t="str">
         <f t="shared" si="4"/>
-        <v>AlburyStoreGP_STOREGP</v>
+        <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="5"/>
-        <v>AlburyDeliverTRUCKGP</v>
+        <v>NoneGP</v>
       </c>
       <c r="O63">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P63" t="str">
         <f t="shared" si="7"/>
-        <v>AlburyStoreGP</v>
+        <v>AlburyDeliverGP</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="array" ref="A64">IF(ISNA(_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63)),IF(COUNTIFS($P$2:P64,P64)=1,IF(COUNTIFS($C$2:C63,C64)=0,1,_xlfn.MAXIFS($A$2:A63,$C$2:C63,C64)+1),A63),_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" t="s">
+        <v>35</v>
+      </c>
+      <c r="I64" t="s">
+        <v>55</v>
+      </c>
+      <c r="J64" t="s">
         <v>36</v>
       </c>
-      <c r="E64" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" t="s">
-        <v>35</v>
-      </c>
-      <c r="G64" t="s">
-        <v>19</v>
-      </c>
-      <c r="H64" t="s">
-        <v>22</v>
-      </c>
       <c r="K64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M64" t="str">
         <f t="shared" si="4"/>
-        <v>AlburyDeliverTRUCKGP</v>
+        <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>ClydeDeliverTRUCKGP</v>
       </c>
       <c r="O64">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P64" t="str">
         <f t="shared" si="7"/>
-        <v>AlburyDeliverGP</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+        <v>ClydeStoreGP</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="array" ref="A65">IF(ISNA(_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64)),IF(COUNTIFS($P$2:P65,P65)=1,IF(COUNTIFS($C$2:C64,C65)=0,1,_xlfn.MAXIFS($A$2:A64,$C$2:C64,C65)+1),A64),_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64))</f>
+        <v>2</v>
+      </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G65" t="s">
         <v>19</v>
       </c>
       <c r="H65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65">
+        <v>4</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="4"/>
+        <v>ClydeDeliverTRUCKGP</v>
+      </c>
+      <c r="P65" t="str">
+        <f t="shared" si="7"/>
+        <v>ClydeDeliverGP</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" t="s">
+        <v>56</v>
+      </c>
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
+      </c>
+      <c r="J66" t="s">
+        <v>29</v>
+      </c>
+      <c r="K66">
+        <v>2</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="4"/>
+        <v>GladstoneStoreFA_STOREFA</v>
+      </c>
+      <c r="P66" t="str">
+        <f t="shared" si="7"/>
+        <v>GladstoneStoreFA</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F67" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" t="s">
+        <v>25</v>
+      </c>
+      <c r="I67" t="s">
+        <v>46</v>
+      </c>
+      <c r="J67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K67">
+        <v>3</v>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" si="4"/>
+        <v>GladstoneMoveSHIPFA</v>
+      </c>
+      <c r="P67" t="str">
+        <f t="shared" si="7"/>
+        <v>GladstoneMoveFA</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E68" t="s">
+        <v>56</v>
+      </c>
+      <c r="F68" t="s">
+        <v>28</v>
+      </c>
+      <c r="G68" t="s">
+        <v>56</v>
+      </c>
+      <c r="H68" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" t="s">
+        <v>38</v>
+      </c>
+      <c r="J68" t="s">
+        <v>57</v>
+      </c>
+      <c r="K68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" t="s">
+        <v>56</v>
+      </c>
+      <c r="F69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69" t="s">
         <v>35</v>
       </c>
-      <c r="I65" t="s">
-        <v>53</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="I69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" t="s">
         <v>36</v>
       </c>
-      <c r="K65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="K69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" t="s">
+        <v>56</v>
+      </c>
+      <c r="H70" t="s">
+        <v>35</v>
+      </c>
+      <c r="I70" t="s">
+        <v>38</v>
+      </c>
+      <c r="J70" t="s">
         <v>36</v>
       </c>
-      <c r="E66" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="K70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" t="s">
+        <v>56</v>
+      </c>
+      <c r="F71" t="s">
         <v>35</v>
       </c>
-      <c r="G66" t="s">
-        <v>19</v>
-      </c>
-      <c r="H66" t="s">
+      <c r="G71" t="s">
+        <v>56</v>
+      </c>
+      <c r="H71" t="s">
         <v>22</v>
       </c>
-      <c r="K66">
+      <c r="K71">
         <v>4</v>
       </c>
     </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>36</v>
+      </c>
+      <c r="E72" t="s">
+        <v>56</v>
+      </c>
+      <c r="F72" t="s">
+        <v>35</v>
+      </c>
+      <c r="G72" t="s">
+        <v>56</v>
+      </c>
+      <c r="H72" t="s">
+        <v>22</v>
+      </c>
+      <c r="K72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" t="s">
+        <v>79</v>
+      </c>
+      <c r="F73" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" t="s">
+        <v>79</v>
+      </c>
+      <c r="H73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" t="s">
+        <v>48</v>
+      </c>
+      <c r="J73" t="s">
+        <v>29</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" t="s">
+        <v>79</v>
+      </c>
+      <c r="F74" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" t="s">
+        <v>79</v>
+      </c>
+      <c r="H74" t="s">
+        <v>25</v>
+      </c>
+      <c r="I74" t="s">
+        <v>38</v>
+      </c>
+      <c r="J74" t="s">
+        <v>78</v>
+      </c>
+      <c r="K74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" t="s">
+        <v>48</v>
+      </c>
+      <c r="D75" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" t="s">
+        <v>79</v>
+      </c>
+      <c r="F75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" t="s">
+        <v>79</v>
+      </c>
+      <c r="H75" t="s">
+        <v>25</v>
+      </c>
+      <c r="I75" t="s">
+        <v>30</v>
+      </c>
+      <c r="J75" t="s">
+        <v>78</v>
+      </c>
+      <c r="K75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" t="s">
+        <v>79</v>
+      </c>
+      <c r="F76" t="s">
+        <v>25</v>
+      </c>
+      <c r="G76" t="s">
+        <v>79</v>
+      </c>
+      <c r="H76" t="s">
+        <v>23</v>
+      </c>
+      <c r="I76" t="s">
+        <v>38</v>
+      </c>
+      <c r="J76" t="s">
+        <v>52</v>
+      </c>
+      <c r="K76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" t="s">
+        <v>79</v>
+      </c>
+      <c r="F77" t="s">
+        <v>23</v>
+      </c>
+      <c r="G77" t="s">
+        <v>77</v>
+      </c>
+      <c r="H77" t="s">
+        <v>25</v>
+      </c>
+      <c r="I77" t="s">
+        <v>38</v>
+      </c>
+      <c r="J77" t="s">
+        <v>80</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>80</v>
+      </c>
+      <c r="E78" t="s">
+        <v>77</v>
+      </c>
+      <c r="F78" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" t="s">
+        <v>77</v>
+      </c>
+      <c r="H78" t="s">
+        <v>35</v>
+      </c>
+      <c r="I78" t="s">
+        <v>38</v>
+      </c>
+      <c r="J78" t="s">
+        <v>36</v>
+      </c>
+      <c r="K78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" t="s">
+        <v>77</v>
+      </c>
+      <c r="F79" t="s">
+        <v>35</v>
+      </c>
+      <c r="G79" t="s">
+        <v>77</v>
+      </c>
+      <c r="K79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" t="s">
+        <v>80</v>
+      </c>
+      <c r="E80" t="s">
+        <v>77</v>
+      </c>
+      <c r="F80" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" t="s">
+        <v>77</v>
+      </c>
+      <c r="H80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I80" t="s">
+        <v>38</v>
+      </c>
+      <c r="J80" t="s">
+        <v>29</v>
+      </c>
+      <c r="K80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>77</v>
+      </c>
+      <c r="C81" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" t="s">
+        <v>77</v>
+      </c>
+      <c r="F81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" t="s">
+        <v>77</v>
+      </c>
+      <c r="H81" t="s">
+        <v>28</v>
+      </c>
+      <c r="I81" t="s">
+        <v>38</v>
+      </c>
+      <c r="J81" t="s">
+        <v>34</v>
+      </c>
+      <c r="K81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>4</v>
+      </c>
+      <c r="B82" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" t="s">
+        <v>77</v>
+      </c>
+      <c r="F82" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" t="s">
+        <v>77</v>
+      </c>
+      <c r="H82" t="s">
+        <v>25</v>
+      </c>
+      <c r="I82" t="s">
+        <v>46</v>
+      </c>
+      <c r="J82" t="s">
+        <v>80</v>
+      </c>
+      <c r="K82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>4</v>
+      </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" t="s">
+        <v>77</v>
+      </c>
+      <c r="F83" t="s">
+        <v>28</v>
+      </c>
+      <c r="G83" t="s">
+        <v>77</v>
+      </c>
+      <c r="H83" t="s">
+        <v>25</v>
+      </c>
+      <c r="I83" t="s">
+        <v>55</v>
+      </c>
+      <c r="J83" t="s">
+        <v>80</v>
+      </c>
+      <c r="K83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>4</v>
+      </c>
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" t="s">
+        <v>77</v>
+      </c>
+      <c r="F84" t="s">
+        <v>28</v>
+      </c>
+      <c r="G84" t="s">
+        <v>77</v>
+      </c>
+      <c r="H84" t="s">
+        <v>25</v>
+      </c>
+      <c r="I84" t="s">
+        <v>82</v>
+      </c>
+      <c r="J84" t="s">
+        <v>80</v>
+      </c>
+      <c r="K84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>4</v>
+      </c>
+      <c r="B85" t="s">
+        <v>77</v>
+      </c>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" t="s">
+        <v>77</v>
+      </c>
+      <c r="F85" t="s">
+        <v>28</v>
+      </c>
+      <c r="G85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H85" t="s">
+        <v>25</v>
+      </c>
+      <c r="I85" t="s">
+        <v>39</v>
+      </c>
+      <c r="J85" t="s">
+        <v>80</v>
+      </c>
+      <c r="K85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" t="s">
+        <v>78</v>
+      </c>
+      <c r="E86" t="s">
+        <v>79</v>
+      </c>
+      <c r="F86" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" t="s">
+        <v>79</v>
+      </c>
+      <c r="H86" t="s">
+        <v>23</v>
+      </c>
+      <c r="I86" t="s">
+        <v>30</v>
+      </c>
+      <c r="J86" t="s">
+        <v>50</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>1</v>
+      </c>
+      <c r="B87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C87" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F87" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" t="s">
+        <v>79</v>
+      </c>
+      <c r="H87" t="s">
+        <v>23</v>
+      </c>
+      <c r="I87" t="s">
+        <v>30</v>
+      </c>
+      <c r="J87" t="s">
+        <v>51</v>
+      </c>
+      <c r="K87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>2</v>
+      </c>
+      <c r="B88" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" t="s">
+        <v>30</v>
+      </c>
+      <c r="D88" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" t="s">
+        <v>79</v>
+      </c>
+      <c r="F88" t="s">
+        <v>23</v>
+      </c>
+      <c r="G88" t="s">
+        <v>77</v>
+      </c>
+      <c r="H88" t="s">
+        <v>25</v>
+      </c>
+      <c r="I88" t="s">
+        <v>30</v>
+      </c>
+      <c r="J88" t="s">
+        <v>80</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>2</v>
+      </c>
+      <c r="B89" t="s">
+        <v>77</v>
+      </c>
+      <c r="C89" t="s">
+        <v>30</v>
+      </c>
+      <c r="D89" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>77</v>
+      </c>
+      <c r="H89" t="s">
+        <v>25</v>
+      </c>
+      <c r="I89" t="s">
+        <v>30</v>
+      </c>
+      <c r="J89" t="s">
+        <v>80</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>77</v>
+      </c>
+      <c r="C90" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" t="s">
+        <v>80</v>
+      </c>
+      <c r="E90" t="s">
+        <v>77</v>
+      </c>
+      <c r="F90" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" t="s">
+        <v>77</v>
+      </c>
+      <c r="H90" t="s">
+        <v>28</v>
+      </c>
+      <c r="I90" t="s">
+        <v>30</v>
+      </c>
+      <c r="J90" t="s">
+        <v>34</v>
+      </c>
+      <c r="K90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>77</v>
+      </c>
+      <c r="C91" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91" t="s">
+        <v>77</v>
+      </c>
+      <c r="F91" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" t="s">
+        <v>77</v>
+      </c>
+      <c r="H91" t="s">
+        <v>35</v>
+      </c>
+      <c r="I91" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" t="s">
+        <v>36</v>
+      </c>
+      <c r="K91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>77</v>
+      </c>
+      <c r="C92" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" t="s">
+        <v>77</v>
+      </c>
+      <c r="F92" t="s">
+        <v>28</v>
+      </c>
+      <c r="G92" t="s">
+        <v>77</v>
+      </c>
+      <c r="H92" t="s">
+        <v>25</v>
+      </c>
+      <c r="I92" t="s">
+        <v>81</v>
+      </c>
+      <c r="J92" t="s">
+        <v>80</v>
+      </c>
+      <c r="K92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" t="s">
+        <v>77</v>
+      </c>
+      <c r="F93" t="s">
+        <v>35</v>
+      </c>
+      <c r="G93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>1</v>
+      </c>
+      <c r="B94" t="s">
+        <v>77</v>
+      </c>
+      <c r="C94" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" t="s">
+        <v>80</v>
+      </c>
+      <c r="E94" t="s">
+        <v>77</v>
+      </c>
+      <c r="F94" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" t="s">
+        <v>77</v>
+      </c>
+      <c r="H94" t="s">
+        <v>35</v>
+      </c>
+      <c r="I94" t="s">
+        <v>81</v>
+      </c>
+      <c r="J94" t="s">
+        <v>36</v>
+      </c>
+      <c r="K94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>2</v>
+      </c>
+      <c r="B95" t="s">
+        <v>77</v>
+      </c>
+      <c r="C95" t="s">
+        <v>81</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95" t="s">
+        <v>77</v>
+      </c>
+      <c r="F95" t="s">
+        <v>35</v>
+      </c>
+      <c r="G95" t="s">
+        <v>77</v>
+      </c>
+      <c r="K95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>1</v>
+      </c>
+      <c r="B96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C96" t="s">
+        <v>46</v>
+      </c>
+      <c r="D96" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" t="s">
+        <v>77</v>
+      </c>
+      <c r="F96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" t="s">
+        <v>77</v>
+      </c>
+      <c r="H96" t="s">
+        <v>35</v>
+      </c>
+      <c r="I96" t="s">
+        <v>46</v>
+      </c>
+      <c r="J96" t="s">
+        <v>36</v>
+      </c>
+      <c r="K96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>2</v>
+      </c>
+      <c r="B97" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" t="s">
+        <v>46</v>
+      </c>
+      <c r="D97" t="s">
+        <v>36</v>
+      </c>
+      <c r="E97" t="s">
+        <v>77</v>
+      </c>
+      <c r="F97" t="s">
+        <v>35</v>
+      </c>
+      <c r="G97" t="s">
+        <v>77</v>
+      </c>
+      <c r="K97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>1</v>
+      </c>
+      <c r="B98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C98" t="s">
+        <v>55</v>
+      </c>
+      <c r="D98" t="s">
+        <v>80</v>
+      </c>
+      <c r="E98" t="s">
+        <v>77</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" t="s">
+        <v>77</v>
+      </c>
+      <c r="H98" t="s">
+        <v>35</v>
+      </c>
+      <c r="I98" t="s">
+        <v>55</v>
+      </c>
+      <c r="J98" t="s">
+        <v>36</v>
+      </c>
+      <c r="K98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>77</v>
+      </c>
+      <c r="C99" t="s">
+        <v>55</v>
+      </c>
+      <c r="D99" t="s">
+        <v>36</v>
+      </c>
+      <c r="E99" t="s">
+        <v>77</v>
+      </c>
+      <c r="F99" t="s">
+        <v>35</v>
+      </c>
+      <c r="G99" t="s">
+        <v>77</v>
+      </c>
+      <c r="K99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>1</v>
+      </c>
+      <c r="B100" t="s">
+        <v>77</v>
+      </c>
+      <c r="C100" t="s">
+        <v>82</v>
+      </c>
+      <c r="D100" t="s">
+        <v>80</v>
+      </c>
+      <c r="E100" t="s">
+        <v>77</v>
+      </c>
+      <c r="F100" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" t="s">
+        <v>77</v>
+      </c>
+      <c r="H100" t="s">
+        <v>35</v>
+      </c>
+      <c r="I100" t="s">
+        <v>82</v>
+      </c>
+      <c r="J100" t="s">
+        <v>36</v>
+      </c>
+      <c r="K100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>2</v>
+      </c>
+      <c r="B101" t="s">
+        <v>77</v>
+      </c>
+      <c r="C101" t="s">
+        <v>82</v>
+      </c>
+      <c r="D101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E101" t="s">
+        <v>77</v>
+      </c>
+      <c r="F101" t="s">
+        <v>35</v>
+      </c>
+      <c r="G101" t="s">
+        <v>77</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>1</v>
+      </c>
+      <c r="B102" t="s">
+        <v>77</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>80</v>
+      </c>
+      <c r="E102" t="s">
+        <v>77</v>
+      </c>
+      <c r="F102" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" t="s">
+        <v>77</v>
+      </c>
+      <c r="H102" t="s">
+        <v>35</v>
+      </c>
+      <c r="I102" t="s">
+        <v>39</v>
+      </c>
+      <c r="J102" t="s">
+        <v>36</v>
+      </c>
+      <c r="K102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>2</v>
+      </c>
+      <c r="B103" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" t="s">
+        <v>36</v>
+      </c>
+      <c r="E103" t="s">
+        <v>77</v>
+      </c>
+      <c r="F103" t="s">
+        <v>35</v>
+      </c>
+      <c r="G103" t="s">
+        <v>77</v>
+      </c>
+      <c r="K103">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:K66" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:K104" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="M1:N1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4180,11 +5528,12 @@
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4195,19 +5544,22 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -4218,200 +5570,305 @@
         <v>24</v>
       </c>
       <c r="D2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G2">
         <v>3.3000000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D3">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G3">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="D4">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G4">
-        <v>0.1646</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D5">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G5">
-        <v>0.13189999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>226</v>
+        <v>103</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G6">
-        <v>7.4499999999999997E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1646</v>
+      </c>
+      <c r="H6">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7">
-        <v>205</v>
+        <v>118</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="D8">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G8">
-        <v>5.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G9">
-        <v>0.1101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="H9">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D10">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G10">
+        <v>0.05</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12">
+        <v>0.1101</v>
+      </c>
+      <c r="H12">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13">
+        <v>150</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13">
         <v>2.98E-2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4421,16 +5878,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -4448,13 +5905,13 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4467,6 +5924,15 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
+      <c r="D2">
+        <v>99999</v>
+      </c>
+      <c r="E2">
+        <v>50000</v>
+      </c>
+      <c r="F2">
+        <v>20000</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4530,98 +5996,107 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="D6">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="E6">
-        <v>15000</v>
+        <v>40000</v>
       </c>
       <c r="F6">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="D7">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="E7">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="F7">
-        <v>30000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D8">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E8">
         <v>30000</v>
       </c>
       <c r="F8">
-        <v>15000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>999999</v>
+        <v>30000</v>
       </c>
       <c r="E9">
-        <v>999999</v>
+        <v>25000</v>
       </c>
       <c r="F9">
-        <v>999999</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+      <c r="E10">
+        <v>10000</v>
+      </c>
+      <c r="F10">
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -4630,95 +6105,104 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="E11">
-        <v>35000</v>
+        <v>15000</v>
       </c>
       <c r="F11">
-        <v>8000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>27000</v>
+        <v>60000</v>
       </c>
       <c r="E12">
-        <v>27000</v>
+        <v>60000</v>
       </c>
       <c r="F12">
-        <v>2500</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>999999</v>
+      </c>
+      <c r="E13">
+        <v>999999</v>
+      </c>
+      <c r="F13">
+        <v>999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D14">
-        <v>86000</v>
+        <v>30000</v>
       </c>
       <c r="E14">
-        <v>86000</v>
+        <v>30000</v>
       </c>
       <c r="F14">
-        <v>25000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>20000</v>
+        <v>999999</v>
       </c>
       <c r="E15">
-        <v>20000</v>
+        <v>999999</v>
       </c>
       <c r="F15">
-        <v>15000</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>999999</v>
@@ -4732,18 +6216,27 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="D17">
+        <v>50000</v>
+      </c>
+      <c r="E17">
+        <v>40000</v>
+      </c>
+      <c r="F17">
+        <v>20000</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -4752,24 +6245,313 @@
         <v>19</v>
       </c>
       <c r="D18">
-        <v>30000</v>
+        <v>99999</v>
       </c>
       <c r="E18">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F18">
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
+      </c>
+      <c r="D19">
+        <v>35000</v>
+      </c>
+      <c r="E19">
+        <v>35000</v>
+      </c>
+      <c r="F19">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20">
+        <v>25000</v>
+      </c>
+      <c r="E20">
+        <v>25000</v>
+      </c>
+      <c r="F20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>27000</v>
+      </c>
+      <c r="E21">
+        <v>27000</v>
+      </c>
+      <c r="F21">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
+      </c>
+      <c r="F22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>99999</v>
+      </c>
+      <c r="E23">
+        <v>50000</v>
+      </c>
+      <c r="F23">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>86000</v>
+      </c>
+      <c r="E24">
+        <v>86000</v>
+      </c>
+      <c r="F24">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25">
+        <v>8000</v>
+      </c>
+      <c r="F25">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>50000</v>
+      </c>
+      <c r="E26">
+        <v>50000</v>
+      </c>
+      <c r="F26">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>20000</v>
+      </c>
+      <c r="E27">
+        <v>20000</v>
+      </c>
+      <c r="F27">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28">
+        <v>20000</v>
+      </c>
+      <c r="E28">
+        <v>20000</v>
+      </c>
+      <c r="F28">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <v>999999</v>
+      </c>
+      <c r="E29">
+        <v>999999</v>
+      </c>
+      <c r="F29">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <v>99999</v>
+      </c>
+      <c r="E30">
+        <v>99999</v>
+      </c>
+      <c r="F30">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31">
+        <v>10000</v>
+      </c>
+      <c r="E31">
+        <v>10000</v>
+      </c>
+      <c r="F31">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>30000</v>
+      </c>
+      <c r="E32">
+        <v>30000</v>
+      </c>
+      <c r="F32">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>99999</v>
+      </c>
+      <c r="E33">
+        <v>50000</v>
+      </c>
+      <c r="F33">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
@@ -4791,16 +6573,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4808,18 +6594,26 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>8707/(364*24)</f>
+        <v>0.99668040293040294</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2*364*24</f>
+        <v>8707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -4827,108 +6621,525 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>7.78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>632953/(364*24)</f>
+        <v>72.453411172161168</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D23" si="0">C3*364*24</f>
+        <v>632953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <f>271783/(364*24)</f>
+        <v>31.110691391941391</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>271783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <f>43297/(364*24)</f>
+        <v>4.9561584249084252</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>43297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <f>75000/(364*24)</f>
+        <v>8.5851648351648358</v>
+      </c>
+      <c r="D6" s="3">
+        <f>C6*364*24</f>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7">
+        <f>82348/(364*24)</f>
+        <v>9.4262820512820511</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>82348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>34.909999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <f>273496/(364*24)</f>
+        <v>31.306776556776558</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>273496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <f>32346/(364*24)</f>
+        <v>3.7026098901098901</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>32346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>96.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <f>843403/(364*24)</f>
+        <v>96.543383699633694</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>843403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <f>413226/(364*24)</f>
+        <v>47.301510989010985</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>413226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12">
+        <f>426604/(364*24)</f>
+        <v>48.83287545787546</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>426604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>4.46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <f>200000/(364*24)</f>
+        <v>22.893772893772894</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <f>29812/(364*24)</f>
+        <v>3.4125457875457874</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>29811.999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>15.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <f>139033/(364*24)</f>
+        <v>15.914949633699633</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>139033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16">
+        <f>63707/(364*24)</f>
+        <v>7.2924679487179489</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16" si="1">C16*364*24</f>
+        <v>63707</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>40.18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <f>810842/(364*24)</f>
+        <v>92.816163003663007</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>810842</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <f>315900/(364*24)</f>
+        <v>36.160714285714285</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>315900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19">
+        <f>366601/(364*24)</f>
+        <v>41.964400183150182</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>366601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>19.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>171055/(364*24)</f>
+        <v>19.580471611721613</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>171055</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21">
+        <f>106550/(364*24)</f>
+        <v>12.196657509157509</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>106550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>48.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f>420346/(364*24)</f>
+        <v>48.116529304029307</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>420346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <f>1395/(364*24)</f>
+        <v>0.15968406593406592</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>1394.9999999999998</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D23" xr:uid="{00000000-0001-0000-0500-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -5183,34 +7394,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{961C2B7A-B291-4292-A6D6-F3946C520675}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57379405-3584-4520-B492-BEDAAFE9CA45}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85BCBB88-E525-4101-BD7A-D7100E5A6AD8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
11 DEC WIP - Debugging SIMPY
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="629" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ADA8D9B-C862-4168-9370-96B025B8DE20}"/>
+  <xr:revisionPtr revIDLastSave="707" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09C537E5-CEA7-417D-B7FD-5931EDD581E8}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="0" windowWidth="24615" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38610" yWindow="7440" windowWidth="25185" windowHeight="21750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Deliver!$A$1:$D$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$105</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2284" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="188">
   <si>
     <t>Setting</t>
   </si>
@@ -544,9 +566,6 @@
     <t>Confirm With Peter</t>
   </si>
   <si>
-    <t>load rate 1000t/h</t>
-  </si>
-  <si>
     <t>Unconstrained for this model, can load instantly</t>
   </si>
   <si>
@@ -593,6 +612,24 @@
   </si>
   <si>
     <t>Travel back Time (Min)</t>
+  </si>
+  <si>
+    <t>Silo S&amp;T</t>
+  </si>
+  <si>
+    <t>load rate 1000t/h, Silo Z</t>
+  </si>
+  <si>
+    <t>=IF(ISNA(XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),XLOOKUP(P3,$P$2:P2,$A$2:A2))</t>
+  </si>
+  <si>
+    <t>GP_STORE_ST</t>
+  </si>
+  <si>
+    <t>GP_STORE_Q</t>
+  </si>
+  <si>
+    <t>Silo Q</t>
   </si>
 </sst>
 </file>
@@ -689,7 +726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,6 +739,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1093,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q103"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1147,7 @@
     <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1150,7 +1188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1205,8 +1243,8 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" cm="1">
         <f t="array" ref="A3">IF(ISNA(_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,_xlfn.MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
         <v>2</v>
       </c>
@@ -1260,9 +1298,12 @@
         <v>GladstoneStoreCL</v>
       </c>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="S3" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" cm="1">
         <f t="array" ref="A4">IF(ISNA(_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3)),IF(COUNTIFS($P$2:P4,P4)=1,IF(COUNTIFS($C$2:C3,C4)=0,1,_xlfn.MAXIFS($A$2:A3,$C$2:C3,C4)+1),A3),_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3))</f>
         <v>3</v>
       </c>
@@ -1316,8 +1357,8 @@
         <v>GladstoneMoveCL</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" cm="1">
         <f t="array" ref="A5">IF(ISNA(_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4)),IF(COUNTIFS($P$2:P5,P5)=1,IF(COUNTIFS($C$2:C4,C5)=0,1,_xlfn.MAXIFS($A$2:A4,$C$2:C4,C5)+1),A4),_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4))</f>
         <v>2</v>
       </c>
@@ -1371,8 +1412,8 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" cm="1">
         <f t="array" ref="A6">IF(ISNA(_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5)),IF(COUNTIFS($P$2:P6,P6)=1,IF(COUNTIFS($C$2:C5,C6)=0,1,_xlfn.MAXIFS($A$2:A5,$C$2:C5,C6)+1),A5),_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5))</f>
         <v>2</v>
       </c>
@@ -1426,8 +1467,8 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" cm="1">
         <f t="array" ref="A7">IF(ISNA(_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6)),IF(COUNTIFS($P$2:P7,P7)=1,IF(COUNTIFS($C$2:C6,C7)=0,1,_xlfn.MAXIFS($A$2:A6,$C$2:C6,C7)+1),A6),_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6))</f>
         <v>4</v>
       </c>
@@ -1481,8 +1522,8 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" cm="1">
         <f t="array" ref="A8">IF(ISNA(_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7)),IF(COUNTIFS($P$2:P8,P8)=1,IF(COUNTIFS($C$2:C7,C8)=0,1,_xlfn.MAXIFS($A$2:A7,$C$2:C7,C8)+1),A7),_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7))</f>
         <v>4</v>
       </c>
@@ -1536,8 +1577,8 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" cm="1">
         <f t="array" ref="A9">IF(ISNA(_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8)),IF(COUNTIFS($P$2:P9,P9)=1,IF(COUNTIFS($C$2:C8,C9)=0,1,_xlfn.MAXIFS($A$2:A8,$C$2:C8,C9)+1),A8),_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8))</f>
         <v>5</v>
       </c>
@@ -1591,8 +1632,8 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" cm="1">
         <f t="array" ref="A10">IF(ISNA(_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9)),IF(COUNTIFS($P$2:P10,P10)=1,IF(COUNTIFS($C$2:C9,C10)=0,1,_xlfn.MAXIFS($A$2:A9,$C$2:C9,C10)+1),A9),_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9))</f>
         <v>5</v>
       </c>
@@ -1646,8 +1687,8 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" cm="1">
         <f t="array" ref="A11">IF(ISNA(_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10)),IF(COUNTIFS($P$2:P11,P11)=1,IF(COUNTIFS($C$2:C10,C11)=0,1,_xlfn.MAXIFS($A$2:A10,$C$2:C10,C11)+1),A10),_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10))</f>
         <v>5</v>
       </c>
@@ -1701,8 +1742,8 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" cm="1">
         <f t="array" ref="A12">IF(ISNA(_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11)),IF(COUNTIFS($P$2:P12,P12)=1,IF(COUNTIFS($C$2:C11,C12)=0,1,_xlfn.MAXIFS($A$2:A11,$C$2:C11,C12)+1),A11),_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11))</f>
         <v>6</v>
       </c>
@@ -1756,8 +1797,8 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" cm="1">
         <f t="array" ref="A13">IF(ISNA(_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12)),IF(COUNTIFS($P$2:P13,P13)=1,IF(COUNTIFS($C$2:C12,C13)=0,1,_xlfn.MAXIFS($A$2:A12,$C$2:C12,C13)+1),A12),_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12))</f>
         <v>6</v>
       </c>
@@ -1811,8 +1852,8 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" cm="1">
         <f t="array" ref="A14">IF(ISNA(_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13)),IF(COUNTIFS($P$2:P14,P14)=1,IF(COUNTIFS($C$2:C13,C14)=0,1,_xlfn.MAXIFS($A$2:A13,$C$2:C13,C14)+1),A13),_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13))</f>
         <v>6</v>
       </c>
@@ -1866,8 +1907,8 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" cm="1">
         <f t="array" ref="A15">IF(ISNA(_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14)),IF(COUNTIFS($P$2:P15,P15)=1,IF(COUNTIFS($C$2:C14,C15)=0,1,_xlfn.MAXIFS($A$2:A14,$C$2:C14,C15)+1),A14),_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14))</f>
         <v>6</v>
       </c>
@@ -1921,8 +1962,8 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" cm="1">
         <f t="array" ref="A16">IF(ISNA(_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15)),IF(COUNTIFS($P$2:P16,P16)=1,IF(COUNTIFS($C$2:C15,C16)=0,1,_xlfn.MAXIFS($A$2:A15,$C$2:C15,C16)+1),A15),_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15))</f>
         <v>6</v>
       </c>
@@ -1998,9 +2039,6 @@
       <c r="G17" t="s">
         <v>19</v>
       </c>
-      <c r="H17" t="s">
-        <v>22</v>
-      </c>
       <c r="K17">
         <v>4</v>
       </c>
@@ -2013,7 +2051,7 @@
       </c>
       <c r="N17" t="str">
         <f t="shared" si="1"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
@@ -2025,7 +2063,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" cm="1">
         <f t="array" ref="A18">IF(ISNA(_xlfn.XLOOKUP(P18,$P$2:P17,$A$2:A17)),IF(COUNTIFS($P$2:P18,P18)=1,IF(COUNTIFS($C$2:C17,C18)=0,1,_xlfn.MAXIFS($A$2:A17,$C$2:C17,C18)+1),A17),_xlfn.XLOOKUP(P18,$P$2:P17,$A$2:A17))</f>
         <v>1</v>
       </c>
@@ -2080,7 +2118,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" cm="1">
         <f t="array" ref="A19">IF(ISNA(_xlfn.XLOOKUP(P19,$P$2:P18,$A$2:A18)),IF(COUNTIFS($P$2:P19,P19)=1,IF(COUNTIFS($C$2:C18,C19)=0,1,_xlfn.MAXIFS($A$2:A18,$C$2:C18,C19)+1),A18),_xlfn.XLOOKUP(P19,$P$2:P18,$A$2:A18))</f>
         <v>2</v>
       </c>
@@ -2127,7 +2165,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="3"/>
@@ -2135,7 +2173,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" cm="1">
         <f t="array" ref="A20">IF(ISNA(_xlfn.XLOOKUP(P20,$P$2:P19,$A$2:A19)),IF(COUNTIFS($P$2:P20,P20)=1,IF(COUNTIFS($C$2:C19,C20)=0,1,_xlfn.MAXIFS($A$2:A19,$C$2:C19,C20)+1),A19),_xlfn.XLOOKUP(P20,$P$2:P19,$A$2:A19))</f>
         <v>2</v>
       </c>
@@ -2182,7 +2220,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="3"/>
@@ -2190,7 +2228,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" cm="1">
         <f t="array" ref="A21">IF(ISNA(_xlfn.XLOOKUP(P21,$P$2:P20,$A$2:A20)),IF(COUNTIFS($P$2:P21,P21)=1,IF(COUNTIFS($C$2:C20,C21)=0,1,_xlfn.MAXIFS($A$2:A20,$C$2:C20,C21)+1),A20),_xlfn.XLOOKUP(P21,$P$2:P20,$A$2:A20))</f>
         <v>3</v>
       </c>
@@ -2219,7 +2257,7 @@
         <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2233,11 +2271,11 @@
       </c>
       <c r="N21" t="str">
         <f t="shared" si="1"/>
-        <v>RailtonStoreGP_STOREGP</v>
+        <v>RailtonStoreGP_STORE_STGP</v>
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="3"/>
@@ -2245,7 +2283,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" cm="1">
         <f t="array" ref="A22">IF(ISNA(_xlfn.XLOOKUP(P22,$P$2:P21,$A$2:A21)),IF(COUNTIFS($P$2:P22,P22)=1,IF(COUNTIFS($C$2:C21,C22)=0,1,_xlfn.MAXIFS($A$2:A21,$C$2:C21,C22)+1),A21),_xlfn.XLOOKUP(P22,$P$2:P21,$A$2:A21))</f>
         <v>3</v>
       </c>
@@ -2274,7 +2312,7 @@
         <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2288,11 +2326,11 @@
       </c>
       <c r="N22" t="str">
         <f t="shared" si="1"/>
-        <v>RailtonStoreGP_STOREGP</v>
+        <v>RailtonStoreGP_STORE_STGP</v>
       </c>
       <c r="O22">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P22" t="str">
         <f t="shared" si="3"/>
@@ -2300,9 +2338,9 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" cm="1">
         <f t="array" ref="A23">IF(ISNA(_xlfn.XLOOKUP(P23,$P$2:P22,$A$2:A22)),IF(COUNTIFS($P$2:P23,P23)=1,IF(COUNTIFS($C$2:C22,C23)=0,1,_xlfn.MAXIFS($A$2:A22,$C$2:C22,C23)+1),A22),_xlfn.XLOOKUP(P23,$P$2:P22,$A$2:A22))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -2311,39 +2349,39 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" t="s">
         <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" t="s">
-        <v>35</v>
       </c>
       <c r="I23" t="s">
         <v>41</v>
       </c>
       <c r="J23" t="s">
-        <v>36</v>
+        <v>186</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L23" t="s">
         <v>27</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
-        <v>RailtonStoreGP_STOREGP</v>
+        <v>RailtonMakeCM4CL</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="1"/>
-        <v>RailtonDeliverTRUCKGP</v>
+        <v>RailtonStoreGP_STORE_QGP</v>
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
@@ -2351,13 +2389,13 @@
       </c>
       <c r="P23" t="str">
         <f t="shared" si="3"/>
-        <v>RailtonStoreGP</v>
+        <v>RailtonMakeGP</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" cm="1">
         <f t="array" ref="A24">IF(ISNA(_xlfn.XLOOKUP(P24,$P$2:P23,$A$2:A23)),IF(COUNTIFS($P$2:P24,P24)=1,IF(COUNTIFS($C$2:C23,C24)=0,1,_xlfn.MAXIFS($A$2:A23,$C$2:C23,C24)+1),A23),_xlfn.XLOOKUP(P24,$P$2:P23,$A$2:A23))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -2366,39 +2404,39 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" t="s">
         <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" t="s">
-        <v>28</v>
       </c>
       <c r="I24" t="s">
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L24" t="s">
         <v>27</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
-        <v>RailtonStoreGP_STOREGP</v>
+        <v>RailtonMakeCM5CL</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="1"/>
-        <v>RailtonMoveTRAINGP</v>
+        <v>RailtonStoreGP_STORE_QGP</v>
       </c>
       <c r="O24">
         <f t="shared" si="2"/>
@@ -2406,13 +2444,13 @@
       </c>
       <c r="P24" t="str">
         <f t="shared" si="3"/>
-        <v>RailtonStoreGP</v>
+        <v>RailtonMakeGP</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" cm="1">
         <f t="array" ref="A25">IF(ISNA(_xlfn.XLOOKUP(P25,$P$2:P24,$A$2:A24)),IF(COUNTIFS($P$2:P25,P25)=1,IF(COUNTIFS($C$2:C24,C25)=0,1,_xlfn.MAXIFS($A$2:A24,$C$2:C24,C25)+1),A24),_xlfn.XLOOKUP(P25,$P$2:P24,$A$2:A24))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -2421,39 +2459,39 @@
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
         <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L25" t="s">
         <v>27</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
-        <v>RailtonMoveTRAINGP</v>
+        <v>RailtonStoreGP_STORE_QGP</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="1"/>
-        <v>DevonportStoreGP_STOREGP</v>
+        <v>RailtonDeliverTRUCKGP</v>
       </c>
       <c r="O25">
         <f t="shared" si="2"/>
@@ -2461,12 +2499,13 @@
       </c>
       <c r="P25" t="str">
         <f t="shared" si="3"/>
-        <v>RailtonMoveGP</v>
+        <v>RailtonStoreGP</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>5</v>
+      <c r="A26" cm="1">
+        <f t="array" ref="A26">IF(ISNA(_xlfn.XLOOKUP(P26,$P$2:P25,$A$2:A25)),IF(COUNTIFS($P$2:P26,P26)=1,IF(COUNTIFS($C$2:C25,C26)=0,1,_xlfn.MAXIFS($A$2:A25,$C$2:C25,C26)+1),A25),_xlfn.XLOOKUP(P26,$P$2:P25,$A$2:A25))</f>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
@@ -2475,157 +2514,153 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>185</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G26" t="s">
         <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
       </c>
       <c r="K26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L26" t="s">
         <v>27</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
-        <v>RailtonDeliverTRUCKGP</v>
+        <v>RailtonStoreGP_STORE_STGP</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
-        <v>NoneGP</v>
+        <v>RailtonMoveTRAINGP</v>
       </c>
       <c r="O26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="3"/>
-        <v>RailtonDeliverGP</v>
+        <v>RailtonStoreGP</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" cm="1">
         <f t="array" ref="A27">IF(ISNA(_xlfn.XLOOKUP(P27,$P$2:P26,$A$2:A26)),IF(COUNTIFS($P$2:P27,P27)=1,IF(COUNTIFS($C$2:C26,C27)=0,1,_xlfn.MAXIFS($A$2:A26,$C$2:C26,C27)+1),A26),_xlfn.XLOOKUP(P27,$P$2:P26,$A$2:A26))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" t="s">
         <v>25</v>
-      </c>
-      <c r="G27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" t="s">
-        <v>28</v>
       </c>
       <c r="I27" t="s">
         <v>98</v>
       </c>
       <c r="J27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L27" t="s">
         <v>27</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
-        <v>DevonportStoreGP_STOREGP</v>
+        <v>RailtonMoveTRAINGP</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="1"/>
-        <v>DevonportMoveSHIPGP</v>
+        <v>DevonportStoreGP_STOREGP</v>
       </c>
       <c r="O27">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" si="3"/>
-        <v>DevonportStoreGP</v>
+        <v>RailtonMoveGP</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="array" ref="A28">IF(ISNA(_xlfn.XLOOKUP(P28,$P$2:P27,$A$2:A27)),IF(COUNTIFS($P$2:P28,P28)=1,IF(COUNTIFS($C$2:C27,C28)=0,1,_xlfn.MAXIFS($A$2:A27,$C$2:C27,C28)+1),A27),_xlfn.XLOOKUP(P28,$P$2:P27,$A$2:A27))</f>
-        <v>2</v>
+      <c r="A28" s="1">
+        <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
         <v>19</v>
       </c>
-      <c r="H28" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" t="s">
-        <v>45</v>
-      </c>
-      <c r="J28" t="s">
-        <v>33</v>
-      </c>
       <c r="K28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L28" t="s">
         <v>27</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
-        <v>DevonportMoveSHIPGP</v>
+        <v>RailtonDeliverTRUCKGP</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="1"/>
-        <v>MelbourneStoreGP_STOREGP</v>
+        <v>GP</v>
       </c>
       <c r="O28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" si="3"/>
-        <v>DevonportMoveGP</v>
+        <v>RailtonDeliverGP</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" cm="1">
         <f t="array" ref="A29">IF(ISNA(_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28)),IF(COUNTIFS($P$2:P29,P29)=1,IF(COUNTIFS($C$2:C28,C29)=0,1,_xlfn.MAXIFS($A$2:A28,$C$2:C28,C29)+1),A28),_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -2634,51 +2669,51 @@
         <v>98</v>
       </c>
       <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>98</v>
+      </c>
+      <c r="J29" t="s">
         <v>29</v>
       </c>
-      <c r="E29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" t="s">
-        <v>46</v>
-      </c>
-      <c r="J29" t="s">
-        <v>33</v>
-      </c>
       <c r="K29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L29" t="s">
         <v>27</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
-        <v>DevonportMoveSHIPGP</v>
+        <v>DevonportStoreGP_STOREGP</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="1"/>
-        <v>OsbornStoreGP_STOREGP</v>
+        <v>DevonportMoveSHIPGP</v>
       </c>
       <c r="O29">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" si="3"/>
-        <v>DevonportMoveGP</v>
+        <v>DevonportStoreGP</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" cm="1">
         <f t="array" ref="A30">IF(ISNA(_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29)),IF(COUNTIFS($P$2:P30,P30)=1,IF(COUNTIFS($C$2:C29,C30)=0,1,_xlfn.MAXIFS($A$2:A29,$C$2:C29,C30)+1),A29),_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29))</f>
         <v>2</v>
       </c>
@@ -2704,7 +2739,7 @@
         <v>25</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J30" t="s">
         <v>33</v>
@@ -2721,7 +2756,7 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="1"/>
-        <v>NewcastleStoreGP_STOREGP</v>
+        <v>MelbourneStoreGP_STOREGP</v>
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
@@ -2733,62 +2768,62 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" cm="1">
         <f t="array" ref="A31">IF(ISNA(_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30)),IF(COUNTIFS($P$2:P31,P31)=1,IF(COUNTIFS($C$2:C30,C31)=0,1,_xlfn.MAXIFS($A$2:A30,$C$2:C30,C31)+1),A30),_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" t="s">
         <v>25</v>
       </c>
-      <c r="G31" t="s">
-        <v>24</v>
-      </c>
-      <c r="H31" t="s">
-        <v>28</v>
-      </c>
       <c r="I31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L31" t="s">
         <v>27</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
-        <v>ImportStoreCL_STORECL</v>
+        <v>DevonportMoveSHIPGP</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="1"/>
-        <v>ImportMoveSHIPCL</v>
+        <v>OsbornStoreGP_STOREGP</v>
       </c>
       <c r="O31">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P31" t="str">
         <f t="shared" si="3"/>
-        <v>ImportStoreCL</v>
+        <v>DevonportMoveGP</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" cm="1">
         <f t="array" ref="A32">IF(ISNA(_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31)),IF(COUNTIFS($P$2:P32,P32)=1,IF(COUNTIFS($C$2:C31,C32)=0,1,_xlfn.MAXIFS($A$2:A31,$C$2:C31,C32)+1),A31),_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31))</f>
         <v>2</v>
       </c>
@@ -2796,28 +2831,28 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F32" t="s">
         <v>28</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J32" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K32">
         <v>3</v>
@@ -2827,25 +2862,25 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
-        <v>ImportMoveSHIPCL</v>
+        <v>DevonportMoveSHIPGP</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="1"/>
-        <v>Port KemblaMoveCL_STORE_ICL</v>
+        <v>NewcastleStoreGP_STOREGP</v>
       </c>
       <c r="O32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="3"/>
-        <v>ImportMoveCL</v>
+        <v>DevonportMoveGP</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" cm="1">
         <f t="array" ref="A33">IF(ISNA(_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32)),IF(COUNTIFS($P$2:P33,P33)=1,IF(COUNTIFS($C$2:C32,C33)=0,1,_xlfn.MAXIFS($A$2:A32,$C$2:C32,C33)+1),A32),_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -2854,13 +2889,13 @@
         <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -2869,76 +2904,76 @@
         <v>28</v>
       </c>
       <c r="I33" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="J33" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="K33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L33" t="s">
         <v>27</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
-        <v>ImportMoveSHIPCL</v>
+        <v>ImportStoreCL_STORECL</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="1"/>
-        <v>Bulwer IslandMoveCL_STORE_ICL</v>
+        <v>ImportMoveSHIPCL</v>
       </c>
       <c r="O33">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P33" t="str">
         <f t="shared" si="3"/>
-        <v>ImportMoveCL</v>
+        <v>ImportStoreCL</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" cm="1">
         <f t="array" ref="A34">IF(ISNA(_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33)),IF(COUNTIFS($P$2:P34,P34)=1,IF(COUNTIFS($C$2:C33,C34)=0,1,_xlfn.MAXIFS($A$2:A33,$C$2:C33,C34)+1),A33),_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
         <v>24</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I34" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ref="M34:M67" si="4">C34&amp;F34&amp;D34&amp;E34</f>
-        <v>Bulwer IslandStoreCL_STORECL</v>
+        <v>ImportMoveSHIPCL</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" ref="N34:N64" si="5">I34&amp;H34&amp;J34&amp;G34</f>
-        <v>Bulwer IslandMakeCM10CL</v>
+        <v>Port KemblaStoreCL_STORE_ICL</v>
       </c>
       <c r="O34">
         <f t="shared" ref="O34:O64" si="6">COUNTIFS(M:M,N34)</f>
@@ -2946,63 +2981,63 @@
       </c>
       <c r="P34" t="str">
         <f t="shared" ref="P34:P67" si="7">C34&amp;F34&amp;G34</f>
-        <v>Bulwer IslandStoreCL</v>
+        <v>ImportMoveCL</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" cm="1">
         <f t="array" ref="A35">IF(ISNA(_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34)),IF(COUNTIFS($P$2:P35,P35)=1,IF(COUNTIFS($C$2:C34,C35)=0,1,_xlfn.MAXIFS($A$2:A34,$C$2:C34,C35)+1),A34),_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
         <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
       </c>
       <c r="H35" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I35" t="s">
         <v>30</v>
       </c>
       <c r="J35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORECL</v>
+        <v>ImportMoveSHIPCL</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandMakeCM11CL</v>
+        <v>Bulwer IslandStoreCL_STORE_ICL</v>
       </c>
       <c r="O35">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandStoreCL</v>
+        <v>ImportMoveCL</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" cm="1">
         <f t="array" ref="A36">IF(ISNA(_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35)),IF(COUNTIFS($P$2:P36,P36)=1,IF(COUNTIFS($C$2:C35,C36)=0,1,_xlfn.MAXIFS($A$2:A35,$C$2:C35,C36)+1),A35),_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35))</f>
         <v>1</v>
       </c>
@@ -3013,7 +3048,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E36" t="s">
         <v>24</v>
@@ -3038,7 +3073,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORE_ICL</v>
+        <v>Bulwer IslandStoreCL_STORECL</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="5"/>
@@ -3054,7 +3089,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" cm="1">
         <f t="array" ref="A37">IF(ISNA(_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36)),IF(COUNTIFS($P$2:P37,P37)=1,IF(COUNTIFS($C$2:C36,C37)=0,1,_xlfn.MAXIFS($A$2:A36,$C$2:C36,C37)+1),A36),_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36))</f>
         <v>1</v>
       </c>
@@ -3065,7 +3100,7 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
         <v>24</v>
@@ -3090,7 +3125,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreCL_STORE_ICL</v>
+        <v>Bulwer IslandStoreCL_STORECL</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="5"/>
@@ -3106,9 +3141,9 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" cm="1">
         <f t="array" ref="A38">IF(ISNA(_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37)),IF(COUNTIFS($P$2:P38,P38)=1,IF(COUNTIFS($C$2:C37,C38)=0,1,_xlfn.MAXIFS($A$2:A37,$C$2:C37,C38)+1),A37),_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
@@ -3117,39 +3152,39 @@
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
       </c>
       <c r="F38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" t="s">
         <v>23</v>
-      </c>
-      <c r="G38" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" t="s">
-        <v>25</v>
       </c>
       <c r="I38" t="s">
         <v>30</v>
       </c>
       <c r="J38" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L38" t="s">
         <v>27</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandMakeCM10CL</v>
+        <v>Bulwer IslandStoreCL_STORE_ICL</v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM10CL</v>
       </c>
       <c r="O38">
         <f t="shared" si="6"/>
@@ -3157,13 +3192,13 @@
       </c>
       <c r="P38" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandMakeGP</v>
+        <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" cm="1">
         <f t="array" ref="A39">IF(ISNA(_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38)),IF(COUNTIFS($P$2:P39,P39)=1,IF(COUNTIFS($C$2:C38,C39)=0,1,_xlfn.MAXIFS($A$2:A38,$C$2:C38,C39)+1),A38),_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -3172,39 +3207,39 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
         <v>24</v>
       </c>
       <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
         <v>23</v>
-      </c>
-      <c r="G39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" t="s">
-        <v>25</v>
       </c>
       <c r="I39" t="s">
         <v>30</v>
       </c>
       <c r="J39" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L39" t="s">
         <v>27</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandMakeCM11CL</v>
+        <v>Bulwer IslandStoreCL_STORE_ICL</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM11CL</v>
       </c>
       <c r="O39">
         <f t="shared" si="6"/>
@@ -3212,13 +3247,13 @@
       </c>
       <c r="P39" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandMakeGP</v>
+        <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" cm="1">
         <f t="array" ref="A40">IF(ISNA(_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39)),IF(COUNTIFS($P$2:P40,P40)=1,IF(COUNTIFS($C$2:C39,C40)=0,1,_xlfn.MAXIFS($A$2:A39,$C$2:C39,C40)+1),A39),_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -3227,36 +3262,36 @@
         <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" t="s">
         <v>25</v>
-      </c>
-      <c r="G40" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" t="s">
-        <v>35</v>
       </c>
       <c r="I40" t="s">
         <v>30</v>
       </c>
       <c r="J40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandStoreGP_STOREGP</v>
+        <v>Bulwer IslandMakeCM10CL</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="5"/>
-        <v>Bulwer IslandDeliverTRUCKGP</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="O40">
         <f t="shared" si="6"/>
@@ -3264,13 +3299,13 @@
       </c>
       <c r="P40" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandStoreGP</v>
+        <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" cm="1">
         <f t="array" ref="A41">IF(ISNA(_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40)),IF(COUNTIFS($P$2:P41,P41)=1,IF(COUNTIFS($C$2:C40,C41)=0,1,_xlfn.MAXIFS($A$2:A40,$C$2:C40,C41)+1),A40),_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
@@ -3279,74 +3314,80 @@
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F41" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G41" t="s">
         <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="I41" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
       </c>
       <c r="K41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L41" t="s">
         <v>27</v>
       </c>
       <c r="M41" t="str">
         <f t="shared" si="4"/>
-        <v>Bulwer IslandDeliverTRUCKGP</v>
+        <v>Bulwer IslandMakeCM11CL</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="O41">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P41" t="str">
         <f t="shared" si="7"/>
-        <v>Bulwer IslandDeliverGP</v>
+        <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" cm="1">
         <f t="array" ref="A42">IF(ISNA(_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41)),IF(COUNTIFS($P$2:P42,P42)=1,IF(COUNTIFS($C$2:C41,C42)=0,1,_xlfn.MAXIFS($A$2:A41,$C$2:C41,C42)+1),A41),_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F42" t="s">
         <v>25</v>
       </c>
       <c r="G42" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H42" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I42" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J42" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -3356,11 +3397,11 @@
       </c>
       <c r="M42" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaStoreCL_STORE_ICL</v>
+        <v>Bulwer IslandStoreGP_STOREGP</v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaMakeVRMCL</v>
+        <v>Bulwer IslandDeliverTRUCKGP</v>
       </c>
       <c r="O42">
         <f t="shared" si="6"/>
@@ -3368,68 +3409,59 @@
       </c>
       <c r="P42" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaStoreCL</v>
+        <v>Bulwer IslandStoreGP</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" cm="1">
         <f t="array" ref="A43">IF(ISNA(_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42)),IF(COUNTIFS($P$2:P43,P43)=1,IF(COUNTIFS($C$2:C42,C43)=0,1,_xlfn.MAXIFS($A$2:A42,$C$2:C42,C43)+1),A42),_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G43" t="s">
         <v>19</v>
       </c>
-      <c r="H43" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" t="s">
-        <v>33</v>
-      </c>
       <c r="K43">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L43" t="s">
         <v>27</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaMakeVRMCL</v>
+        <v>Bulwer IslandDeliverTRUCKGP</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>GP</v>
       </c>
       <c r="O43">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P43" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaMakeGP</v>
+        <v>Bulwer IslandDeliverGP</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" cm="1">
         <f t="array" ref="A44">IF(ISNA(_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43)),IF(COUNTIFS($P$2:P44,P44)=1,IF(COUNTIFS($C$2:C43,C44)=0,1,_xlfn.MAXIFS($A$2:A43,$C$2:C43,C44)+1),A43),_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
@@ -3438,25 +3470,25 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E44" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
         <v>25</v>
       </c>
       <c r="G44" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I44" t="s">
         <v>38</v>
       </c>
       <c r="J44" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -3466,25 +3498,25 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>Port KemblaStoreCL_STORE_ICL</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaMoveTRAINGP</v>
+        <v>Port KemblaMakeVRMCL</v>
       </c>
       <c r="O44">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaStoreGP</v>
+        <v>Port KemblaStoreCL</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" cm="1">
         <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),A44),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -3493,53 +3525,53 @@
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" t="s">
         <v>25</v>
-      </c>
-      <c r="G45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" t="s">
-        <v>35</v>
       </c>
       <c r="I45" t="s">
         <v>38</v>
       </c>
       <c r="J45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L45" t="s">
         <v>27</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>Port KemblaMakeVRMCL</v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="5"/>
-        <v>Port KemblaDeliverTRUCKGP</v>
+        <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="O45">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P45" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaStoreGP</v>
+        <v>Port KemblaMakeGP</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" cm="1">
         <f t="array" ref="A46">IF(ISNA(_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45)),IF(COUNTIFS($P$2:P46,P46)=1,IF(COUNTIFS($C$2:C45,C46)=0,1,_xlfn.MAXIFS($A$2:A45,$C$2:C45,C46)+1),A45),_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -3548,50 +3580,50 @@
         <v>38</v>
       </c>
       <c r="D46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" t="s">
         <v>34</v>
       </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>28</v>
-      </c>
-      <c r="G46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" t="s">
-        <v>25</v>
-      </c>
-      <c r="I46" t="s">
-        <v>52</v>
-      </c>
-      <c r="J46" t="s">
-        <v>33</v>
-      </c>
       <c r="K46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M46" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaMoveTRAINGP</v>
+        <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="5"/>
-        <v>AlburyStoreGP_STOREGP</v>
+        <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="O46">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P46" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaMoveGP</v>
+        <v>Port KemblaStoreGP</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" cm="1">
         <f t="array" ref="A47">IF(ISNA(_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46)),IF(COUNTIFS($P$2:P47,P47)=1,IF(COUNTIFS($C$2:C46,C47)=0,1,_xlfn.MAXIFS($A$2:A46,$C$2:C46,C47)+1),A46),_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -3600,36 +3632,36 @@
         <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G47" t="s">
         <v>19</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I47" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="J47" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M47" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaMoveTRAINGP</v>
+        <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="N47" t="str">
         <f t="shared" si="5"/>
-        <v>WaggaStoreGP_STOREGP</v>
+        <v>Port KemblaDeliverTRUCKGP</v>
       </c>
       <c r="O47">
         <f t="shared" si="6"/>
@@ -3637,11 +3669,11 @@
       </c>
       <c r="P47" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaMoveGP</v>
+        <v>Port KemblaStoreGP</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" cm="1">
         <f t="array" ref="A48">IF(ISNA(_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47)),IF(COUNTIFS($P$2:P48,P48)=1,IF(COUNTIFS($C$2:C47,C48)=0,1,_xlfn.MAXIFS($A$2:A47,$C$2:C47,C48)+1),A47),_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47))</f>
         <v>4</v>
       </c>
@@ -3667,7 +3699,7 @@
         <v>25</v>
       </c>
       <c r="I48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J48" t="s">
         <v>33</v>
@@ -3681,7 +3713,7 @@
       </c>
       <c r="N48" t="str">
         <f t="shared" si="5"/>
-        <v>ClydeStoreGP_STOREGP</v>
+        <v>AlburyStoreGP_STOREGP</v>
       </c>
       <c r="O48">
         <f t="shared" si="6"/>
@@ -3693,7 +3725,8 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" cm="1">
+        <f t="array" ref="A49">IF(ISNA(_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48)),IF(COUNTIFS($P$2:P49,P49)=1,IF(COUNTIFS($C$2:C48,C49)=0,1,_xlfn.MAXIFS($A$2:A48,$C$2:C48,C49)+1),A48),_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48))</f>
         <v>4</v>
       </c>
       <c r="B49" t="s">
@@ -3703,82 +3736,88 @@
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G49" t="s">
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="I49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" t="s">
+        <v>33</v>
       </c>
       <c r="K49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="4"/>
-        <v>Port KemblaDeliverTRUCKGP</v>
+        <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>WaggaStoreGP_STOREGP</v>
       </c>
       <c r="O49">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" t="str">
         <f t="shared" si="7"/>
-        <v>Port KemblaDeliverGP</v>
+        <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" cm="1">
         <f t="array" ref="A50">IF(ISNA(_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49)),IF(COUNTIFS($P$2:P50,P50)=1,IF(COUNTIFS($C$2:C49,C50)=0,1,_xlfn.MAXIFS($A$2:A49,$C$2:C49,C50)+1),A49),_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J50" t="s">
         <v>33</v>
       </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" t="s">
-        <v>35</v>
-      </c>
-      <c r="I50" t="s">
-        <v>39</v>
-      </c>
-      <c r="J50" t="s">
-        <v>36</v>
-      </c>
       <c r="K50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M50" t="str">
         <f t="shared" si="4"/>
-        <v>NewcastleStoreGP_STOREGP</v>
+        <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N50" t="str">
         <f t="shared" si="5"/>
-        <v>NewcastleDeliverTRUCKGP</v>
+        <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="O50">
         <f t="shared" si="6"/>
@@ -3786,19 +3825,18 @@
       </c>
       <c r="P50" t="str">
         <f t="shared" si="7"/>
-        <v>NewcastleStoreGP</v>
+        <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="array" ref="A51">IF(ISNA(_xlfn.XLOOKUP(P51,$P$2:P50,$A$2:A50)),IF(COUNTIFS($P$2:P51,P51)=1,IF(COUNTIFS($C$2:C50,C51)=0,1,_xlfn.MAXIFS($A$2:A50,$C$2:C50,C51)+1),A50),_xlfn.XLOOKUP(P51,$P$2:P50,$A$2:A50))</f>
-        <v>2</v>
+      <c r="A51" s="1">
+        <v>4</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
         <v>36</v>
@@ -3812,19 +3850,16 @@
       <c r="G51" t="s">
         <v>19</v>
       </c>
-      <c r="H51" t="s">
-        <v>22</v>
-      </c>
       <c r="K51">
         <v>4</v>
       </c>
       <c r="M51" t="str">
         <f t="shared" si="4"/>
-        <v>NewcastleDeliverTRUCKGP</v>
+        <v>Port KemblaDeliverTRUCKGP</v>
       </c>
       <c r="N51" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O51">
         <f t="shared" si="6"/>
@@ -3832,11 +3867,11 @@
       </c>
       <c r="P51" t="str">
         <f t="shared" si="7"/>
-        <v>NewcastleDeliverGP</v>
+        <v>Port KemblaDeliverGP</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" cm="1">
         <f t="array" ref="A52">IF(ISNA(_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51)),IF(COUNTIFS($P$2:P52,P52)=1,IF(COUNTIFS($C$2:C51,C52)=0,1,_xlfn.MAXIFS($A$2:A51,$C$2:C51,C52)+1),A51),_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51))</f>
         <v>1</v>
       </c>
@@ -3844,7 +3879,7 @@
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
         <v>33</v>
@@ -3862,7 +3897,7 @@
         <v>35</v>
       </c>
       <c r="I52" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J52" t="s">
         <v>36</v>
@@ -3872,11 +3907,11 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="4"/>
-        <v>MelbourneStoreGP_STOREGP</v>
+        <v>NewcastleStoreGP_STOREGP</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="5"/>
-        <v>MelbourneDeliverTRUCKGP</v>
+        <v>NewcastleDeliverTRUCKGP</v>
       </c>
       <c r="O52">
         <f t="shared" si="6"/>
@@ -3884,11 +3919,11 @@
       </c>
       <c r="P52" t="str">
         <f t="shared" si="7"/>
-        <v>MelbourneStoreGP</v>
+        <v>NewcastleStoreGP</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" cm="1">
         <f t="array" ref="A53">IF(ISNA(_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52)),IF(COUNTIFS($P$2:P53,P53)=1,IF(COUNTIFS($C$2:C52,C53)=0,1,_xlfn.MAXIFS($A$2:A52,$C$2:C52,C53)+1),A52),_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52))</f>
         <v>2</v>
       </c>
@@ -3896,7 +3931,7 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
         <v>36</v>
@@ -3910,19 +3945,16 @@
       <c r="G53" t="s">
         <v>19</v>
       </c>
-      <c r="H53" t="s">
-        <v>22</v>
-      </c>
       <c r="K53">
         <v>4</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="4"/>
-        <v>MelbourneDeliverTRUCKGP</v>
+        <v>NewcastleDeliverTRUCKGP</v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O53">
         <f t="shared" si="6"/>
@@ -3930,11 +3962,11 @@
       </c>
       <c r="P53" t="str">
         <f t="shared" si="7"/>
-        <v>MelbourneDeliverGP</v>
+        <v>NewcastleDeliverGP</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" cm="1">
         <f t="array" ref="A54">IF(ISNA(_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53)),IF(COUNTIFS($P$2:P54,P54)=1,IF(COUNTIFS($C$2:C53,C54)=0,1,_xlfn.MAXIFS($A$2:A53,$C$2:C53,C54)+1),A53),_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53))</f>
         <v>1</v>
       </c>
@@ -3942,7 +3974,7 @@
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" t="s">
         <v>33</v>
@@ -3960,7 +3992,7 @@
         <v>35</v>
       </c>
       <c r="I54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J54" t="s">
         <v>36</v>
@@ -3970,11 +4002,11 @@
       </c>
       <c r="M54" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornStoreGP_STOREGP</v>
+        <v>MelbourneStoreGP_STOREGP</v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="5"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="O54">
         <f t="shared" si="6"/>
@@ -3982,11 +4014,11 @@
       </c>
       <c r="P54" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornStoreGP</v>
+        <v>MelbourneStoreGP</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" cm="1">
         <f t="array" ref="A55">IF(ISNA(_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54)),IF(COUNTIFS($P$2:P55,P55)=1,IF(COUNTIFS($C$2:C54,C55)=0,1,_xlfn.MAXIFS($A$2:A54,$C$2:C54,C55)+1),A54),_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54))</f>
         <v>2</v>
       </c>
@@ -3994,7 +4026,7 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
         <v>36</v>
@@ -4008,19 +4040,16 @@
       <c r="G55" t="s">
         <v>19</v>
       </c>
-      <c r="H55" t="s">
-        <v>22</v>
-      </c>
       <c r="K55">
         <v>4</v>
       </c>
       <c r="M55" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O55">
         <f t="shared" si="6"/>
@@ -4028,11 +4057,11 @@
       </c>
       <c r="P55" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornDeliverGP</v>
+        <v>MelbourneDeliverGP</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" cm="1">
         <f t="array" ref="A56">IF(ISNA(_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55)),IF(COUNTIFS($P$2:P56,P56)=1,IF(COUNTIFS($C$2:C55,C56)=0,1,_xlfn.MAXIFS($A$2:A55,$C$2:C55,C56)+1),A55),_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55))</f>
         <v>1</v>
       </c>
@@ -4040,7 +4069,7 @@
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D56" t="s">
         <v>33</v>
@@ -4058,7 +4087,7 @@
         <v>35</v>
       </c>
       <c r="I56" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="J56" t="s">
         <v>36</v>
@@ -4068,11 +4097,11 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="4"/>
-        <v>TownsvilleStoreGP_STOREGP</v>
+        <v>OsbornStoreGP_STOREGP</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="5"/>
-        <v>TownsvilleDeliverTRUCKGP</v>
+        <v>OsbornDeliverTRUCKGP</v>
       </c>
       <c r="O56">
         <f t="shared" si="6"/>
@@ -4080,11 +4109,11 @@
       </c>
       <c r="P56" t="str">
         <f t="shared" si="7"/>
-        <v>TownsvilleStoreGP</v>
+        <v>OsbornStoreGP</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" cm="1">
         <f t="array" ref="A57">IF(ISNA(_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56)),IF(COUNTIFS($P$2:P57,P57)=1,IF(COUNTIFS($C$2:C56,C57)=0,1,_xlfn.MAXIFS($A$2:A56,$C$2:C56,C57)+1),A56),_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56))</f>
         <v>2</v>
       </c>
@@ -4092,7 +4121,7 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D57" t="s">
         <v>36</v>
@@ -4106,19 +4135,16 @@
       <c r="G57" t="s">
         <v>19</v>
       </c>
-      <c r="H57" t="s">
-        <v>22</v>
-      </c>
       <c r="K57">
         <v>4</v>
       </c>
       <c r="M57" t="str">
         <f t="shared" si="4"/>
-        <v>TownsvilleDeliverTRUCKGP</v>
+        <v>OsbornDeliverTRUCKGP</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O57">
         <f t="shared" si="6"/>
@@ -4126,11 +4152,11 @@
       </c>
       <c r="P57" t="str">
         <f t="shared" si="7"/>
-        <v>TownsvilleDeliverGP</v>
+        <v>OsbornDeliverGP</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" cm="1">
         <f t="array" ref="A58">IF(ISNA(_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57)),IF(COUNTIFS($P$2:P58,P58)=1,IF(COUNTIFS($C$2:C57,C58)=0,1,_xlfn.MAXIFS($A$2:A57,$C$2:C57,C58)+1),A57),_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57))</f>
         <v>1</v>
       </c>
@@ -4138,7 +4164,7 @@
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s">
         <v>33</v>
@@ -4156,7 +4182,7 @@
         <v>35</v>
       </c>
       <c r="I58" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J58" t="s">
         <v>36</v>
@@ -4166,11 +4192,11 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="4"/>
-        <v>MackayStoreGP_STOREGP</v>
+        <v>TownsvilleStoreGP_STOREGP</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="5"/>
-        <v>MackayDeliverTRUCKGP</v>
+        <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="O58">
         <f t="shared" si="6"/>
@@ -4178,11 +4204,11 @@
       </c>
       <c r="P58" t="str">
         <f t="shared" si="7"/>
-        <v>MackayStoreGP</v>
+        <v>TownsvilleStoreGP</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" cm="1">
         <f t="array" ref="A59">IF(ISNA(_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58)),IF(COUNTIFS($P$2:P59,P59)=1,IF(COUNTIFS($C$2:C58,C59)=0,1,_xlfn.MAXIFS($A$2:A58,$C$2:C58,C59)+1),A58),_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58))</f>
         <v>2</v>
       </c>
@@ -4190,7 +4216,7 @@
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D59" t="s">
         <v>36</v>
@@ -4204,19 +4230,16 @@
       <c r="G59" t="s">
         <v>19</v>
       </c>
-      <c r="H59" t="s">
-        <v>22</v>
-      </c>
       <c r="K59">
         <v>4</v>
       </c>
       <c r="M59" t="str">
         <f t="shared" si="4"/>
-        <v>MackayDeliverTRUCKGP</v>
+        <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O59">
         <f t="shared" si="6"/>
@@ -4224,11 +4247,11 @@
       </c>
       <c r="P59" t="str">
         <f t="shared" si="7"/>
-        <v>MackayDeliverGP</v>
+        <v>TownsvilleDeliverGP</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" cm="1">
         <f t="array" ref="A60">IF(ISNA(_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59)),IF(COUNTIFS($P$2:P60,P60)=1,IF(COUNTIFS($C$2:C59,C60)=0,1,_xlfn.MAXIFS($A$2:A59,$C$2:C59,C60)+1),A59),_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59))</f>
         <v>1</v>
       </c>
@@ -4236,7 +4259,7 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
         <v>33</v>
@@ -4254,7 +4277,7 @@
         <v>35</v>
       </c>
       <c r="I60" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="J60" t="s">
         <v>36</v>
@@ -4264,11 +4287,11 @@
       </c>
       <c r="M60" t="str">
         <f t="shared" si="4"/>
-        <v>WaggaStoreGP_STOREGP</v>
+        <v>MackayStoreGP_STOREGP</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="5"/>
-        <v>WaggaDeliverTRUCKGP</v>
+        <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="O60">
         <f t="shared" si="6"/>
@@ -4276,11 +4299,11 @@
       </c>
       <c r="P60" t="str">
         <f t="shared" si="7"/>
-        <v>WaggaStoreGP</v>
+        <v>MackayStoreGP</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" cm="1">
         <f t="array" ref="A61">IF(ISNA(_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60)),IF(COUNTIFS($P$2:P61,P61)=1,IF(COUNTIFS($C$2:C60,C61)=0,1,_xlfn.MAXIFS($A$2:A60,$C$2:C60,C61)+1),A60),_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60))</f>
         <v>2</v>
       </c>
@@ -4288,7 +4311,7 @@
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
         <v>36</v>
@@ -4302,19 +4325,16 @@
       <c r="G61" t="s">
         <v>19</v>
       </c>
-      <c r="H61" t="s">
-        <v>22</v>
-      </c>
       <c r="K61">
         <v>4</v>
       </c>
       <c r="M61" t="str">
         <f t="shared" si="4"/>
-        <v>WaggaDeliverTRUCKGP</v>
+        <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O61">
         <f t="shared" si="6"/>
@@ -4322,11 +4342,11 @@
       </c>
       <c r="P61" t="str">
         <f t="shared" si="7"/>
-        <v>WaggaDeliverGP</v>
+        <v>MackayDeliverGP</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" cm="1">
         <f t="array" ref="A62">IF(ISNA(_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61)),IF(COUNTIFS($P$2:P62,P62)=1,IF(COUNTIFS($C$2:C61,C62)=0,1,_xlfn.MAXIFS($A$2:A61,$C$2:C61,C62)+1),A61),_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61))</f>
         <v>1</v>
       </c>
@@ -4334,7 +4354,7 @@
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D62" t="s">
         <v>33</v>
@@ -4352,7 +4372,7 @@
         <v>35</v>
       </c>
       <c r="I62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J62" t="s">
         <v>36</v>
@@ -4362,11 +4382,11 @@
       </c>
       <c r="M62" t="str">
         <f t="shared" si="4"/>
-        <v>AlburyStoreGP_STOREGP</v>
+        <v>WaggaStoreGP_STOREGP</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="5"/>
-        <v>AlburyDeliverTRUCKGP</v>
+        <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="O62">
         <f t="shared" si="6"/>
@@ -4374,11 +4394,11 @@
       </c>
       <c r="P62" t="str">
         <f t="shared" si="7"/>
-        <v>AlburyStoreGP</v>
+        <v>WaggaStoreGP</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" cm="1">
         <f t="array" ref="A63">IF(ISNA(_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62)),IF(COUNTIFS($P$2:P63,P63)=1,IF(COUNTIFS($C$2:C62,C63)=0,1,_xlfn.MAXIFS($A$2:A62,$C$2:C62,C63)+1),A62),_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62))</f>
         <v>2</v>
       </c>
@@ -4386,7 +4406,7 @@
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D63" t="s">
         <v>36</v>
@@ -4400,19 +4420,16 @@
       <c r="G63" t="s">
         <v>19</v>
       </c>
-      <c r="H63" t="s">
-        <v>22</v>
-      </c>
       <c r="K63">
         <v>4</v>
       </c>
       <c r="M63" t="str">
         <f t="shared" si="4"/>
-        <v>AlburyDeliverTRUCKGP</v>
+        <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="5"/>
-        <v>NoneGP</v>
+        <v>GP</v>
       </c>
       <c r="O63">
         <f t="shared" si="6"/>
@@ -4420,11 +4437,11 @@
       </c>
       <c r="P63" t="str">
         <f t="shared" si="7"/>
-        <v>AlburyDeliverGP</v>
+        <v>WaggaDeliverGP</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" cm="1">
         <f t="array" ref="A64">IF(ISNA(_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63)),IF(COUNTIFS($P$2:P64,P64)=1,IF(COUNTIFS($C$2:C63,C64)=0,1,_xlfn.MAXIFS($A$2:A63,$C$2:C63,C64)+1),A63),_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63))</f>
         <v>1</v>
       </c>
@@ -4432,7 +4449,7 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D64" t="s">
         <v>33</v>
@@ -4450,7 +4467,7 @@
         <v>35</v>
       </c>
       <c r="I64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J64" t="s">
         <v>36</v>
@@ -4460,11 +4477,11 @@
       </c>
       <c r="M64" t="str">
         <f t="shared" si="4"/>
-        <v>ClydeStoreGP_STOREGP</v>
+        <v>AlburyStoreGP_STOREGP</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="5"/>
-        <v>ClydeDeliverTRUCKGP</v>
+        <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="O64">
         <f t="shared" si="6"/>
@@ -4472,11 +4489,11 @@
       </c>
       <c r="P64" t="str">
         <f t="shared" si="7"/>
-        <v>ClydeStoreGP</v>
+        <v>AlburyStoreGP</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" cm="1">
         <f t="array" ref="A65">IF(ISNA(_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64)),IF(COUNTIFS($P$2:P65,P65)=1,IF(COUNTIFS($C$2:C64,C65)=0,1,_xlfn.MAXIFS($A$2:A64,$C$2:C64,C65)+1),A64),_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64))</f>
         <v>2</v>
       </c>
@@ -4484,7 +4501,7 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D65" t="s">
         <v>36</v>
@@ -4498,110 +4515,100 @@
       <c r="G65" t="s">
         <v>19</v>
       </c>
-      <c r="H65" t="s">
-        <v>22</v>
-      </c>
       <c r="K65">
         <v>4</v>
       </c>
       <c r="M65" t="str">
         <f t="shared" si="4"/>
-        <v>ClydeDeliverTRUCKGP</v>
+        <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="P65" t="str">
         <f t="shared" si="7"/>
-        <v>ClydeDeliverGP</v>
+        <v>AlburyDeliverGP</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" cm="1">
+        <f t="array" ref="A66">IF(ISNA(_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65)),IF(COUNTIFS($P$2:P66,P66)=1,IF(COUNTIFS($C$2:C65,C66)=0,1,_xlfn.MAXIFS($A$2:A65,$C$2:C65,C66)+1),A65),_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65))</f>
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E66" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="F66" t="s">
         <v>25</v>
       </c>
       <c r="G66" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H66" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I66" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="J66" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K66">
         <v>2</v>
       </c>
       <c r="M66" t="str">
         <f t="shared" si="4"/>
-        <v>GladstoneStoreFA_STOREFA</v>
+        <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="P66" t="str">
         <f t="shared" si="7"/>
-        <v>GladstoneStoreFA</v>
+        <v>ClydeStoreGP</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" cm="1">
+        <f t="array" ref="A67">IF(ISNA(_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66)),IF(COUNTIFS($P$2:P67,P67)=1,IF(COUNTIFS($C$2:C66,C67)=0,1,_xlfn.MAXIFS($A$2:A66,$C$2:C66,C67)+1),A66),_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66))</f>
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D67" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E67" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G67" t="s">
-        <v>55</v>
-      </c>
-      <c r="H67" t="s">
-        <v>25</v>
-      </c>
-      <c r="I67" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="K67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M67" t="str">
         <f t="shared" si="4"/>
-        <v>GladstoneMoveSHIPFA</v>
+        <v>ClydeDeliverTRUCKGP</v>
       </c>
       <c r="P67" t="str">
         <f t="shared" si="7"/>
-        <v>GladstoneMoveFA</v>
+        <v>ClydeDeliverGP</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -4610,103 +4617,103 @@
         <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E68" t="s">
         <v>55</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G68" t="s">
         <v>55</v>
       </c>
       <c r="H68" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I68" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J68" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="K68">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
         <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D69" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E69" t="s">
         <v>55</v>
       </c>
       <c r="F69" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G69" t="s">
         <v>55</v>
       </c>
       <c r="H69" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I69" t="s">
         <v>45</v>
       </c>
       <c r="J69" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="K69">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
         <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D70" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E70" t="s">
         <v>55</v>
       </c>
       <c r="F70" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G70" t="s">
         <v>55</v>
       </c>
       <c r="H70" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I70" t="s">
         <v>38</v>
       </c>
       <c r="J70" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="K70">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B71" t="s">
         <v>55</v>
@@ -4715,27 +4722,33 @@
         <v>45</v>
       </c>
       <c r="D71" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E71" t="s">
         <v>55</v>
       </c>
       <c r="F71" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G71" t="s">
         <v>55</v>
       </c>
       <c r="H71" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="I71" t="s">
+        <v>45</v>
+      </c>
+      <c r="J71" t="s">
+        <v>36</v>
       </c>
       <c r="K71">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
         <v>55</v>
@@ -4744,57 +4757,54 @@
         <v>38</v>
       </c>
       <c r="D72" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E72" t="s">
         <v>55</v>
       </c>
       <c r="F72" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G72" t="s">
         <v>55</v>
       </c>
       <c r="H72" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="I72" t="s">
+        <v>38</v>
+      </c>
+      <c r="J72" t="s">
+        <v>36</v>
       </c>
       <c r="K72">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D73" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E73" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F73" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>77</v>
-      </c>
-      <c r="H73" t="s">
-        <v>28</v>
-      </c>
-      <c r="I73" t="s">
-        <v>47</v>
-      </c>
-      <c r="J73" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="K73">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -4802,39 +4812,30 @@
         <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E74" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F74" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>77</v>
-      </c>
-      <c r="H74" t="s">
-        <v>25</v>
-      </c>
-      <c r="I74" t="s">
-        <v>38</v>
-      </c>
-      <c r="J74" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="K74">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
         <v>75</v>
@@ -4843,63 +4844,63 @@
         <v>47</v>
       </c>
       <c r="D75" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E75" t="s">
         <v>77</v>
       </c>
       <c r="F75" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G75" t="s">
         <v>77</v>
       </c>
       <c r="H75" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I75" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="J75" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="K75">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D76" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E76" t="s">
         <v>77</v>
       </c>
       <c r="F76" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G76" t="s">
         <v>77</v>
       </c>
       <c r="H76" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I76" t="s">
         <v>38</v>
       </c>
       <c r="J76" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="K76">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -4910,36 +4911,36 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D77" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E77" t="s">
         <v>77</v>
       </c>
       <c r="F77" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G77" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H77" t="s">
         <v>25</v>
       </c>
       <c r="I77" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J77" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K77">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B78" t="s">
         <v>75</v>
@@ -4948,25 +4949,25 @@
         <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E78" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F78" t="s">
         <v>25</v>
       </c>
       <c r="G78" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H78" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I78" t="s">
         <v>38</v>
       </c>
       <c r="J78" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="K78">
         <v>2</v>
@@ -4974,7 +4975,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B79" t="s">
         <v>75</v>
@@ -4983,19 +4984,28 @@
         <v>38</v>
       </c>
       <c r="D79" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E79" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F79" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G79" t="s">
         <v>75</v>
       </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
+      <c r="I79" t="s">
+        <v>38</v>
+      </c>
+      <c r="J79" t="s">
+        <v>78</v>
+      </c>
       <c r="K79">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -5021,13 +5031,13 @@
         <v>75</v>
       </c>
       <c r="H80" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I80" t="s">
         <v>38</v>
       </c>
       <c r="J80" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K80">
         <v>2</v>
@@ -5035,7 +5045,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
         <v>75</v>
@@ -5044,33 +5054,24 @@
         <v>38</v>
       </c>
       <c r="D81" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E81" t="s">
         <v>75</v>
       </c>
       <c r="F81" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G81" t="s">
         <v>75</v>
       </c>
-      <c r="H81" t="s">
-        <v>28</v>
-      </c>
-      <c r="I81" t="s">
-        <v>38</v>
-      </c>
-      <c r="J81" t="s">
-        <v>34</v>
-      </c>
       <c r="K81">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
         <v>75</v>
@@ -5079,33 +5080,33 @@
         <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E82" t="s">
         <v>75</v>
       </c>
       <c r="F82" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G82" t="s">
         <v>75</v>
       </c>
       <c r="H82" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I82" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J82" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="K82">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
         <v>75</v>
@@ -5114,28 +5115,28 @@
         <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E83" t="s">
         <v>75</v>
       </c>
       <c r="F83" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G83" t="s">
         <v>75</v>
       </c>
       <c r="H83" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I83" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J83" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="K83">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -5149,7 +5150,7 @@
         <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E84" t="s">
         <v>75</v>
@@ -5164,7 +5165,7 @@
         <v>25</v>
       </c>
       <c r="I84" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="J84" t="s">
         <v>78</v>
@@ -5199,7 +5200,7 @@
         <v>25</v>
       </c>
       <c r="I85" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J85" t="s">
         <v>78</v>
@@ -5210,77 +5211,77 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
         <v>75</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D86" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F86" t="s">
+        <v>28</v>
+      </c>
+      <c r="G86" t="s">
+        <v>75</v>
+      </c>
+      <c r="H86" t="s">
         <v>25</v>
       </c>
-      <c r="G86" t="s">
-        <v>77</v>
-      </c>
-      <c r="H86" t="s">
-        <v>23</v>
-      </c>
       <c r="I86" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="J86" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="K86">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B87" t="s">
         <v>75</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E87" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F87" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" t="s">
+        <v>75</v>
+      </c>
+      <c r="H87" t="s">
         <v>25</v>
       </c>
-      <c r="G87" t="s">
-        <v>77</v>
-      </c>
-      <c r="H87" t="s">
-        <v>23</v>
-      </c>
       <c r="I87" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J87" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="K87">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88" t="s">
         <v>75</v>
@@ -5289,33 +5290,33 @@
         <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="E88" t="s">
         <v>77</v>
       </c>
       <c r="F88" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" t="s">
+        <v>77</v>
+      </c>
+      <c r="H88" t="s">
         <v>23</v>
-      </c>
-      <c r="G88" t="s">
-        <v>75</v>
-      </c>
-      <c r="H88" t="s">
-        <v>25</v>
       </c>
       <c r="I88" t="s">
         <v>30</v>
       </c>
       <c r="J88" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="K88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
         <v>75</v>
@@ -5324,33 +5325,33 @@
         <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="E89" t="s">
         <v>77</v>
       </c>
       <c r="F89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" t="s">
+        <v>77</v>
+      </c>
+      <c r="H89" t="s">
         <v>23</v>
-      </c>
-      <c r="G89" t="s">
-        <v>75</v>
-      </c>
-      <c r="H89" t="s">
-        <v>25</v>
       </c>
       <c r="I89" t="s">
         <v>30</v>
       </c>
       <c r="J89" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="K89">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
         <v>75</v>
@@ -5359,33 +5360,33 @@
         <v>30</v>
       </c>
       <c r="D90" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E90" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F90" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G90" t="s">
         <v>75</v>
       </c>
       <c r="H90" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I90" t="s">
         <v>30</v>
       </c>
       <c r="J90" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="K90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
         <v>75</v>
@@ -5394,33 +5395,33 @@
         <v>30</v>
       </c>
       <c r="D91" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E91" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F91" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G91" t="s">
         <v>75</v>
       </c>
       <c r="H91" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I91" t="s">
         <v>30</v>
       </c>
       <c r="J91" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="K91">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
         <v>75</v>
@@ -5429,33 +5430,33 @@
         <v>30</v>
       </c>
       <c r="D92" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E92" t="s">
         <v>75</v>
       </c>
       <c r="F92" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G92" t="s">
         <v>75</v>
       </c>
       <c r="H92" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I92" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="J92" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="K92">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B93" t="s">
         <v>75</v>
@@ -5464,65 +5465,74 @@
         <v>30</v>
       </c>
       <c r="D93" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="E93" t="s">
         <v>75</v>
       </c>
       <c r="F93" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G93" t="s">
         <v>75</v>
       </c>
+      <c r="H93" t="s">
+        <v>35</v>
+      </c>
+      <c r="I93" t="s">
+        <v>30</v>
+      </c>
+      <c r="J93" t="s">
+        <v>36</v>
+      </c>
       <c r="K93">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B94" t="s">
         <v>75</v>
       </c>
       <c r="C94" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="D94" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E94" t="s">
         <v>75</v>
       </c>
       <c r="F94" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G94" t="s">
         <v>75</v>
       </c>
       <c r="H94" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I94" t="s">
         <v>79</v>
       </c>
       <c r="J94" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="K94">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s">
         <v>75</v>
       </c>
       <c r="C95" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
@@ -5548,7 +5558,7 @@
         <v>75</v>
       </c>
       <c r="C96" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="D96" t="s">
         <v>78</v>
@@ -5566,13 +5576,13 @@
         <v>35</v>
       </c>
       <c r="I96" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="J96" t="s">
         <v>36</v>
       </c>
       <c r="K96">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -5583,7 +5593,7 @@
         <v>75</v>
       </c>
       <c r="C97" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="D97" t="s">
         <v>36</v>
@@ -5609,7 +5619,7 @@
         <v>75</v>
       </c>
       <c r="C98" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D98" t="s">
         <v>78</v>
@@ -5627,7 +5637,7 @@
         <v>35</v>
       </c>
       <c r="I98" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J98" t="s">
         <v>36</v>
@@ -5644,7 +5654,7 @@
         <v>75</v>
       </c>
       <c r="C99" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D99" t="s">
         <v>36</v>
@@ -5670,7 +5680,7 @@
         <v>75</v>
       </c>
       <c r="C100" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D100" t="s">
         <v>78</v>
@@ -5688,7 +5698,7 @@
         <v>35</v>
       </c>
       <c r="I100" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="J100" t="s">
         <v>36</v>
@@ -5705,7 +5715,7 @@
         <v>75</v>
       </c>
       <c r="C101" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D101" t="s">
         <v>36</v>
@@ -5731,7 +5741,7 @@
         <v>75</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="D102" t="s">
         <v>78</v>
@@ -5749,7 +5759,7 @@
         <v>35</v>
       </c>
       <c r="I102" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="J102" t="s">
         <v>36</v>
@@ -5766,7 +5776,7 @@
         <v>75</v>
       </c>
       <c r="C103" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="D103" t="s">
         <v>36</v>
@@ -5784,8 +5794,69 @@
         <v>4</v>
       </c>
     </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>75</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" t="s">
+        <v>78</v>
+      </c>
+      <c r="E104" t="s">
+        <v>75</v>
+      </c>
+      <c r="F104" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" t="s">
+        <v>75</v>
+      </c>
+      <c r="H104" t="s">
+        <v>35</v>
+      </c>
+      <c r="I104" t="s">
+        <v>39</v>
+      </c>
+      <c r="J104" t="s">
+        <v>36</v>
+      </c>
+      <c r="K104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>75</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E105" t="s">
+        <v>75</v>
+      </c>
+      <c r="F105" t="s">
+        <v>35</v>
+      </c>
+      <c r="G105" t="s">
+        <v>75</v>
+      </c>
+      <c r="K105">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:K104" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:K105" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="M1:N1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -5799,7 +5870,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6193,10 +6264,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6279,7 +6350,7 @@
         <v>25000</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G33" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G30" si="0">E3-F3</f>
         <v>25000</v>
       </c>
       <c r="H3" t="s">
@@ -6526,7 +6597,7 @@
         <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6646,7 +6717,7 @@
         <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -6676,7 +6747,7 @@
         <v>27</v>
       </c>
       <c r="I16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -6706,7 +6777,7 @@
         <v>160</v>
       </c>
       <c r="I17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6760,7 +6831,7 @@
         <v>27</v>
       </c>
       <c r="I19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -6790,7 +6861,7 @@
         <v>27</v>
       </c>
       <c r="I20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6820,7 +6891,7 @@
         <v>27</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -6847,10 +6918,10 @@
         <v>1500</v>
       </c>
       <c r="H22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6880,7 +6951,7 @@
         <v>27</v>
       </c>
       <c r="I23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6937,7 +7008,7 @@
         <v>4000</v>
       </c>
       <c r="H25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -6964,7 +7035,7 @@
         <v>40000</v>
       </c>
       <c r="H26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6994,7 +7065,7 @@
         <v>27</v>
       </c>
       <c r="I27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -7024,7 +7095,7 @@
         <v>27</v>
       </c>
       <c r="I28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -7051,7 +7122,7 @@
         <v>40000</v>
       </c>
       <c r="H29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -7059,40 +7130,43 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
       </c>
       <c r="D30">
-        <v>1500</v>
+        <v>3600</v>
       </c>
       <c r="E30">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="F30">
         <v>500</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="H30" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="I30" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D31">
-        <v>99999</v>
+        <v>1500</v>
       </c>
       <c r="E31">
         <v>1000</v>
@@ -7101,49 +7175,49 @@
         <v>500</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G31:G34" si="1">E31-F31</f>
         <v>500</v>
       </c>
       <c r="H31" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="I31" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="D32">
-        <v>30000</v>
+        <v>99999</v>
       </c>
       <c r="E32">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="F32">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>500</v>
       </c>
       <c r="H32" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
       <c r="I32" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
@@ -7152,22 +7226,52 @@
         <v>19</v>
       </c>
       <c r="D33">
+        <v>30000</v>
+      </c>
+      <c r="E33">
+        <v>15000</v>
+      </c>
+      <c r="F33">
+        <v>5000</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="H33" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34">
         <v>99999</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>1000</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>500</v>
       </c>
-      <c r="G33">
-        <f t="shared" si="0"/>
+      <c r="G34">
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>160</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>161</v>
       </c>
     </row>
@@ -7181,7 +7285,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E2:E25"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7201,7 +7305,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -7213,25 +7317,25 @@
         <v>14</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7878,25 +7982,25 @@
         <v>98</v>
       </c>
       <c r="E20">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>675</v>
       </c>
       <c r="H20">
-        <v>1000</v>
+        <v>675</v>
       </c>
       <c r="I20">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J20">
-        <v>1000</v>
+        <v>675</v>
       </c>
       <c r="K20">
-        <v>500</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -8084,7 +8188,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14980,6 +15084,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -15234,15 +15347,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -15255,6 +15359,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15273,14 +15385,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
13 DEC - WORKING MODEL - SOlVES BUT NOT PERFORMING ALL MOVES AS EXPECTED
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="966" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E97C1E6-58EC-443B-B2D7-C519899D89A1}"/>
+  <xr:revisionPtr revIDLastSave="969" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A16261E6-5C7B-44D8-8456-5FFC60772E8E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1243,13 +1243,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1367,7 +1368,7 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" cm="1">
         <f t="array" ref="A3">IF(ISNA(_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,_xlfn.MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
         <v>2</v>
@@ -1426,7 +1427,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" cm="1">
         <f t="array" ref="A4">IF(ISNA(_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3)),IF(COUNTIFS($P$2:P4,P4)=1,IF(COUNTIFS($C$2:C3,C4)=0,1,_xlfn.MAXIFS($A$2:A3,$C$2:C3,C4)+1),A3),_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3))</f>
         <v>3</v>
@@ -1481,7 +1482,7 @@
         <v>GladstoneMoveCL</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(ISNA(_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4)),IF(COUNTIFS($P$2:P5,P5)=1,IF(COUNTIFS($C$2:C4,C5)=0,1,_xlfn.MAXIFS($A$2:A4,$C$2:C4,C5)+1),A4),_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4))</f>
         <v>2</v>
@@ -1536,7 +1537,7 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" cm="1">
         <f t="array" ref="A6">IF(ISNA(_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5)),IF(COUNTIFS($P$2:P6,P6)=1,IF(COUNTIFS($C$2:C5,C6)=0,1,_xlfn.MAXIFS($A$2:A5,$C$2:C5,C6)+1),A5),_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5))</f>
         <v>2</v>
@@ -1591,7 +1592,7 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" cm="1">
         <f t="array" ref="A7">IF(ISNA(_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6)),IF(COUNTIFS($P$2:P7,P7)=1,IF(COUNTIFS($C$2:C6,C7)=0,1,_xlfn.MAXIFS($A$2:A6,$C$2:C6,C7)+1),A6),_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6))</f>
         <v>4</v>
@@ -1646,7 +1647,7 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" cm="1">
         <f t="array" ref="A8">IF(ISNA(_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7)),IF(COUNTIFS($P$2:P8,P8)=1,IF(COUNTIFS($C$2:C7,C8)=0,1,_xlfn.MAXIFS($A$2:A7,$C$2:C7,C8)+1),A7),_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7))</f>
         <v>4</v>
@@ -1701,7 +1702,7 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" cm="1">
         <f t="array" ref="A9">IF(ISNA(_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8)),IF(COUNTIFS($P$2:P9,P9)=1,IF(COUNTIFS($C$2:C8,C9)=0,1,_xlfn.MAXIFS($A$2:A8,$C$2:C8,C9)+1),A8),_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8))</f>
         <v>5</v>
@@ -1756,7 +1757,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" cm="1">
         <f t="array" ref="A10">IF(ISNA(_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9)),IF(COUNTIFS($P$2:P10,P10)=1,IF(COUNTIFS($C$2:C9,C10)=0,1,_xlfn.MAXIFS($A$2:A9,$C$2:C9,C10)+1),A9),_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9))</f>
         <v>5</v>
@@ -1811,7 +1812,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" cm="1">
         <f t="array" ref="A11">IF(ISNA(_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10)),IF(COUNTIFS($P$2:P11,P11)=1,IF(COUNTIFS($C$2:C10,C11)=0,1,_xlfn.MAXIFS($A$2:A10,$C$2:C10,C11)+1),A10),_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10))</f>
         <v>5</v>
@@ -1866,7 +1867,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" cm="1">
         <f t="array" ref="A12">IF(ISNA(_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11)),IF(COUNTIFS($P$2:P12,P12)=1,IF(COUNTIFS($C$2:C11,C12)=0,1,_xlfn.MAXIFS($A$2:A11,$C$2:C11,C12)+1),A11),_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11))</f>
         <v>6</v>
@@ -1921,7 +1922,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" cm="1">
         <f t="array" ref="A13">IF(ISNA(_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12)),IF(COUNTIFS($P$2:P13,P13)=1,IF(COUNTIFS($C$2:C12,C13)=0,1,_xlfn.MAXIFS($A$2:A12,$C$2:C12,C13)+1),A12),_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12))</f>
         <v>6</v>
@@ -1976,7 +1977,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" cm="1">
         <f t="array" ref="A14">IF(ISNA(_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13)),IF(COUNTIFS($P$2:P14,P14)=1,IF(COUNTIFS($C$2:C13,C14)=0,1,_xlfn.MAXIFS($A$2:A13,$C$2:C13,C14)+1),A13),_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13))</f>
         <v>6</v>
@@ -2031,7 +2032,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" cm="1">
         <f t="array" ref="A15">IF(ISNA(_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14)),IF(COUNTIFS($P$2:P15,P15)=1,IF(COUNTIFS($C$2:C14,C15)=0,1,_xlfn.MAXIFS($A$2:A14,$C$2:C14,C15)+1),A14),_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14))</f>
         <v>6</v>
@@ -2086,7 +2087,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" cm="1">
         <f t="array" ref="A16">IF(ISNA(_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15)),IF(COUNTIFS($P$2:P16,P16)=1,IF(COUNTIFS($C$2:C15,C16)=0,1,_xlfn.MAXIFS($A$2:A15,$C$2:C15,C16)+1),A15),_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15))</f>
         <v>6</v>
@@ -2141,7 +2142,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>RailtonDeliverGP</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" cm="1">
         <f t="array" ref="A29">IF(ISNA(_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28)),IF(COUNTIFS($P$2:P29,P29)=1,IF(COUNTIFS($C$2:C28,C29)=0,1,_xlfn.MAXIFS($A$2:A28,$C$2:C28,C29)+1),A28),_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28))</f>
         <v>1</v>
@@ -2836,7 +2837,7 @@
         <v>DevonportStoreGP</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" cm="1">
         <f t="array" ref="A30">IF(ISNA(_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29)),IF(COUNTIFS($P$2:P30,P30)=1,IF(COUNTIFS($C$2:C29,C30)=0,1,_xlfn.MAXIFS($A$2:A29,$C$2:C29,C30)+1),A29),_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29))</f>
         <v>2</v>
@@ -2891,7 +2892,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" cm="1">
         <f t="array" ref="A31">IF(ISNA(_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30)),IF(COUNTIFS($P$2:P31,P31)=1,IF(COUNTIFS($C$2:C30,C31)=0,1,_xlfn.MAXIFS($A$2:A30,$C$2:C30,C31)+1),A30),_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30))</f>
         <v>2</v>
@@ -2946,7 +2947,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" cm="1">
         <f t="array" ref="A32">IF(ISNA(_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31)),IF(COUNTIFS($P$2:P32,P32)=1,IF(COUNTIFS($C$2:C31,C32)=0,1,_xlfn.MAXIFS($A$2:A31,$C$2:C31,C32)+1),A31),_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31))</f>
         <v>2</v>
@@ -3001,7 +3002,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" cm="1">
         <f t="array" ref="A33">IF(ISNA(_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32)),IF(COUNTIFS($P$2:P33,P33)=1,IF(COUNTIFS($C$2:C32,C33)=0,1,_xlfn.MAXIFS($A$2:A32,$C$2:C32,C33)+1),A32),_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32))</f>
         <v>1</v>
@@ -3056,7 +3057,7 @@
         <v>ImportStoreCL</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" cm="1">
         <f t="array" ref="A34">IF(ISNA(_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33)),IF(COUNTIFS($P$2:P34,P34)=1,IF(COUNTIFS($C$2:C33,C34)=0,1,_xlfn.MAXIFS($A$2:A33,$C$2:C33,C34)+1),A33),_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33))</f>
         <v>2</v>
@@ -3108,7 +3109,7 @@
         <v>ImportMoveCL</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" cm="1">
         <f t="array" ref="A35">IF(ISNA(_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34)),IF(COUNTIFS($P$2:P35,P35)=1,IF(COUNTIFS($C$2:C34,C35)=0,1,_xlfn.MAXIFS($A$2:A34,$C$2:C34,C35)+1),A34),_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34))</f>
         <v>2</v>
@@ -3160,7 +3161,7 @@
         <v>ImportMoveCL</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" cm="1">
         <f t="array" ref="A36">IF(ISNA(_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35)),IF(COUNTIFS($P$2:P36,P36)=1,IF(COUNTIFS($C$2:C35,C36)=0,1,_xlfn.MAXIFS($A$2:A35,$C$2:C35,C36)+1),A35),_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35))</f>
         <v>1</v>
@@ -3212,7 +3213,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" cm="1">
         <f t="array" ref="A37">IF(ISNA(_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36)),IF(COUNTIFS($P$2:P37,P37)=1,IF(COUNTIFS($C$2:C36,C37)=0,1,_xlfn.MAXIFS($A$2:A36,$C$2:C36,C37)+1),A36),_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36))</f>
         <v>1</v>
@@ -3264,7 +3265,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" cm="1">
         <f t="array" ref="A38">IF(ISNA(_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37)),IF(COUNTIFS($P$2:P38,P38)=1,IF(COUNTIFS($C$2:C37,C38)=0,1,_xlfn.MAXIFS($A$2:A37,$C$2:C37,C38)+1),A37),_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37))</f>
         <v>1</v>
@@ -3319,7 +3320,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" cm="1">
         <f t="array" ref="A39">IF(ISNA(_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38)),IF(COUNTIFS($P$2:P39,P39)=1,IF(COUNTIFS($C$2:C38,C39)=0,1,_xlfn.MAXIFS($A$2:A38,$C$2:C38,C39)+1),A38),_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38))</f>
         <v>1</v>
@@ -3374,7 +3375,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" cm="1">
         <f t="array" ref="A40">IF(ISNA(_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39)),IF(COUNTIFS($P$2:P40,P40)=1,IF(COUNTIFS($C$2:C39,C40)=0,1,_xlfn.MAXIFS($A$2:A39,$C$2:C39,C40)+1),A39),_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39))</f>
         <v>2</v>
@@ -3426,7 +3427,7 @@
         <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" cm="1">
         <f t="array" ref="A41">IF(ISNA(_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40)),IF(COUNTIFS($P$2:P41,P41)=1,IF(COUNTIFS($C$2:C40,C41)=0,1,_xlfn.MAXIFS($A$2:A40,$C$2:C40,C41)+1),A40),_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40))</f>
         <v>2</v>
@@ -3481,7 +3482,7 @@
         <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" cm="1">
         <f t="array" ref="A42">IF(ISNA(_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41)),IF(COUNTIFS($P$2:P42,P42)=1,IF(COUNTIFS($C$2:C41,C42)=0,1,_xlfn.MAXIFS($A$2:A41,$C$2:C41,C42)+1),A41),_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41))</f>
         <v>3</v>
@@ -3536,7 +3537,7 @@
         <v>Bulwer IslandStoreGP</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" cm="1">
         <f t="array" ref="A43">IF(ISNA(_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42)),IF(COUNTIFS($P$2:P43,P43)=1,IF(COUNTIFS($C$2:C42,C43)=0,1,_xlfn.MAXIFS($A$2:A42,$C$2:C42,C43)+1),A42),_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42))</f>
         <v>4</v>
@@ -3582,7 +3583,7 @@
         <v>Bulwer IslandDeliverGP</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" cm="1">
         <f t="array" ref="A44">IF(ISNA(_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43)),IF(COUNTIFS($P$2:P44,P44)=1,IF(COUNTIFS($C$2:C43,C44)=0,1,_xlfn.MAXIFS($A$2:A43,$C$2:C43,C44)+1),A43),_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43))</f>
         <v>1</v>
@@ -3637,7 +3638,7 @@
         <v>Port KemblaStoreCL</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" cm="1">
         <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),A44),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
         <v>2</v>
@@ -3692,7 +3693,7 @@
         <v>Port KemblaMakeGP</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" cm="1">
         <f t="array" ref="A46">IF(ISNA(_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45)),IF(COUNTIFS($P$2:P46,P46)=1,IF(COUNTIFS($C$2:C45,C46)=0,1,_xlfn.MAXIFS($A$2:A45,$C$2:C45,C46)+1),A45),_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45))</f>
         <v>3</v>
@@ -3744,7 +3745,7 @@
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" cm="1">
         <f t="array" ref="A47">IF(ISNA(_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46)),IF(COUNTIFS($P$2:P47,P47)=1,IF(COUNTIFS($C$2:C46,C47)=0,1,_xlfn.MAXIFS($A$2:A46,$C$2:C46,C47)+1),A46),_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46))</f>
         <v>3</v>
@@ -3796,7 +3797,7 @@
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" cm="1">
         <f t="array" ref="A48">IF(ISNA(_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47)),IF(COUNTIFS($P$2:P48,P48)=1,IF(COUNTIFS($C$2:C47,C48)=0,1,_xlfn.MAXIFS($A$2:A47,$C$2:C47,C48)+1),A47),_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47))</f>
         <v>4</v>
@@ -3848,7 +3849,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" cm="1">
         <f t="array" ref="A49">IF(ISNA(_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48)),IF(COUNTIFS($P$2:P49,P49)=1,IF(COUNTIFS($C$2:C48,C49)=0,1,_xlfn.MAXIFS($A$2:A48,$C$2:C48,C49)+1),A48),_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48))</f>
         <v>4</v>
@@ -3900,7 +3901,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" cm="1">
         <f t="array" ref="A50">IF(ISNA(_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49)),IF(COUNTIFS($P$2:P50,P50)=1,IF(COUNTIFS($C$2:C49,C50)=0,1,_xlfn.MAXIFS($A$2:A49,$C$2:C49,C50)+1),A49),_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49))</f>
         <v>4</v>
@@ -3952,7 +3953,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>4</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>Port KemblaDeliverGP</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" cm="1">
         <f t="array" ref="A52">IF(ISNA(_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51)),IF(COUNTIFS($P$2:P52,P52)=1,IF(COUNTIFS($C$2:C51,C52)=0,1,_xlfn.MAXIFS($A$2:A51,$C$2:C51,C52)+1),A51),_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51))</f>
         <v>1</v>
@@ -4046,7 +4047,7 @@
         <v>NewcastleStoreGP</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" cm="1">
         <f t="array" ref="A53">IF(ISNA(_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52)),IF(COUNTIFS($P$2:P53,P53)=1,IF(COUNTIFS($C$2:C52,C53)=0,1,_xlfn.MAXIFS($A$2:A52,$C$2:C52,C53)+1),A52),_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52))</f>
         <v>2</v>
@@ -4089,7 +4090,7 @@
         <v>NewcastleDeliverGP</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" cm="1">
         <f t="array" ref="A54">IF(ISNA(_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53)),IF(COUNTIFS($P$2:P54,P54)=1,IF(COUNTIFS($C$2:C53,C54)=0,1,_xlfn.MAXIFS($A$2:A53,$C$2:C53,C54)+1),A53),_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53))</f>
         <v>1</v>
@@ -4141,7 +4142,7 @@
         <v>MelbourneStoreGP</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" cm="1">
         <f t="array" ref="A55">IF(ISNA(_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54)),IF(COUNTIFS($P$2:P55,P55)=1,IF(COUNTIFS($C$2:C54,C55)=0,1,_xlfn.MAXIFS($A$2:A54,$C$2:C54,C55)+1),A54),_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54))</f>
         <v>2</v>
@@ -4184,7 +4185,7 @@
         <v>MelbourneDeliverGP</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" cm="1">
         <f t="array" ref="A56">IF(ISNA(_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55)),IF(COUNTIFS($P$2:P56,P56)=1,IF(COUNTIFS($C$2:C55,C56)=0,1,_xlfn.MAXIFS($A$2:A55,$C$2:C55,C56)+1),A55),_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55))</f>
         <v>1</v>
@@ -4236,7 +4237,7 @@
         <v>OsbornStoreGP</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" cm="1">
         <f t="array" ref="A57">IF(ISNA(_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56)),IF(COUNTIFS($P$2:P57,P57)=1,IF(COUNTIFS($C$2:C56,C57)=0,1,_xlfn.MAXIFS($A$2:A56,$C$2:C56,C57)+1),A56),_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56))</f>
         <v>2</v>
@@ -4279,7 +4280,7 @@
         <v>OsbornDeliverGP</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" cm="1">
         <f t="array" ref="A58">IF(ISNA(_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57)),IF(COUNTIFS($P$2:P58,P58)=1,IF(COUNTIFS($C$2:C57,C58)=0,1,_xlfn.MAXIFS($A$2:A57,$C$2:C57,C58)+1),A57),_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57))</f>
         <v>1</v>
@@ -4331,7 +4332,7 @@
         <v>TownsvilleStoreGP</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" cm="1">
         <f t="array" ref="A59">IF(ISNA(_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58)),IF(COUNTIFS($P$2:P59,P59)=1,IF(COUNTIFS($C$2:C58,C59)=0,1,_xlfn.MAXIFS($A$2:A58,$C$2:C58,C59)+1),A58),_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58))</f>
         <v>2</v>
@@ -4374,7 +4375,7 @@
         <v>TownsvilleDeliverGP</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" cm="1">
         <f t="array" ref="A60">IF(ISNA(_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59)),IF(COUNTIFS($P$2:P60,P60)=1,IF(COUNTIFS($C$2:C59,C60)=0,1,_xlfn.MAXIFS($A$2:A59,$C$2:C59,C60)+1),A59),_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59))</f>
         <v>1</v>
@@ -4426,7 +4427,7 @@
         <v>MackayStoreGP</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" cm="1">
         <f t="array" ref="A61">IF(ISNA(_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60)),IF(COUNTIFS($P$2:P61,P61)=1,IF(COUNTIFS($C$2:C60,C61)=0,1,_xlfn.MAXIFS($A$2:A60,$C$2:C60,C61)+1),A60),_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60))</f>
         <v>2</v>
@@ -4469,7 +4470,7 @@
         <v>MackayDeliverGP</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" cm="1">
         <f t="array" ref="A62">IF(ISNA(_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61)),IF(COUNTIFS($P$2:P62,P62)=1,IF(COUNTIFS($C$2:C61,C62)=0,1,_xlfn.MAXIFS($A$2:A61,$C$2:C61,C62)+1),A61),_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61))</f>
         <v>1</v>
@@ -4521,7 +4522,7 @@
         <v>WaggaStoreGP</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" cm="1">
         <f t="array" ref="A63">IF(ISNA(_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62)),IF(COUNTIFS($P$2:P63,P63)=1,IF(COUNTIFS($C$2:C62,C63)=0,1,_xlfn.MAXIFS($A$2:A62,$C$2:C62,C63)+1),A62),_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62))</f>
         <v>2</v>
@@ -4564,7 +4565,7 @@
         <v>WaggaDeliverGP</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" cm="1">
         <f t="array" ref="A64">IF(ISNA(_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63)),IF(COUNTIFS($P$2:P64,P64)=1,IF(COUNTIFS($C$2:C63,C64)=0,1,_xlfn.MAXIFS($A$2:A63,$C$2:C63,C64)+1),A63),_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63))</f>
         <v>1</v>
@@ -4616,7 +4617,7 @@
         <v>AlburyStoreGP</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" cm="1">
         <f t="array" ref="A65">IF(ISNA(_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64)),IF(COUNTIFS($P$2:P65,P65)=1,IF(COUNTIFS($C$2:C64,C65)=0,1,_xlfn.MAXIFS($A$2:A64,$C$2:C64,C65)+1),A64),_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64))</f>
         <v>2</v>
@@ -4651,7 +4652,7 @@
         <v>AlburyDeliverGP</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" cm="1">
         <f t="array" ref="A66">IF(ISNA(_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65)),IF(COUNTIFS($P$2:P66,P66)=1,IF(COUNTIFS($C$2:C65,C66)=0,1,_xlfn.MAXIFS($A$2:A65,$C$2:C65,C66)+1),A65),_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65))</f>
         <v>1</v>
@@ -4695,7 +4696,7 @@
         <v>ClydeStoreGP</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" cm="1">
         <f t="array" ref="A67">IF(ISNA(_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66)),IF(COUNTIFS($P$2:P67,P67)=1,IF(COUNTIFS($C$2:C66,C67)=0,1,_xlfn.MAXIFS($A$2:A66,$C$2:C66,C67)+1),A66),_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66))</f>
         <v>2</v>
@@ -4730,7 +4731,7 @@
         <v>ClydeDeliverGP</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>GladstoneMakeFA</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2</v>
       </c>
@@ -4801,7 +4802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -4836,7 +4837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>3</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>3</v>
       </c>
@@ -4906,7 +4907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1</v>
       </c>
@@ -4941,7 +4942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -4976,7 +4977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2</v>
       </c>
@@ -5037,7 +5038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1</v>
       </c>
@@ -5124,7 +5125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2</v>
       </c>
@@ -5159,7 +5160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1</v>
       </c>
@@ -5229,7 +5230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -5264,7 +5265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>3</v>
       </c>
@@ -5299,7 +5300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>4</v>
       </c>
@@ -5325,7 +5326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>3</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -5395,7 +5396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>4</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>4</v>
       </c>
@@ -5465,7 +5466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>4</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>4</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1</v>
       </c>
@@ -5605,7 +5606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2</v>
       </c>
@@ -5675,7 +5676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>3</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>3</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>4</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>4</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1</v>
       </c>
@@ -5841,7 +5842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>1</v>
       </c>
@@ -5902,7 +5903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2</v>
       </c>
@@ -5928,7 +5929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -5963,7 +5964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2</v>
       </c>
@@ -5989,7 +5990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1</v>
       </c>
@@ -6024,7 +6025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>1</v>
       </c>
@@ -6085,7 +6086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -6112,7 +6113,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K109" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:K109" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Railton"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="M1:N1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -6547,8 +6554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7502,7 +7509,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7604,7 +7611,7 @@
         <v>30</v>
       </c>
       <c r="E3">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -7639,7 +7646,7 @@
         <v>38</v>
       </c>
       <c r="E4">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -8434,7 +8441,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" activeCellId="2" sqref="D16 D18 D11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
13 DEC - Added Grok Sim version
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="969" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A16261E6-5C7B-44D8-8456-5FFC60772E8E}"/>
+  <xr:revisionPtr revIDLastSave="970" documentId="11_7702EEA085167BEC471CB38504FABC4A36F5DBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5CE7083-C28A-45E1-BEB5-6636EACD566E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1243,14 +1243,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight" activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1368,7 +1367,7 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" cm="1">
         <f t="array" ref="A3">IF(ISNA(_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,_xlfn.MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),_xlfn.XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
         <v>2</v>
@@ -1427,7 +1426,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" cm="1">
         <f t="array" ref="A4">IF(ISNA(_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3)),IF(COUNTIFS($P$2:P4,P4)=1,IF(COUNTIFS($C$2:C3,C4)=0,1,_xlfn.MAXIFS($A$2:A3,$C$2:C3,C4)+1),A3),_xlfn.XLOOKUP(P4,$P$2:P3,$A$2:A3))</f>
         <v>3</v>
@@ -1482,7 +1481,7 @@
         <v>GladstoneMoveCL</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(ISNA(_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4)),IF(COUNTIFS($P$2:P5,P5)=1,IF(COUNTIFS($C$2:C4,C5)=0,1,_xlfn.MAXIFS($A$2:A4,$C$2:C4,C5)+1),A4),_xlfn.XLOOKUP(P5,$P$2:P4,$A$2:A4))</f>
         <v>2</v>
@@ -1537,7 +1536,7 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" cm="1">
         <f t="array" ref="A6">IF(ISNA(_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5)),IF(COUNTIFS($P$2:P6,P6)=1,IF(COUNTIFS($C$2:C5,C6)=0,1,_xlfn.MAXIFS($A$2:A5,$C$2:C5,C6)+1),A5),_xlfn.XLOOKUP(P6,$P$2:P5,$A$2:A5))</f>
         <v>2</v>
@@ -1592,7 +1591,7 @@
         <v>GladstoneStoreCL</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" cm="1">
         <f t="array" ref="A7">IF(ISNA(_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6)),IF(COUNTIFS($P$2:P7,P7)=1,IF(COUNTIFS($C$2:C6,C7)=0,1,_xlfn.MAXIFS($A$2:A6,$C$2:C6,C7)+1),A6),_xlfn.XLOOKUP(P7,$P$2:P6,$A$2:A6))</f>
         <v>4</v>
@@ -1647,7 +1646,7 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" cm="1">
         <f t="array" ref="A8">IF(ISNA(_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7)),IF(COUNTIFS($P$2:P8,P8)=1,IF(COUNTIFS($C$2:C7,C8)=0,1,_xlfn.MAXIFS($A$2:A7,$C$2:C7,C8)+1),A7),_xlfn.XLOOKUP(P8,$P$2:P7,$A$2:A7))</f>
         <v>4</v>
@@ -1702,7 +1701,7 @@
         <v>GladstoneMakeGP</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" cm="1">
         <f t="array" ref="A9">IF(ISNA(_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8)),IF(COUNTIFS($P$2:P9,P9)=1,IF(COUNTIFS($C$2:C8,C9)=0,1,_xlfn.MAXIFS($A$2:A8,$C$2:C8,C9)+1),A8),_xlfn.XLOOKUP(P9,$P$2:P8,$A$2:A8))</f>
         <v>5</v>
@@ -1757,7 +1756,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" cm="1">
         <f t="array" ref="A10">IF(ISNA(_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9)),IF(COUNTIFS($P$2:P10,P10)=1,IF(COUNTIFS($C$2:C9,C10)=0,1,_xlfn.MAXIFS($A$2:A9,$C$2:C9,C10)+1),A9),_xlfn.XLOOKUP(P10,$P$2:P9,$A$2:A9))</f>
         <v>5</v>
@@ -1812,7 +1811,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" cm="1">
         <f t="array" ref="A11">IF(ISNA(_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10)),IF(COUNTIFS($P$2:P11,P11)=1,IF(COUNTIFS($C$2:C10,C11)=0,1,_xlfn.MAXIFS($A$2:A10,$C$2:C10,C11)+1),A10),_xlfn.XLOOKUP(P11,$P$2:P10,$A$2:A10))</f>
         <v>5</v>
@@ -1867,7 +1866,7 @@
         <v>GladstoneStoreGP</v>
       </c>
     </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" cm="1">
         <f t="array" ref="A12">IF(ISNA(_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11)),IF(COUNTIFS($P$2:P12,P12)=1,IF(COUNTIFS($C$2:C11,C12)=0,1,_xlfn.MAXIFS($A$2:A11,$C$2:C11,C12)+1),A11),_xlfn.XLOOKUP(P12,$P$2:P11,$A$2:A11))</f>
         <v>6</v>
@@ -1922,7 +1921,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" cm="1">
         <f t="array" ref="A13">IF(ISNA(_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12)),IF(COUNTIFS($P$2:P13,P13)=1,IF(COUNTIFS($C$2:C12,C13)=0,1,_xlfn.MAXIFS($A$2:A12,$C$2:C12,C13)+1),A12),_xlfn.XLOOKUP(P13,$P$2:P12,$A$2:A12))</f>
         <v>6</v>
@@ -1977,7 +1976,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" cm="1">
         <f t="array" ref="A14">IF(ISNA(_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13)),IF(COUNTIFS($P$2:P14,P14)=1,IF(COUNTIFS($C$2:C13,C14)=0,1,_xlfn.MAXIFS($A$2:A13,$C$2:C13,C14)+1),A13),_xlfn.XLOOKUP(P14,$P$2:P13,$A$2:A13))</f>
         <v>6</v>
@@ -2032,7 +2031,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" cm="1">
         <f t="array" ref="A15">IF(ISNA(_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14)),IF(COUNTIFS($P$2:P15,P15)=1,IF(COUNTIFS($C$2:C14,C15)=0,1,_xlfn.MAXIFS($A$2:A14,$C$2:C14,C15)+1),A14),_xlfn.XLOOKUP(P15,$P$2:P14,$A$2:A14))</f>
         <v>6</v>
@@ -2087,7 +2086,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" cm="1">
         <f t="array" ref="A16">IF(ISNA(_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15)),IF(COUNTIFS($P$2:P16,P16)=1,IF(COUNTIFS($C$2:C15,C16)=0,1,_xlfn.MAXIFS($A$2:A15,$C$2:C15,C16)+1),A15),_xlfn.XLOOKUP(P16,$P$2:P15,$A$2:A15))</f>
         <v>6</v>
@@ -2142,7 +2141,7 @@
         <v>GladstoneMoveGP</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>RailtonDeliverGP</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" cm="1">
         <f t="array" ref="A29">IF(ISNA(_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28)),IF(COUNTIFS($P$2:P29,P29)=1,IF(COUNTIFS($C$2:C28,C29)=0,1,_xlfn.MAXIFS($A$2:A28,$C$2:C28,C29)+1),A28),_xlfn.XLOOKUP(P29,$P$2:P28,$A$2:A28))</f>
         <v>1</v>
@@ -2837,7 +2836,7 @@
         <v>DevonportStoreGP</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" cm="1">
         <f t="array" ref="A30">IF(ISNA(_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29)),IF(COUNTIFS($P$2:P30,P30)=1,IF(COUNTIFS($C$2:C29,C30)=0,1,_xlfn.MAXIFS($A$2:A29,$C$2:C29,C30)+1),A29),_xlfn.XLOOKUP(P30,$P$2:P29,$A$2:A29))</f>
         <v>2</v>
@@ -2892,7 +2891,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" cm="1">
         <f t="array" ref="A31">IF(ISNA(_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30)),IF(COUNTIFS($P$2:P31,P31)=1,IF(COUNTIFS($C$2:C30,C31)=0,1,_xlfn.MAXIFS($A$2:A30,$C$2:C30,C31)+1),A30),_xlfn.XLOOKUP(P31,$P$2:P30,$A$2:A30))</f>
         <v>2</v>
@@ -2947,7 +2946,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" cm="1">
         <f t="array" ref="A32">IF(ISNA(_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31)),IF(COUNTIFS($P$2:P32,P32)=1,IF(COUNTIFS($C$2:C31,C32)=0,1,_xlfn.MAXIFS($A$2:A31,$C$2:C31,C32)+1),A31),_xlfn.XLOOKUP(P32,$P$2:P31,$A$2:A31))</f>
         <v>2</v>
@@ -3002,7 +3001,7 @@
         <v>DevonportMoveGP</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" cm="1">
         <f t="array" ref="A33">IF(ISNA(_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32)),IF(COUNTIFS($P$2:P33,P33)=1,IF(COUNTIFS($C$2:C32,C33)=0,1,_xlfn.MAXIFS($A$2:A32,$C$2:C32,C33)+1),A32),_xlfn.XLOOKUP(P33,$P$2:P32,$A$2:A32))</f>
         <v>1</v>
@@ -3057,7 +3056,7 @@
         <v>ImportStoreCL</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" cm="1">
         <f t="array" ref="A34">IF(ISNA(_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33)),IF(COUNTIFS($P$2:P34,P34)=1,IF(COUNTIFS($C$2:C33,C34)=0,1,_xlfn.MAXIFS($A$2:A33,$C$2:C33,C34)+1),A33),_xlfn.XLOOKUP(P34,$P$2:P33,$A$2:A33))</f>
         <v>2</v>
@@ -3109,7 +3108,7 @@
         <v>ImportMoveCL</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" cm="1">
         <f t="array" ref="A35">IF(ISNA(_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34)),IF(COUNTIFS($P$2:P35,P35)=1,IF(COUNTIFS($C$2:C34,C35)=0,1,_xlfn.MAXIFS($A$2:A34,$C$2:C34,C35)+1),A34),_xlfn.XLOOKUP(P35,$P$2:P34,$A$2:A34))</f>
         <v>2</v>
@@ -3161,7 +3160,7 @@
         <v>ImportMoveCL</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" cm="1">
         <f t="array" ref="A36">IF(ISNA(_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35)),IF(COUNTIFS($P$2:P36,P36)=1,IF(COUNTIFS($C$2:C35,C36)=0,1,_xlfn.MAXIFS($A$2:A35,$C$2:C35,C36)+1),A35),_xlfn.XLOOKUP(P36,$P$2:P35,$A$2:A35))</f>
         <v>1</v>
@@ -3213,7 +3212,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" cm="1">
         <f t="array" ref="A37">IF(ISNA(_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36)),IF(COUNTIFS($P$2:P37,P37)=1,IF(COUNTIFS($C$2:C36,C37)=0,1,_xlfn.MAXIFS($A$2:A36,$C$2:C36,C37)+1),A36),_xlfn.XLOOKUP(P37,$P$2:P36,$A$2:A36))</f>
         <v>1</v>
@@ -3265,7 +3264,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" cm="1">
         <f t="array" ref="A38">IF(ISNA(_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37)),IF(COUNTIFS($P$2:P38,P38)=1,IF(COUNTIFS($C$2:C37,C38)=0,1,_xlfn.MAXIFS($A$2:A37,$C$2:C37,C38)+1),A37),_xlfn.XLOOKUP(P38,$P$2:P37,$A$2:A37))</f>
         <v>1</v>
@@ -3320,7 +3319,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" cm="1">
         <f t="array" ref="A39">IF(ISNA(_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38)),IF(COUNTIFS($P$2:P39,P39)=1,IF(COUNTIFS($C$2:C38,C39)=0,1,_xlfn.MAXIFS($A$2:A38,$C$2:C38,C39)+1),A38),_xlfn.XLOOKUP(P39,$P$2:P38,$A$2:A38))</f>
         <v>1</v>
@@ -3375,7 +3374,7 @@
         <v>Bulwer IslandStoreCL</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" cm="1">
         <f t="array" ref="A40">IF(ISNA(_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39)),IF(COUNTIFS($P$2:P40,P40)=1,IF(COUNTIFS($C$2:C39,C40)=0,1,_xlfn.MAXIFS($A$2:A39,$C$2:C39,C40)+1),A39),_xlfn.XLOOKUP(P40,$P$2:P39,$A$2:A39))</f>
         <v>2</v>
@@ -3427,7 +3426,7 @@
         <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" cm="1">
         <f t="array" ref="A41">IF(ISNA(_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40)),IF(COUNTIFS($P$2:P41,P41)=1,IF(COUNTIFS($C$2:C40,C41)=0,1,_xlfn.MAXIFS($A$2:A40,$C$2:C40,C41)+1),A40),_xlfn.XLOOKUP(P41,$P$2:P40,$A$2:A40))</f>
         <v>2</v>
@@ -3482,7 +3481,7 @@
         <v>Bulwer IslandMakeGP</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" cm="1">
         <f t="array" ref="A42">IF(ISNA(_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41)),IF(COUNTIFS($P$2:P42,P42)=1,IF(COUNTIFS($C$2:C41,C42)=0,1,_xlfn.MAXIFS($A$2:A41,$C$2:C41,C42)+1),A41),_xlfn.XLOOKUP(P42,$P$2:P41,$A$2:A41))</f>
         <v>3</v>
@@ -3537,7 +3536,7 @@
         <v>Bulwer IslandStoreGP</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" cm="1">
         <f t="array" ref="A43">IF(ISNA(_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42)),IF(COUNTIFS($P$2:P43,P43)=1,IF(COUNTIFS($C$2:C42,C43)=0,1,_xlfn.MAXIFS($A$2:A42,$C$2:C42,C43)+1),A42),_xlfn.XLOOKUP(P43,$P$2:P42,$A$2:A42))</f>
         <v>4</v>
@@ -3583,7 +3582,7 @@
         <v>Bulwer IslandDeliverGP</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" cm="1">
         <f t="array" ref="A44">IF(ISNA(_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43)),IF(COUNTIFS($P$2:P44,P44)=1,IF(COUNTIFS($C$2:C43,C44)=0,1,_xlfn.MAXIFS($A$2:A43,$C$2:C43,C44)+1),A43),_xlfn.XLOOKUP(P44,$P$2:P43,$A$2:A43))</f>
         <v>1</v>
@@ -3638,7 +3637,7 @@
         <v>Port KemblaStoreCL</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" cm="1">
         <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),A44),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
         <v>2</v>
@@ -3693,7 +3692,7 @@
         <v>Port KemblaMakeGP</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" cm="1">
         <f t="array" ref="A46">IF(ISNA(_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45)),IF(COUNTIFS($P$2:P46,P46)=1,IF(COUNTIFS($C$2:C45,C46)=0,1,_xlfn.MAXIFS($A$2:A45,$C$2:C45,C46)+1),A45),_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45))</f>
         <v>3</v>
@@ -3745,7 +3744,7 @@
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" cm="1">
         <f t="array" ref="A47">IF(ISNA(_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46)),IF(COUNTIFS($P$2:P47,P47)=1,IF(COUNTIFS($C$2:C46,C47)=0,1,_xlfn.MAXIFS($A$2:A46,$C$2:C46,C47)+1),A46),_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46))</f>
         <v>3</v>
@@ -3797,7 +3796,7 @@
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" cm="1">
         <f t="array" ref="A48">IF(ISNA(_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47)),IF(COUNTIFS($P$2:P48,P48)=1,IF(COUNTIFS($C$2:C47,C48)=0,1,_xlfn.MAXIFS($A$2:A47,$C$2:C47,C48)+1),A47),_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47))</f>
         <v>4</v>
@@ -3849,7 +3848,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" cm="1">
         <f t="array" ref="A49">IF(ISNA(_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48)),IF(COUNTIFS($P$2:P49,P49)=1,IF(COUNTIFS($C$2:C48,C49)=0,1,_xlfn.MAXIFS($A$2:A48,$C$2:C48,C49)+1),A48),_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48))</f>
         <v>4</v>
@@ -3901,7 +3900,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" cm="1">
         <f t="array" ref="A50">IF(ISNA(_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49)),IF(COUNTIFS($P$2:P50,P50)=1,IF(COUNTIFS($C$2:C49,C50)=0,1,_xlfn.MAXIFS($A$2:A49,$C$2:C49,C50)+1),A49),_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49))</f>
         <v>4</v>
@@ -3953,7 +3952,7 @@
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>4</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>Port KemblaDeliverGP</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" cm="1">
         <f t="array" ref="A52">IF(ISNA(_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51)),IF(COUNTIFS($P$2:P52,P52)=1,IF(COUNTIFS($C$2:C51,C52)=0,1,_xlfn.MAXIFS($A$2:A51,$C$2:C51,C52)+1),A51),_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51))</f>
         <v>1</v>
@@ -4047,7 +4046,7 @@
         <v>NewcastleStoreGP</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" cm="1">
         <f t="array" ref="A53">IF(ISNA(_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52)),IF(COUNTIFS($P$2:P53,P53)=1,IF(COUNTIFS($C$2:C52,C53)=0,1,_xlfn.MAXIFS($A$2:A52,$C$2:C52,C53)+1),A52),_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52))</f>
         <v>2</v>
@@ -4090,7 +4089,7 @@
         <v>NewcastleDeliverGP</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" cm="1">
         <f t="array" ref="A54">IF(ISNA(_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53)),IF(COUNTIFS($P$2:P54,P54)=1,IF(COUNTIFS($C$2:C53,C54)=0,1,_xlfn.MAXIFS($A$2:A53,$C$2:C53,C54)+1),A53),_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53))</f>
         <v>1</v>
@@ -4142,7 +4141,7 @@
         <v>MelbourneStoreGP</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" cm="1">
         <f t="array" ref="A55">IF(ISNA(_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54)),IF(COUNTIFS($P$2:P55,P55)=1,IF(COUNTIFS($C$2:C54,C55)=0,1,_xlfn.MAXIFS($A$2:A54,$C$2:C54,C55)+1),A54),_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54))</f>
         <v>2</v>
@@ -4185,7 +4184,7 @@
         <v>MelbourneDeliverGP</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" cm="1">
         <f t="array" ref="A56">IF(ISNA(_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55)),IF(COUNTIFS($P$2:P56,P56)=1,IF(COUNTIFS($C$2:C55,C56)=0,1,_xlfn.MAXIFS($A$2:A55,$C$2:C55,C56)+1),A55),_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55))</f>
         <v>1</v>
@@ -4237,7 +4236,7 @@
         <v>OsbornStoreGP</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" cm="1">
         <f t="array" ref="A57">IF(ISNA(_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56)),IF(COUNTIFS($P$2:P57,P57)=1,IF(COUNTIFS($C$2:C56,C57)=0,1,_xlfn.MAXIFS($A$2:A56,$C$2:C56,C57)+1),A56),_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56))</f>
         <v>2</v>
@@ -4280,7 +4279,7 @@
         <v>OsbornDeliverGP</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" cm="1">
         <f t="array" ref="A58">IF(ISNA(_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57)),IF(COUNTIFS($P$2:P58,P58)=1,IF(COUNTIFS($C$2:C57,C58)=0,1,_xlfn.MAXIFS($A$2:A57,$C$2:C57,C58)+1),A57),_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57))</f>
         <v>1</v>
@@ -4332,7 +4331,7 @@
         <v>TownsvilleStoreGP</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" cm="1">
         <f t="array" ref="A59">IF(ISNA(_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58)),IF(COUNTIFS($P$2:P59,P59)=1,IF(COUNTIFS($C$2:C58,C59)=0,1,_xlfn.MAXIFS($A$2:A58,$C$2:C58,C59)+1),A58),_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58))</f>
         <v>2</v>
@@ -4375,7 +4374,7 @@
         <v>TownsvilleDeliverGP</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" cm="1">
         <f t="array" ref="A60">IF(ISNA(_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59)),IF(COUNTIFS($P$2:P60,P60)=1,IF(COUNTIFS($C$2:C59,C60)=0,1,_xlfn.MAXIFS($A$2:A59,$C$2:C59,C60)+1),A59),_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59))</f>
         <v>1</v>
@@ -4427,7 +4426,7 @@
         <v>MackayStoreGP</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" cm="1">
         <f t="array" ref="A61">IF(ISNA(_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60)),IF(COUNTIFS($P$2:P61,P61)=1,IF(COUNTIFS($C$2:C60,C61)=0,1,_xlfn.MAXIFS($A$2:A60,$C$2:C60,C61)+1),A60),_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60))</f>
         <v>2</v>
@@ -4470,7 +4469,7 @@
         <v>MackayDeliverGP</v>
       </c>
     </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" cm="1">
         <f t="array" ref="A62">IF(ISNA(_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61)),IF(COUNTIFS($P$2:P62,P62)=1,IF(COUNTIFS($C$2:C61,C62)=0,1,_xlfn.MAXIFS($A$2:A61,$C$2:C61,C62)+1),A61),_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61))</f>
         <v>1</v>
@@ -4522,7 +4521,7 @@
         <v>WaggaStoreGP</v>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" cm="1">
         <f t="array" ref="A63">IF(ISNA(_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62)),IF(COUNTIFS($P$2:P63,P63)=1,IF(COUNTIFS($C$2:C62,C63)=0,1,_xlfn.MAXIFS($A$2:A62,$C$2:C62,C63)+1),A62),_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62))</f>
         <v>2</v>
@@ -4565,7 +4564,7 @@
         <v>WaggaDeliverGP</v>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" cm="1">
         <f t="array" ref="A64">IF(ISNA(_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63)),IF(COUNTIFS($P$2:P64,P64)=1,IF(COUNTIFS($C$2:C63,C64)=0,1,_xlfn.MAXIFS($A$2:A63,$C$2:C63,C64)+1),A63),_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63))</f>
         <v>1</v>
@@ -4617,7 +4616,7 @@
         <v>AlburyStoreGP</v>
       </c>
     </row>
-    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" cm="1">
         <f t="array" ref="A65">IF(ISNA(_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64)),IF(COUNTIFS($P$2:P65,P65)=1,IF(COUNTIFS($C$2:C64,C65)=0,1,_xlfn.MAXIFS($A$2:A64,$C$2:C64,C65)+1),A64),_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64))</f>
         <v>2</v>
@@ -4652,7 +4651,7 @@
         <v>AlburyDeliverGP</v>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" cm="1">
         <f t="array" ref="A66">IF(ISNA(_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65)),IF(COUNTIFS($P$2:P66,P66)=1,IF(COUNTIFS($C$2:C65,C66)=0,1,_xlfn.MAXIFS($A$2:A65,$C$2:C65,C66)+1),A65),_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65))</f>
         <v>1</v>
@@ -4696,7 +4695,7 @@
         <v>ClydeStoreGP</v>
       </c>
     </row>
-    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" cm="1">
         <f t="array" ref="A67">IF(ISNA(_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66)),IF(COUNTIFS($P$2:P67,P67)=1,IF(COUNTIFS($C$2:C66,C67)=0,1,_xlfn.MAXIFS($A$2:A66,$C$2:C66,C67)+1),A66),_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66))</f>
         <v>2</v>
@@ -4731,7 +4730,7 @@
         <v>ClydeDeliverGP</v>
       </c>
     </row>
-    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>GladstoneMakeFA</v>
       </c>
     </row>
-    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2</v>
       </c>
@@ -4802,7 +4801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>3</v>
       </c>
@@ -4872,7 +4871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>3</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1</v>
       </c>
@@ -4942,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -4977,7 +4976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1</v>
       </c>
@@ -5012,7 +5011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2</v>
       </c>
@@ -5038,7 +5037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2</v>
       </c>
@@ -5064,7 +5063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2</v>
       </c>
@@ -5090,7 +5089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1</v>
       </c>
@@ -5125,7 +5124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2</v>
       </c>
@@ -5160,7 +5159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2</v>
       </c>
@@ -5195,7 +5194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1</v>
       </c>
@@ -5230,7 +5229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -5265,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>3</v>
       </c>
@@ -5300,7 +5299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>4</v>
       </c>
@@ -5326,7 +5325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>3</v>
       </c>
@@ -5361,7 +5360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -5396,7 +5395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>4</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>4</v>
       </c>
@@ -5466,7 +5465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>4</v>
       </c>
@@ -5501,7 +5500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>4</v>
       </c>
@@ -5536,7 +5535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1</v>
       </c>
@@ -5571,7 +5570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1</v>
       </c>
@@ -5606,7 +5605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2</v>
       </c>
@@ -5641,7 +5640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2</v>
       </c>
@@ -5676,7 +5675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>3</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>3</v>
       </c>
@@ -5746,7 +5745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>4</v>
       </c>
@@ -5781,7 +5780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>4</v>
       </c>
@@ -5807,7 +5806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1</v>
       </c>
@@ -5842,7 +5841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>1</v>
       </c>
@@ -5903,7 +5902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2</v>
       </c>
@@ -5929,7 +5928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2</v>
       </c>
@@ -5990,7 +5989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1</v>
       </c>
@@ -6025,7 +6024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2</v>
       </c>
@@ -6051,7 +6050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>1</v>
       </c>
@@ -6086,7 +6085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -6113,13 +6112,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K109" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Railton"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:K109" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="M1:N1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -15557,17 +15550,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -15822,6 +15804,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
   <ds:schemaRefs>
@@ -15831,17 +15824,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15858,4 +15840,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code now very modular, many smaller integrated scripts to adjustments are made on small segments only.
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E95670B-2C56-4D9C-BF68-5BF9EDB64562}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97818669-65CA-43C2-8BE5-964F4CD7F304}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,7 +706,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,6 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6608,7 +6615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -8216,8 +8223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA5544C-34DA-4E23-978C-2BA3091E3A4F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,7 +8299,7 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E2" t="s">
@@ -8336,7 +8343,7 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="16" t="s">
         <v>51</v>
       </c>
       <c r="E3" t="s">
@@ -8380,7 +8387,7 @@
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E4" t="s">
@@ -8424,7 +8431,7 @@
       <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E5" t="s">
@@ -8512,7 +8519,7 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>77</v>
       </c>
       <c r="E7" t="s">
@@ -8556,7 +8563,7 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="16" t="s">
         <v>78</v>
       </c>
       <c r="E8" t="s">
@@ -8600,7 +8607,7 @@
       <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E9" t="s">
@@ -8644,7 +8651,7 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E10" t="s">
@@ -9603,26 +9610,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9877,10 +9864,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9897,20 +9915,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update interactive report button style after simulation completion
Add an ID to the 'View Interactive Report' button and implement JavaScript to change its class from 'btn-outline-light' to 'btn-primary' upon successful report generation, visually indicating report readiness.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: ed37ccb4-a993-463b-92a3-c52b37080af4
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/31ejA8F
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97818669-65CA-43C2-8BE5-964F4CD7F304}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E87A31EF-1EF8-4B43-B74D-80F5223868D7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="178">
   <si>
     <t>Setting</t>
   </si>
@@ -594,6 +595,15 @@
   </si>
   <si>
     <t>Silo Q, No Shipping</t>
+  </si>
+  <si>
+    <t>&lt;- This is part of North, Duplicate so data prep will ignore this line</t>
+  </si>
+  <si>
+    <t>Route 14</t>
+  </si>
+  <si>
+    <t>Route 15</t>
   </si>
 </sst>
 </file>
@@ -1092,6 +1102,7 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1142,6 +1153,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C14"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1319,6 +1331,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6196,6 +6209,7 @@
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M12" sqref="M11:M12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6618,6 +6632,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7790,6 +7805,7 @@
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8223,9 +8239,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA5544C-34DA-4E23-978C-2BA3091E3A4F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8692,11 +8709,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D7C592-8DF8-40A4-9452-62826144206E}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8707,7 +8725,7 @@
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>111</v>
       </c>
@@ -8727,7 +8745,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -8747,7 +8765,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -8767,7 +8785,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -8787,7 +8805,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -8807,7 +8825,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -8825,6 +8843,9 @@
       </c>
       <c r="F6">
         <v>5000</v>
+      </c>
+      <c r="H6" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -8839,6 +8860,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:E11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9042,10 +9064,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9064,7 +9089,7 @@
     <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>146</v>
       </c>
@@ -9107,8 +9132,14 @@
       <c r="N1" s="12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -9131,28 +9162,34 @@
         <v>145</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J2" t="s">
         <v>144</v>
       </c>
       <c r="K2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M2" t="s">
         <v>161</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>161</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>160</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -9175,28 +9212,34 @@
         <v>1.6</v>
       </c>
       <c r="H3">
+        <v>1.7</v>
+      </c>
+      <c r="I3">
+        <v>1.8</v>
+      </c>
+      <c r="J3">
         <v>2.1</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>3.1</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>3.2</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -9219,28 +9262,34 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>80</v>
       </c>
       <c r="K4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
         <v>161</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>161</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>160</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -9263,28 +9312,34 @@
         <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
       </c>
       <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
         <v>24</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>75</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -9307,28 +9362,34 @@
         <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
         <v>33</v>
       </c>
       <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>74</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -9336,7 +9397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -9344,7 +9405,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -9364,22 +9425,22 @@
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
         <v>45</v>
       </c>
       <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
         <v>39</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>158</v>
-      </c>
-      <c r="K9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" t="s">
-        <v>38</v>
       </c>
       <c r="M9" t="s">
         <v>30</v>
@@ -9387,8 +9448,14 @@
       <c r="N9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -9411,28 +9478,34 @@
         <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
       </c>
       <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
         <v>24</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>75</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -9455,28 +9528,34 @@
         <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
         <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="L11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="M11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" t="s">
         <v>74</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -9484,7 +9563,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -9492,73 +9571,73 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>136</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>137</v>
       </c>
       <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="G15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
       <c r="E16" t="s">
         <v>76</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>139</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
       <c r="E18" t="s">
         <v>73</v>
       </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
       <c r="E19" t="s">
         <v>76</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -9581,24 +9660,30 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="J20" t="s">
         <v>80</v>
       </c>
       <c r="K20" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" t="s">
+        <v>80</v>
+      </c>
+      <c r="M20" t="s">
         <v>161</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>161</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>160</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ship route graphs to show product and payload details
Modify the ship timeline plot to display Location|Product on the Y-axis and enhance tooltips to include Route ID and payload in kT.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 6893a2a1-e2d4-4d35-8cef-f9c81f0a4d7e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/ljEblrZ
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E87A31EF-1EF8-4B43-B74D-80F5223868D7}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BBEAB1B-DC46-4A15-ADB7-783589507E4E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
@@ -31,6 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Store!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="177">
   <si>
     <t>Setting</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>Melbourne</t>
-  </si>
-  <si>
-    <t>Osborn</t>
   </si>
   <si>
     <t>CL_STORE_I</t>
@@ -1099,10 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1151,9 +1145,8 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1164,13 +1157,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>163</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1171,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -1189,7 +1182,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>1000</v>
@@ -1208,7 +1201,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -1219,7 +1212,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1230,10 +1223,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7">
         <v>583</v>
@@ -1285,7 +1278,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -1296,7 +1289,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -1325,13 +1318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1504,7 +1493,7 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="S3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2462,7 +2451,7 @@
         <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2517,7 +2506,7 @@
         <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2572,7 +2561,7 @@
         <v>41</v>
       </c>
       <c r="J23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2627,7 +2616,7 @@
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2664,7 +2653,7 @@
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -2719,7 +2708,7 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2789,7 +2778,7 @@
         <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J27" t="s">
         <v>33</v>
@@ -2871,7 +2860,7 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
         <v>33</v>
@@ -2889,7 +2878,7 @@
         <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J29" t="s">
         <v>29</v>
@@ -2926,7 +2915,7 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
@@ -2981,7 +2970,7 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
         <v>29</v>
@@ -2999,7 +2988,7 @@
         <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="J31" t="s">
         <v>33</v>
@@ -3016,7 +3005,7 @@
       </c>
       <c r="N31" t="str">
         <f t="shared" si="1"/>
-        <v>OsbornStoreGP_STOREGP</v>
+        <v>OsborneStoreGP_STOREGP</v>
       </c>
       <c r="O31">
         <f t="shared" si="2"/>
@@ -3036,7 +3025,7 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -3091,7 +3080,7 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D33" t="s">
         <v>26</v>
@@ -3109,7 +3098,7 @@
         <v>28</v>
       </c>
       <c r="I33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J33" t="s">
         <v>29</v>
@@ -3146,7 +3135,7 @@
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D34" t="s">
         <v>29</v>
@@ -3167,7 +3156,7 @@
         <v>38</v>
       </c>
       <c r="J34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K34">
         <v>3</v>
@@ -3198,7 +3187,7 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D35" t="s">
         <v>29</v>
@@ -3219,7 +3208,7 @@
         <v>30</v>
       </c>
       <c r="J35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K35">
         <v>3</v>
@@ -3271,7 +3260,7 @@
         <v>30</v>
       </c>
       <c r="J36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K36">
         <v>2</v>
@@ -3323,7 +3312,7 @@
         <v>30</v>
       </c>
       <c r="J37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K37">
         <v>2</v>
@@ -3357,7 +3346,7 @@
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
@@ -3375,7 +3364,7 @@
         <v>30</v>
       </c>
       <c r="J38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K38">
         <v>2</v>
@@ -3412,7 +3401,7 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
         <v>24</v>
@@ -3430,7 +3419,7 @@
         <v>30</v>
       </c>
       <c r="J39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K39">
         <v>2</v>
@@ -3467,7 +3456,7 @@
         <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" t="s">
         <v>24</v>
@@ -3519,7 +3508,7 @@
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
         <v>24</v>
@@ -3675,7 +3664,7 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E44" t="s">
         <v>24</v>
@@ -3693,7 +3682,7 @@
         <v>38</v>
       </c>
       <c r="J44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -3730,7 +3719,7 @@
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E45" t="s">
         <v>24</v>
@@ -3904,7 +3893,7 @@
         <v>25</v>
       </c>
       <c r="I48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J48" t="s">
         <v>33</v>
@@ -3956,7 +3945,7 @@
         <v>25</v>
       </c>
       <c r="I49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J49" t="s">
         <v>33</v>
@@ -4008,7 +3997,7 @@
         <v>25</v>
       </c>
       <c r="I50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J50" t="s">
         <v>33</v>
@@ -4274,7 +4263,7 @@
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D56" t="s">
         <v>33</v>
@@ -4292,7 +4281,7 @@
         <v>35</v>
       </c>
       <c r="I56" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="J56" t="s">
         <v>36</v>
@@ -4302,11 +4291,11 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornStoreGP_STOREGP</v>
+        <v>OsborneStoreGP_STOREGP</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="5"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>OsborneDeliverTRUCKGP</v>
       </c>
       <c r="O56">
         <f t="shared" si="6"/>
@@ -4314,7 +4303,7 @@
       </c>
       <c r="P56" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornStoreGP</v>
+        <v>OsborneStoreGP</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4326,7 +4315,7 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
         <v>36</v>
@@ -4345,7 +4334,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="4"/>
-        <v>OsbornDeliverTRUCKGP</v>
+        <v>OsborneDeliverTRUCKGP</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="5"/>
@@ -4357,7 +4346,7 @@
       </c>
       <c r="P57" t="str">
         <f t="shared" si="7"/>
-        <v>OsbornDeliverGP</v>
+        <v>OsborneDeliverGP</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4559,7 +4548,7 @@
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
         <v>33</v>
@@ -4577,7 +4566,7 @@
         <v>35</v>
       </c>
       <c r="I62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J62" t="s">
         <v>36</v>
@@ -4611,7 +4600,7 @@
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D63" t="s">
         <v>36</v>
@@ -4654,7 +4643,7 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D64" t="s">
         <v>33</v>
@@ -4672,7 +4661,7 @@
         <v>35</v>
       </c>
       <c r="I64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J64" t="s">
         <v>36</v>
@@ -4706,7 +4695,7 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D65" t="s">
         <v>36</v>
@@ -4741,7 +4730,7 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D66" t="s">
         <v>33</v>
@@ -4759,7 +4748,7 @@
         <v>35</v>
       </c>
       <c r="I66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J66" t="s">
         <v>36</v>
@@ -4785,7 +4774,7 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D67" t="s">
         <v>36</v>
@@ -4816,19 +4805,19 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" t="s">
         <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F68" t="s">
         <v>23</v>
       </c>
       <c r="G68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H68" t="s">
         <v>25</v>
@@ -4837,7 +4826,7 @@
         <v>20</v>
       </c>
       <c r="J68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K68">
         <v>1</v>
@@ -4852,22 +4841,22 @@
         <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" t="s">
         <v>20</v>
       </c>
       <c r="D69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F69" t="s">
         <v>25</v>
       </c>
       <c r="G69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H69" t="s">
         <v>28</v>
@@ -4887,7 +4876,7 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C70" t="s">
         <v>20</v>
@@ -4896,13 +4885,13 @@
         <v>29</v>
       </c>
       <c r="E70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F70" t="s">
         <v>28</v>
       </c>
       <c r="G70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H70" t="s">
         <v>25</v>
@@ -4911,7 +4900,7 @@
         <v>45</v>
       </c>
       <c r="J70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K70">
         <v>3</v>
@@ -4922,7 +4911,7 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C71" t="s">
         <v>20</v>
@@ -4931,13 +4920,13 @@
         <v>29</v>
       </c>
       <c r="E71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
         <v>28</v>
       </c>
       <c r="G71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H71" t="s">
         <v>25</v>
@@ -4946,7 +4935,7 @@
         <v>38</v>
       </c>
       <c r="J71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K71">
         <v>3</v>
@@ -4957,7 +4946,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72" t="s">
         <v>20</v>
@@ -4966,22 +4955,22 @@
         <v>29</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
         <v>28</v>
       </c>
       <c r="G72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H72" t="s">
         <v>25</v>
       </c>
       <c r="I72" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="J72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K72">
         <v>3</v>
@@ -4992,22 +4981,22 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" t="s">
         <v>45</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
         <v>25</v>
       </c>
       <c r="G73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H73" t="s">
         <v>35</v>
@@ -5027,22 +5016,22 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F74" t="s">
         <v>25</v>
       </c>
       <c r="G74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H74" t="s">
         <v>35</v>
@@ -5062,28 +5051,28 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" t="s">
         <v>54</v>
       </c>
-      <c r="C75" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" t="s">
-        <v>55</v>
-      </c>
       <c r="E75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
       </c>
       <c r="G75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H75" t="s">
         <v>35</v>
       </c>
       <c r="I75" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="J75" t="s">
         <v>36</v>
@@ -5097,7 +5086,7 @@
         <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" t="s">
         <v>45</v>
@@ -5106,13 +5095,13 @@
         <v>36</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
         <v>35</v>
       </c>
       <c r="G76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K76">
         <v>4</v>
@@ -5123,7 +5112,7 @@
         <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" t="s">
         <v>38</v>
@@ -5132,13 +5121,13 @@
         <v>36</v>
       </c>
       <c r="E77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F77" t="s">
         <v>35</v>
       </c>
       <c r="G77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K77">
         <v>4</v>
@@ -5149,22 +5138,22 @@
         <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D78" t="s">
         <v>36</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F78" t="s">
         <v>35</v>
       </c>
       <c r="G78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K78">
         <v>4</v>
@@ -5175,28 +5164,28 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" t="s">
         <v>73</v>
       </c>
-      <c r="C79" t="s">
-        <v>160</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>74</v>
-      </c>
-      <c r="E79" t="s">
-        <v>75</v>
       </c>
       <c r="F79" t="s">
         <v>25</v>
       </c>
       <c r="G79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H79" t="s">
         <v>28</v>
       </c>
       <c r="I79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J79" t="s">
         <v>29</v>
@@ -5210,22 +5199,22 @@
         <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D80" t="s">
         <v>29</v>
       </c>
       <c r="E80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F80" t="s">
         <v>28</v>
       </c>
       <c r="G80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H80" t="s">
         <v>25</v>
@@ -5234,7 +5223,7 @@
         <v>38</v>
       </c>
       <c r="J80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K80">
         <v>3</v>
@@ -5245,22 +5234,22 @@
         <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D81" t="s">
         <v>29</v>
       </c>
       <c r="E81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F81" t="s">
         <v>28</v>
       </c>
       <c r="G81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H81" t="s">
         <v>25</v>
@@ -5269,7 +5258,7 @@
         <v>30</v>
       </c>
       <c r="J81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K81">
         <v>3</v>
@@ -5280,22 +5269,22 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C82" t="s">
         <v>38</v>
       </c>
       <c r="D82" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" t="s">
         <v>74</v>
-      </c>
-      <c r="E82" t="s">
-        <v>75</v>
       </c>
       <c r="F82" t="s">
         <v>25</v>
       </c>
       <c r="G82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H82" t="s">
         <v>23</v>
@@ -5304,7 +5293,7 @@
         <v>38</v>
       </c>
       <c r="J82" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K82">
         <v>2</v>
@@ -5315,22 +5304,22 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C83" t="s">
         <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E83" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F83" t="s">
         <v>23</v>
       </c>
       <c r="G83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H83" t="s">
         <v>25</v>
@@ -5339,7 +5328,7 @@
         <v>38</v>
       </c>
       <c r="J83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K83">
         <v>1</v>
@@ -5350,22 +5339,22 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C84" t="s">
         <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F84" t="s">
         <v>25</v>
       </c>
       <c r="G84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H84" t="s">
         <v>35</v>
@@ -5385,7 +5374,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C85" t="s">
         <v>38</v>
@@ -5394,13 +5383,13 @@
         <v>36</v>
       </c>
       <c r="E85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F85" t="s">
         <v>35</v>
       </c>
       <c r="G85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K85">
         <v>4</v>
@@ -5411,22 +5400,22 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C86" t="s">
         <v>38</v>
       </c>
       <c r="D86" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E86" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F86" t="s">
         <v>25</v>
       </c>
       <c r="G86" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H86" t="s">
         <v>28</v>
@@ -5446,22 +5435,22 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C87" t="s">
         <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F87" t="s">
         <v>25</v>
       </c>
       <c r="G87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H87" t="s">
         <v>28</v>
@@ -5481,7 +5470,7 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
         <v>38</v>
@@ -5490,13 +5479,13 @@
         <v>29</v>
       </c>
       <c r="E88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F88" t="s">
         <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H88" t="s">
         <v>25</v>
@@ -5505,7 +5494,7 @@
         <v>45</v>
       </c>
       <c r="J88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K88">
         <v>3</v>
@@ -5516,7 +5505,7 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C89" t="s">
         <v>38</v>
@@ -5525,22 +5514,22 @@
         <v>34</v>
       </c>
       <c r="E89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F89" t="s">
         <v>28</v>
       </c>
       <c r="G89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H89" t="s">
         <v>25</v>
       </c>
       <c r="I89" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K89">
         <v>3</v>
@@ -5551,7 +5540,7 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C90" t="s">
         <v>38</v>
@@ -5560,22 +5549,22 @@
         <v>34</v>
       </c>
       <c r="E90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F90" t="s">
         <v>28</v>
       </c>
       <c r="G90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H90" t="s">
         <v>25</v>
       </c>
       <c r="I90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K90">
         <v>3</v>
@@ -5586,7 +5575,7 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C91" t="s">
         <v>38</v>
@@ -5595,13 +5584,13 @@
         <v>34</v>
       </c>
       <c r="E91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F91" t="s">
         <v>28</v>
       </c>
       <c r="G91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H91" t="s">
         <v>25</v>
@@ -5610,7 +5599,7 @@
         <v>39</v>
       </c>
       <c r="J91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K91">
         <v>3</v>
@@ -5621,22 +5610,22 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C92" t="s">
         <v>30</v>
       </c>
       <c r="D92" t="s">
+        <v>73</v>
+      </c>
+      <c r="E92" t="s">
         <v>74</v>
-      </c>
-      <c r="E92" t="s">
-        <v>75</v>
       </c>
       <c r="F92" t="s">
         <v>25</v>
       </c>
       <c r="G92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H92" t="s">
         <v>23</v>
@@ -5645,7 +5634,7 @@
         <v>30</v>
       </c>
       <c r="J92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K92">
         <v>2</v>
@@ -5656,22 +5645,22 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C93" t="s">
         <v>30</v>
       </c>
       <c r="D93" t="s">
+        <v>73</v>
+      </c>
+      <c r="E93" t="s">
         <v>74</v>
-      </c>
-      <c r="E93" t="s">
-        <v>75</v>
       </c>
       <c r="F93" t="s">
         <v>25</v>
       </c>
       <c r="G93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H93" t="s">
         <v>23</v>
@@ -5680,7 +5669,7 @@
         <v>30</v>
       </c>
       <c r="J93" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K93">
         <v>2</v>
@@ -5691,22 +5680,22 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C94" t="s">
         <v>30</v>
       </c>
       <c r="D94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F94" t="s">
         <v>23</v>
       </c>
       <c r="G94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H94" t="s">
         <v>25</v>
@@ -5715,7 +5704,7 @@
         <v>30</v>
       </c>
       <c r="J94" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5726,22 +5715,22 @@
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C95" t="s">
         <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E95" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F95" t="s">
         <v>23</v>
       </c>
       <c r="G95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H95" t="s">
         <v>25</v>
@@ -5750,7 +5739,7 @@
         <v>30</v>
       </c>
       <c r="J95" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5761,22 +5750,22 @@
         <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C96" t="s">
         <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F96" t="s">
         <v>25</v>
       </c>
       <c r="G96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H96" t="s">
         <v>28</v>
@@ -5796,22 +5785,22 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
         <v>30</v>
       </c>
       <c r="D97" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F97" t="s">
         <v>25</v>
       </c>
       <c r="G97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H97" t="s">
         <v>35</v>
@@ -5831,7 +5820,7 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
@@ -5840,22 +5829,22 @@
         <v>34</v>
       </c>
       <c r="E98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F98" t="s">
         <v>28</v>
       </c>
       <c r="G98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H98" t="s">
         <v>25</v>
       </c>
       <c r="I98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J98" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K98">
         <v>3</v>
@@ -5866,7 +5855,7 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C99" t="s">
         <v>30</v>
@@ -5875,13 +5864,13 @@
         <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F99" t="s">
         <v>35</v>
       </c>
       <c r="G99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K99">
         <v>4</v>
@@ -5892,28 +5881,28 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D100" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F100" t="s">
         <v>25</v>
       </c>
       <c r="G100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H100" t="s">
         <v>35</v>
       </c>
       <c r="I100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J100" t="s">
         <v>36</v>
@@ -5927,22 +5916,22 @@
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D101" t="s">
         <v>36</v>
       </c>
       <c r="E101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F101" t="s">
         <v>35</v>
       </c>
       <c r="G101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K101">
         <v>4</v>
@@ -5953,22 +5942,22 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C102" t="s">
         <v>45</v>
       </c>
       <c r="D102" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F102" t="s">
         <v>25</v>
       </c>
       <c r="G102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H102" t="s">
         <v>35</v>
@@ -5988,7 +5977,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C103" t="s">
         <v>45</v>
@@ -5997,13 +5986,13 @@
         <v>36</v>
       </c>
       <c r="E103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F103" t="s">
         <v>35</v>
       </c>
       <c r="G103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K103">
         <v>4</v>
@@ -6014,28 +6003,28 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C104" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D104" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F104" t="s">
         <v>25</v>
       </c>
       <c r="G104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H104" t="s">
         <v>35</v>
       </c>
       <c r="I104" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J104" t="s">
         <v>36</v>
@@ -6049,22 +6038,22 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C105" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D105" t="s">
         <v>36</v>
       </c>
       <c r="E105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F105" t="s">
         <v>35</v>
       </c>
       <c r="G105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K105">
         <v>4</v>
@@ -6075,28 +6064,28 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C106" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D106" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F106" t="s">
         <v>25</v>
       </c>
       <c r="G106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H106" t="s">
         <v>35</v>
       </c>
       <c r="I106" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J106" t="s">
         <v>36</v>
@@ -6110,22 +6099,22 @@
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D107" t="s">
         <v>36</v>
       </c>
       <c r="E107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F107" t="s">
         <v>35</v>
       </c>
       <c r="G107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -6136,22 +6125,22 @@
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C108" t="s">
         <v>39</v>
       </c>
       <c r="D108" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F108" t="s">
         <v>25</v>
       </c>
       <c r="G108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H108" t="s">
         <v>35</v>
@@ -6171,7 +6160,7 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C109" t="s">
         <v>39</v>
@@ -6180,13 +6169,13 @@
         <v>36</v>
       </c>
       <c r="E109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F109" t="s">
         <v>35</v>
       </c>
       <c r="G109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K109">
         <v>4</v>
@@ -6206,10 +6195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M12" sqref="M11:M12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6223,7 +6209,7 @@
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -6237,19 +6223,19 @@
         <v>12</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6257,7 +6243,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -6272,7 +6258,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6286,13 +6272,13 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -6301,7 +6287,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6315,7 +6301,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -6330,7 +6316,7 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6344,13 +6330,13 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -6359,7 +6345,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6388,7 +6374,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="10">
         <v>0.1646</v>
@@ -6417,7 +6403,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="10">
         <v>0.13189999999999999</v>
@@ -6431,10 +6417,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>120</v>
@@ -6443,7 +6429,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="10">
         <v>0.2</v>
@@ -6469,7 +6455,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="10">
         <v>7.4499999999999997E-2</v>
@@ -6483,7 +6469,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -6498,7 +6484,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="10">
         <v>0.05</v>
@@ -6512,13 +6498,13 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11">
         <v>180</v>
@@ -6527,7 +6513,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="10">
         <v>0.05</v>
@@ -6556,7 +6542,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="10">
         <v>5.2999999999999999E-2</v>
@@ -6585,7 +6571,7 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="10">
         <v>0.1101</v>
@@ -6611,7 +6597,7 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" s="10">
         <v>2.98E-2</v>
@@ -6629,10 +6615,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6655,33 +6640,33 @@
         <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="I1" s="3"/>
       <c r="K1" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -6706,10 +6691,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" t="s">
         <v>84</v>
-      </c>
-      <c r="K2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6742,7 +6727,7 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -6750,7 +6735,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -6775,7 +6760,7 @@
         <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6808,7 +6793,7 @@
         <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -6816,10 +6801,10 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
       </c>
       <c r="D6" s="3">
         <v>50000</v>
@@ -6841,7 +6826,7 @@
         <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -6849,10 +6834,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3">
         <v>10000</v>
@@ -6874,18 +6859,18 @@
         <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3">
         <v>3000</v>
@@ -6904,15 +6889,15 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
         <v>84</v>
-      </c>
-      <c r="K8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -6937,21 +6922,21 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
         <v>84</v>
-      </c>
-      <c r="K9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3">
         <v>3000</v>
@@ -6970,15 +6955,15 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" t="s">
         <v>84</v>
-      </c>
-      <c r="K10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -7006,7 +6991,7 @@
         <v>27</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -7039,7 +7024,7 @@
         <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -7047,10 +7032,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="3">
         <v>14000</v>
@@ -7072,7 +7057,7 @@
         <v>27</v>
       </c>
       <c r="K13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -7105,12 +7090,12 @@
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -7138,18 +7123,18 @@
         <v>27</v>
       </c>
       <c r="K15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
         <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>75</v>
       </c>
       <c r="D16" s="3">
         <v>999999</v>
@@ -7171,7 +7156,7 @@
         <v>27</v>
       </c>
       <c r="K16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -7179,10 +7164,10 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3">
         <v>15000</v>
@@ -7201,10 +7186,10 @@
       </c>
       <c r="I17" s="3"/>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7264,7 +7249,7 @@
         <v>27</v>
       </c>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7272,10 +7257,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3">
         <v>25000</v>
@@ -7297,7 +7282,7 @@
         <v>27</v>
       </c>
       <c r="K20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7330,7 +7315,7 @@
         <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -7338,10 +7323,10 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="3">
         <v>3000</v>
@@ -7363,12 +7348,12 @@
         <v>27</v>
       </c>
       <c r="K22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -7396,18 +7381,18 @@
         <v>27</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3">
         <v>7500</v>
@@ -7429,7 +7414,7 @@
         <v>27</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -7437,7 +7422,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
@@ -7462,7 +7447,7 @@
         <v>27</v>
       </c>
       <c r="K25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -7470,10 +7455,10 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="9">
         <v>15000</v>
@@ -7495,7 +7480,7 @@
         <v>27</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -7503,10 +7488,10 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="9">
         <v>50000</v>
@@ -7558,7 +7543,7 @@
         <v>27</v>
       </c>
       <c r="K28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7566,10 +7551,10 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="3">
         <v>20000</v>
@@ -7591,7 +7576,7 @@
         <v>27</v>
       </c>
       <c r="K29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7624,7 +7609,7 @@
         <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7632,7 +7617,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -7657,7 +7642,7 @@
         <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7665,7 +7650,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -7690,18 +7675,18 @@
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3">
         <v>3000</v>
@@ -7720,10 +7705,10 @@
       </c>
       <c r="I33" s="3"/>
       <c r="J33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" t="s">
         <v>84</v>
-      </c>
-      <c r="K33" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -7756,12 +7741,12 @@
         <v>27</v>
       </c>
       <c r="K34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -7786,10 +7771,10 @@
       </c>
       <c r="I35" s="3"/>
       <c r="J35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" t="s">
         <v>84</v>
-      </c>
-      <c r="K35" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -7802,10 +7787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7824,18 +7808,18 @@
         <v>10</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -7874,10 +7858,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
@@ -7889,13 +7873,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
@@ -7907,7 +7891,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -7925,13 +7909,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
@@ -7982,10 +7966,10 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
@@ -8018,10 +8002,10 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
@@ -8054,10 +8038,10 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
@@ -8069,13 +8053,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="0"/>
@@ -8087,7 +8071,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -8108,10 +8092,10 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="0"/>
@@ -8144,10 +8128,10 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="8">
         <f t="shared" si="0"/>
@@ -8165,7 +8149,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" si="0"/>
@@ -8177,13 +8161,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="8">
         <f t="shared" si="0"/>
@@ -8213,7 +8197,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -8239,10 +8223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA5544C-34DA-4E23-978C-2BA3091E3A4F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8267,43 +8248,43 @@
         <v>7</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="12" t="s">
-        <v>120</v>
-      </c>
       <c r="M1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8361,7 +8342,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
@@ -8405,7 +8386,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
@@ -8449,7 +8430,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -8493,10 +8474,10 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
         <v>33</v>
@@ -8528,22 +8509,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7">
         <v>30</v>
@@ -8572,22 +8553,22 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -8616,22 +8597,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -8660,10 +8641,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -8672,10 +8653,10 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10">
         <v>280</v>
@@ -8711,10 +8692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D7C592-8DF8-40A4-9452-62826144206E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8727,30 +8705,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>123</v>
-      </c>
       <c r="E1" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8770,7 +8748,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -8787,10 +8765,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -8807,10 +8785,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -8830,7 +8808,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -8845,7 +8823,7 @@
         <v>5000</v>
       </c>
       <c r="H6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -8858,9 +8836,8 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8875,16 +8852,16 @@
         <v>8</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8906,7 +8883,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -8940,7 +8917,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8957,7 +8934,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9008,7 +8985,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -9067,10 +9044,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9091,107 +9065,107 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="C1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="L1" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="N1" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="O1" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>1.1000000000000001</v>
@@ -9241,7 +9215,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -9268,30 +9242,30 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -9309,13 +9283,13 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
@@ -9333,18 +9307,18 @@
         <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -9359,13 +9333,13 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
         <v>33</v>
@@ -9383,31 +9357,31 @@
         <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -9440,7 +9414,7 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M9" t="s">
         <v>30</v>
@@ -9457,7 +9431,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -9475,13 +9449,13 @@
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
@@ -9499,18 +9473,18 @@
         <v>24</v>
       </c>
       <c r="O10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -9525,13 +9499,13 @@
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J11" t="s">
         <v>33</v>
@@ -9543,51 +9517,51 @@
         <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
@@ -9595,10 +9569,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I16" t="s">
         <v>33</v>
@@ -9606,7 +9580,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -9617,10 +9591,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -9628,10 +9602,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>33</v>
@@ -9639,7 +9613,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -9666,25 +9640,25 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -9695,6 +9669,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9949,27 +9943,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9986,23 +9979,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update input files to enable Fly Ash shipments
Update Model Inputs.xlsx and generated_model_inputs.xlsx to correct data inconsistencies for Fly Ash product loading.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 0cd1f3b3-0f7c-45b1-8d1b-09835c5065b5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/ljEblrZ
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BBEAB1B-DC46-4A15-ADB7-783589507E4E}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E96A07DA-F201-47AB-86F4-C1550EB69310}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
@@ -30,7 +30,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Store!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -9044,7 +9043,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9333,13 +9332,13 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
         <v>33</v>
@@ -9376,7 +9375,7 @@
         <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -9669,26 +9668,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9943,10 +9922,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9963,20 +9973,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix inconsistent naming for store fields in route normalization
Adjust the ship route normalization logic in `sim_run_data_clean.py` to correctly identify store fields by checking multiple naming patterns, resolving issues with SG and FA route deliveries.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: c9c26929-d9d5-4057-a58f-20fbfe8cb0d1
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/zFJnzwl
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E96A07DA-F201-47AB-86F4-C1550EB69310}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE33CE05-3C88-4DE5-B461-3E15D34AC824}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="178">
   <si>
     <t>Setting</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>Route 15</t>
+  </si>
+  <si>
+    <t>Route 16</t>
   </si>
 </sst>
 </file>
@@ -9040,10 +9043,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I1" activeCellId="2" sqref="A1:A20 E1:E20 I1:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9062,7 +9065,7 @@
     <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>145</v>
       </c>
@@ -9111,8 +9114,11 @@
       <c r="P1" s="12" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -9141,7 +9147,7 @@
         <v>144</v>
       </c>
       <c r="J2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K2" t="s">
         <v>143</v>
@@ -9150,19 +9156,22 @@
         <v>143</v>
       </c>
       <c r="M2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="N2" t="s">
         <v>160</v>
       </c>
       <c r="O2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -9191,28 +9200,31 @@
         <v>1.8</v>
       </c>
       <c r="J3">
+        <v>1.9</v>
+      </c>
+      <c r="K3">
         <v>2.1</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>3.1</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3.2</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -9241,7 +9253,7 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
         <v>79</v>
@@ -9250,19 +9262,22 @@
         <v>79</v>
       </c>
       <c r="M4" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="N4" t="s">
         <v>160</v>
       </c>
       <c r="O4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -9291,7 +9306,7 @@
         <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
@@ -9300,19 +9315,22 @@
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
         <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -9341,7 +9359,7 @@
         <v>107</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="K6" t="s">
         <v>33</v>
@@ -9350,19 +9368,22 @@
         <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
         <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="P6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -9370,7 +9391,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -9378,7 +9399,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -9410,25 +9431,28 @@
         <v>45</v>
       </c>
       <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
         <v>39</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>157</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>30</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>30</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -9457,7 +9481,7 @@
         <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="K10" t="s">
         <v>19</v>
@@ -9466,19 +9490,22 @@
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
         <v>24</v>
       </c>
       <c r="O10" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -9507,7 +9534,7 @@
         <v>54</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
         <v>33</v>
@@ -9516,19 +9543,22 @@
         <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="N11" t="s">
         <v>46</v>
       </c>
       <c r="O11" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="P11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -9536,7 +9566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -9544,40 +9574,40 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
       <c r="E15" t="s">
         <v>72</v>
       </c>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
       <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -9585,10 +9615,13 @@
         <v>45</v>
       </c>
       <c r="I17" t="s">
+        <v>157</v>
+      </c>
+      <c r="J17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -9596,10 +9629,13 @@
         <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -9607,10 +9643,13 @@
         <v>75</v>
       </c>
       <c r="I19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -9639,7 +9678,7 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="K20" t="s">
         <v>79</v>
@@ -9648,15 +9687,18 @@
         <v>79</v>
       </c>
       <c r="M20" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="N20" t="s">
         <v>160</v>
       </c>
       <c r="O20" t="s">
+        <v>160</v>
+      </c>
+      <c r="P20" t="s">
         <v>159</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>159</v>
       </c>
     </row>
@@ -9668,6 +9710,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9922,27 +9984,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9959,23 +10020,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Improve supply chain logic to prioritize critical stores
Update route selection to give bonus points to routes serving sole-supplier stores when their stock levels are low.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d0bf8594-07fc-4ffd-b20d-54097ba9465c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/zFJnzwl
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE33CE05-3C88-4DE5-B461-3E15D34AC824}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6920E5-2E57-4FF2-AD4A-FBC5FEFF5769}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="178">
   <si>
     <t>Setting</t>
   </si>
@@ -1144,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1E5A6-CCD5-4160-8FE2-2B3BB5978653}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,10 +1173,10 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C3">
         <v>1000</v>
@@ -1195,10 +1195,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="C4">
-        <v>320</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,10 +1261,10 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="C10">
-        <v>800</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,26 +1272,26 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>433</v>
+        <v>800</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -1302,12 +1302,34 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="C14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
         <v>637</v>
       </c>
     </row>
@@ -9045,7 +9067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" activeCellId="2" sqref="A1:A20 E1:E20 I1:I20"/>
     </sheetView>
   </sheetViews>
@@ -9710,26 +9732,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9984,26 +9986,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10020,4 +10023,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update model inputs to reflect actual production rates
Update Model Inputs.xlsx and generated_model_inputs.xlsx with revised production rates for CL and GP at Railton and Gladstone.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: a163e8c7-2d11-4f14-a17e-12e51e014f0c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/zFJnzwl
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6920E5-2E57-4FF2-AD4A-FBC5FEFF5769}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5CC43D-ECE2-460C-AEE0-EDB430125E0C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="178">
   <si>
     <t>Setting</t>
   </si>
@@ -609,9 +609,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -715,7 +716,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -749,6 +750,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1146,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1E5A6-CCD5-4160-8FE2-2B3BB5978653}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
@@ -6219,7 +6221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9065,10 +9069,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" activeCellId="2" sqref="A1:A20 E1:E20 I1:I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9087,7 +9091,7 @@
     <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>145</v>
       </c>
@@ -9140,7 +9144,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -9172,7 +9176,7 @@
         <v>144</v>
       </c>
       <c r="K2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L2" t="s">
         <v>143</v>
@@ -9181,19 +9185,22 @@
         <v>143</v>
       </c>
       <c r="N2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="O2" t="s">
         <v>160</v>
       </c>
       <c r="P2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Q2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -9224,29 +9231,32 @@
       <c r="J3">
         <v>1.9</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="17">
+        <v>2</v>
+      </c>
+      <c r="L3">
         <v>2.1</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3.1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3.2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -9278,7 +9288,7 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="L4" t="s">
         <v>79</v>
@@ -9287,19 +9297,22 @@
         <v>79</v>
       </c>
       <c r="N4" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="O4" t="s">
         <v>160</v>
       </c>
       <c r="P4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Q4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -9319,7 +9332,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
         <v>53</v>
@@ -9331,7 +9344,7 @@
         <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
@@ -9340,19 +9353,22 @@
         <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O5" t="s">
         <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="Q5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -9372,7 +9388,7 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
         <v>107</v>
@@ -9384,7 +9400,7 @@
         <v>107</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
@@ -9393,35 +9409,50 @@
         <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O6" t="s">
         <v>26</v>
       </c>
       <c r="P6" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="Q6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>129</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -9444,7 +9475,7 @@
         <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
@@ -9456,25 +9487,28 @@
         <v>45</v>
       </c>
       <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
         <v>39</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>157</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>30</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -9494,7 +9528,7 @@
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
         <v>53</v>
@@ -9506,7 +9540,7 @@
         <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
         <v>19</v>
@@ -9515,19 +9549,22 @@
         <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
         <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="Q10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -9547,7 +9584,7 @@
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
         <v>54</v>
@@ -9559,7 +9596,7 @@
         <v>54</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="L11" t="s">
         <v>33</v>
@@ -9568,19 +9605,22 @@
         <v>33</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="O11" t="s">
         <v>46</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="Q11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -9588,7 +9628,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -9596,82 +9636,100 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
       <c r="E15" t="s">
         <v>72</v>
       </c>
-      <c r="J15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
       <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="I17" t="s">
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
         <v>157</v>
       </c>
       <c r="J17" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
       </c>
-      <c r="I18" t="s">
+      <c r="F18" t="s">
         <v>53</v>
       </c>
+      <c r="G18" t="s">
+        <v>53</v>
+      </c>
       <c r="J18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
       <c r="E19" t="s">
         <v>75</v>
       </c>
-      <c r="I19" t="s">
+      <c r="F19" t="s">
         <v>54</v>
       </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
       <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -9703,7 +9761,7 @@
         <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="L20" t="s">
         <v>79</v>
@@ -9712,15 +9770,18 @@
         <v>79</v>
       </c>
       <c r="N20" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="O20" t="s">
         <v>160</v>
       </c>
       <c r="P20" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q20" t="s">
         <v>159</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>159</v>
       </c>
     </row>
@@ -9732,6 +9793,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -9986,27 +10067,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10023,23 +10103,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Improve maintenance date input to support date ranges
Update `_parse_maintenance_days` function in `sim_run_data_factory.py` to parse maintenance dates from comma-separated strings that include ranges (e.g., "1-5,6,9-12").

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d61e4576-89b1-4aec-90cc-721b16d0531a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/NX9D2U8
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5CC43D-ECE2-460C-AEE0-EDB430125E0C}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BC1B21E-D8CD-4A05-95E6-41FEDDFE7782}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="178">
   <si>
     <t>Setting</t>
   </si>
@@ -609,12 +609,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,6 +645,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -716,7 +720,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -750,7 +754,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1146,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1E5A6-CCD5-4160-8FE2-2B3BB5978653}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,179 +1168,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="19" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="18">
         <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="18">
         <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="18">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="18">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="18">
         <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="18">
         <v>583</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="18">
         <v>1298</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="18">
         <v>674</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="18">
         <v>1700</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="18">
         <v>800</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="18">
         <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="18">
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="18">
         <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="18">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="18">
         <v>520</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="18">
         <v>637</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="18">
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -9071,8 +9101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9204,56 +9234,56 @@
       <c r="A3" t="s">
         <v>78</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="17">
+        <v>1.01</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1.03</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1.04</v>
+      </c>
+      <c r="F3" s="17">
+        <v>1.05</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1.06</v>
+      </c>
+      <c r="H3" s="17">
+        <v>1.07</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1.08</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K3" s="17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3">
-        <v>1.2</v>
-      </c>
-      <c r="D3">
-        <v>1.3</v>
-      </c>
-      <c r="E3">
-        <v>1.4</v>
-      </c>
-      <c r="F3">
-        <v>1.5</v>
-      </c>
-      <c r="G3">
-        <v>1.6</v>
-      </c>
-      <c r="H3">
-        <v>1.7</v>
-      </c>
-      <c r="I3">
-        <v>1.8</v>
-      </c>
-      <c r="J3">
-        <v>1.9</v>
-      </c>
-      <c r="K3" s="17">
-        <v>2</v>
-      </c>
       <c r="L3">
-        <v>2.1</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="M3">
-        <v>2.2000000000000002</v>
+        <v>2.02</v>
       </c>
       <c r="N3">
-        <v>2.2999999999999998</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="O3">
-        <v>3.1</v>
+        <v>3.01</v>
       </c>
       <c r="P3">
-        <v>3.2</v>
+        <v>3.02</v>
       </c>
       <c r="Q3">
-        <v>4.0999999999999996</v>
+        <v>4.01</v>
       </c>
       <c r="R3">
-        <v>4.2</v>
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -9793,26 +9823,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -10067,26 +10077,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10103,4 +10114,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update shipping routes to ensure all ports receive supplies
Modify routing logic to balance deliveries between multiple shipping destinations.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 4d760a11-1de6-4def-a339-16243ba8ab29
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/NX9D2U8
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BC1B21E-D8CD-4A05-95E6-41FEDDFE7782}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2ECC71C-8F63-4BD2-BB56-D9D89BFA326B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="173">
   <si>
     <t>Setting</t>
   </si>
@@ -251,33 +251,6 @@
     <t>Consumption %</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 36, 37, 56, 57, 58, 64, 87, 91, 92, 93, 99, 100, 106, 107, 113, 114, 119, 120, 121, 127, 128, 129, 140, 141, 142, 147, 148, 154, 155, 156, 162, 163, 169, 170, 176, 177, 182, 183, 184, 189, 190, 191, 196, 197, 198, 203, 204, 205, 206, 223, 224, 225, 226, 231, 232, 233, 238, 239, 240, 245, 246, 247, 248, 252, 253, 254, 260, 261, 262, 263, 268, 269, 275, 276, 277, 282, 283, 289, 295, 296, 301, 302, 337, 345, 351, 352, 359, 360, 361, 362, 363, 364</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 66, 67, 91, 92, 93, 98, 99, 128, 129, 323, 324, 351, 352, 353, 356, 357, 358, 359, 360, 361, 362, 363, 364</t>
-  </si>
-  <si>
-    <t>9, 27, 28, 29, 30, 31, 37, 38, 98, 99, 100, 104, 105, 112, 113, 114, 115, 116, 117, 130, 131, 135, 136, 137, 138, 162, 163, 185, 186, 201, 202, 203, 227, 228, 229, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 269, 286, 287, 288, 289, 297, 298, 330, 331, 332, 351, 352, 353, 357, 358, 359, 360, 361</t>
-  </si>
-  <si>
-    <t>9, 10, 11, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 36, 39, 40, 71, 72, 73, 74, 85, 86, 98, 99, 104, 105, 110, 111, 112, 113, 114, 115, 116, 117, 118, 128, 129, 130, 162, 163, 203, 204, 214, 215, 216, 227, 228, 229, 247, 248, 249, 269, 270, 279, 280, 286, 287, 288, 317, 330, 331, 332, 352, 353, 358, 359, 360</t>
-  </si>
-  <si>
-    <t>146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 14, 15, 16, 17, 18, 19, 20, 27, 28, 35, 36, 42, 43, 48, 49, 50, 56, 57, 70, 77, 78, 79, 91, 92, 93, 94, 95, 96, 97, 119, 120, 133, 134, 140, 141, 142, 161, 162, 163, 164, 182, 183, 189, 190, 196, 197, 203, 204, 210, 211, 216, 217, 218, 224, 225, 231, 232, 238, 239, 240, 252, 253, 256, 260, 261, 264, 273, 280, 281, 282, 287, 288, 294, 295, 301, 302, 322, 323, 336, 337, 350, 351, 360, 361, 362, 363, 364</t>
-  </si>
-  <si>
-    <t>2, 3, 4, 5, 6, 7, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 245, 294, 295</t>
-  </si>
-  <si>
-    <t>2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 159, 167, 168, 197, 198, 203, 204, 224, 245, 246, 294, 295</t>
-  </si>
-  <si>
-    <t>95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120</t>
-  </si>
-  <si>
     <t>Silo Max Capacity</t>
   </si>
   <si>
@@ -386,9 +359,6 @@
     <t>FA_SUPPLY</t>
   </si>
   <si>
-    <t>10,20,50,100</t>
-  </si>
-  <si>
     <t>Unconstrained supply for this model, can load 350t/h</t>
   </si>
   <si>
@@ -603,6 +573,21 @@
   </si>
   <si>
     <t>Route 16</t>
+  </si>
+  <si>
+    <t>250-274</t>
+  </si>
+  <si>
+    <t>1-10,53,96,139,182,225,268,311</t>
+  </si>
+  <si>
+    <t>12-21,64,107,150,193,236,279,322</t>
+  </si>
+  <si>
+    <t>1-5,53,96-100,148,191,234,277,320,363</t>
+  </si>
+  <si>
+    <t>95-120</t>
   </si>
 </sst>
 </file>
@@ -755,10 +740,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1156,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1E5A6-CCD5-4160-8FE2-2B3BB5978653}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
@@ -1168,200 +1153,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>142</v>
+      <c r="A1" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2">
         <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="18">
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3">
         <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="18">
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6">
         <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7">
         <v>583</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8">
         <v>1298</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9">
         <v>674</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="18">
+      <c r="B10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10">
         <v>1700</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11">
         <v>800</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12">
         <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13">
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="A14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14">
         <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15">
         <v>640</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" s="18">
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16">
         <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17">
         <v>637</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18" s="18" t="s">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18">
         <v>940</v>
       </c>
     </row>
@@ -1549,7 +1534,7 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="S3" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2507,7 +2492,7 @@
         <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2562,7 +2547,7 @@
         <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2617,7 +2602,7 @@
         <v>41</v>
       </c>
       <c r="J23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2672,7 +2657,7 @@
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2709,7 +2694,7 @@
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -2764,7 +2749,7 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2834,7 +2819,7 @@
         <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="J27" t="s">
         <v>33</v>
@@ -2916,7 +2901,7 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
         <v>33</v>
@@ -2934,7 +2919,7 @@
         <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="J29" t="s">
         <v>29</v>
@@ -2971,7 +2956,7 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
@@ -3026,7 +3011,7 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
         <v>29</v>
@@ -3044,7 +3029,7 @@
         <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J31" t="s">
         <v>33</v>
@@ -3081,7 +3066,7 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -3136,7 +3121,7 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
         <v>26</v>
@@ -3154,7 +3139,7 @@
         <v>28</v>
       </c>
       <c r="I33" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="J33" t="s">
         <v>29</v>
@@ -3191,7 +3176,7 @@
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
         <v>29</v>
@@ -3243,7 +3228,7 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
         <v>29</v>
@@ -4319,7 +4304,7 @@
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
         <v>33</v>
@@ -4337,7 +4322,7 @@
         <v>35</v>
       </c>
       <c r="I56" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J56" t="s">
         <v>36</v>
@@ -4371,7 +4356,7 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D57" t="s">
         <v>36</v>
@@ -4867,7 +4852,7 @@
         <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F68" t="s">
         <v>23</v>
@@ -4882,7 +4867,7 @@
         <v>20</v>
       </c>
       <c r="J68" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="K68">
         <v>1</v>
@@ -4903,7 +4888,7 @@
         <v>20</v>
       </c>
       <c r="D69" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E69" t="s">
         <v>53</v>
@@ -5023,7 +5008,7 @@
         <v>25</v>
       </c>
       <c r="I72" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J72" t="s">
         <v>54</v>
@@ -5110,7 +5095,7 @@
         <v>53</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D75" t="s">
         <v>54</v>
@@ -5128,7 +5113,7 @@
         <v>35</v>
       </c>
       <c r="I75" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J75" t="s">
         <v>36</v>
@@ -5197,7 +5182,7 @@
         <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D78" t="s">
         <v>36</v>
@@ -5220,28 +5205,28 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E79" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F79" t="s">
         <v>25</v>
       </c>
       <c r="G79" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H79" t="s">
         <v>28</v>
       </c>
       <c r="I79" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="J79" t="s">
         <v>29</v>
@@ -5255,22 +5240,22 @@
         <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D80" t="s">
         <v>29</v>
       </c>
       <c r="E80" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F80" t="s">
         <v>28</v>
       </c>
       <c r="G80" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H80" t="s">
         <v>25</v>
@@ -5279,7 +5264,7 @@
         <v>38</v>
       </c>
       <c r="J80" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K80">
         <v>3</v>
@@ -5290,22 +5275,22 @@
         <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D81" t="s">
         <v>29</v>
       </c>
       <c r="E81" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F81" t="s">
         <v>28</v>
       </c>
       <c r="G81" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H81" t="s">
         <v>25</v>
@@ -5314,7 +5299,7 @@
         <v>30</v>
       </c>
       <c r="J81" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K81">
         <v>3</v>
@@ -5325,22 +5310,22 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C82" t="s">
         <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E82" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F82" t="s">
         <v>25</v>
       </c>
       <c r="G82" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H82" t="s">
         <v>23</v>
@@ -5360,7 +5345,7 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C83" t="s">
         <v>38</v>
@@ -5369,13 +5354,13 @@
         <v>49</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F83" t="s">
         <v>23</v>
       </c>
       <c r="G83" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H83" t="s">
         <v>25</v>
@@ -5384,7 +5369,7 @@
         <v>38</v>
       </c>
       <c r="J83" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K83">
         <v>1</v>
@@ -5395,22 +5380,22 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C84" t="s">
         <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E84" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F84" t="s">
         <v>25</v>
       </c>
       <c r="G84" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H84" t="s">
         <v>35</v>
@@ -5430,7 +5415,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C85" t="s">
         <v>38</v>
@@ -5439,13 +5424,13 @@
         <v>36</v>
       </c>
       <c r="E85" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F85" t="s">
         <v>35</v>
       </c>
       <c r="G85" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K85">
         <v>4</v>
@@ -5456,22 +5441,22 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C86" t="s">
         <v>38</v>
       </c>
       <c r="D86" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E86" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F86" t="s">
         <v>25</v>
       </c>
       <c r="G86" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H86" t="s">
         <v>28</v>
@@ -5491,22 +5476,22 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C87" t="s">
         <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E87" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F87" t="s">
         <v>25</v>
       </c>
       <c r="G87" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H87" t="s">
         <v>28</v>
@@ -5526,7 +5511,7 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C88" t="s">
         <v>38</v>
@@ -5535,13 +5520,13 @@
         <v>29</v>
       </c>
       <c r="E88" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F88" t="s">
         <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H88" t="s">
         <v>25</v>
@@ -5550,7 +5535,7 @@
         <v>45</v>
       </c>
       <c r="J88" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K88">
         <v>3</v>
@@ -5561,7 +5546,7 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C89" t="s">
         <v>38</v>
@@ -5570,13 +5555,13 @@
         <v>34</v>
       </c>
       <c r="E89" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F89" t="s">
         <v>28</v>
       </c>
       <c r="G89" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H89" t="s">
         <v>25</v>
@@ -5585,7 +5570,7 @@
         <v>52</v>
       </c>
       <c r="J89" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K89">
         <v>3</v>
@@ -5596,7 +5581,7 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C90" t="s">
         <v>38</v>
@@ -5605,22 +5590,22 @@
         <v>34</v>
       </c>
       <c r="E90" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F90" t="s">
         <v>28</v>
       </c>
       <c r="G90" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H90" t="s">
         <v>25</v>
       </c>
       <c r="I90" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J90" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K90">
         <v>3</v>
@@ -5631,7 +5616,7 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C91" t="s">
         <v>38</v>
@@ -5640,13 +5625,13 @@
         <v>34</v>
       </c>
       <c r="E91" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F91" t="s">
         <v>28</v>
       </c>
       <c r="G91" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H91" t="s">
         <v>25</v>
@@ -5655,7 +5640,7 @@
         <v>39</v>
       </c>
       <c r="J91" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K91">
         <v>3</v>
@@ -5666,22 +5651,22 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C92" t="s">
         <v>30</v>
       </c>
       <c r="D92" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E92" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F92" t="s">
         <v>25</v>
       </c>
       <c r="G92" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H92" t="s">
         <v>23</v>
@@ -5701,22 +5686,22 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C93" t="s">
         <v>30</v>
       </c>
       <c r="D93" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E93" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F93" t="s">
         <v>25</v>
       </c>
       <c r="G93" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H93" t="s">
         <v>23</v>
@@ -5736,7 +5721,7 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C94" t="s">
         <v>30</v>
@@ -5745,13 +5730,13 @@
         <v>47</v>
       </c>
       <c r="E94" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F94" t="s">
         <v>23</v>
       </c>
       <c r="G94" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H94" t="s">
         <v>25</v>
@@ -5760,7 +5745,7 @@
         <v>30</v>
       </c>
       <c r="J94" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5771,7 +5756,7 @@
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C95" t="s">
         <v>30</v>
@@ -5780,13 +5765,13 @@
         <v>48</v>
       </c>
       <c r="E95" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F95" t="s">
         <v>23</v>
       </c>
       <c r="G95" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H95" t="s">
         <v>25</v>
@@ -5795,7 +5780,7 @@
         <v>30</v>
       </c>
       <c r="J95" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5806,22 +5791,22 @@
         <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C96" t="s">
         <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E96" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F96" t="s">
         <v>25</v>
       </c>
       <c r="G96" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H96" t="s">
         <v>28</v>
@@ -5841,22 +5826,22 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C97" t="s">
         <v>30</v>
       </c>
       <c r="D97" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E97" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F97" t="s">
         <v>25</v>
       </c>
       <c r="G97" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H97" t="s">
         <v>35</v>
@@ -5876,7 +5861,7 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
@@ -5885,22 +5870,22 @@
         <v>34</v>
       </c>
       <c r="E98" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F98" t="s">
         <v>28</v>
       </c>
       <c r="G98" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H98" t="s">
         <v>25</v>
       </c>
       <c r="I98" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J98" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K98">
         <v>3</v>
@@ -5911,7 +5896,7 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C99" t="s">
         <v>30</v>
@@ -5920,13 +5905,13 @@
         <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F99" t="s">
         <v>35</v>
       </c>
       <c r="G99" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K99">
         <v>4</v>
@@ -5937,28 +5922,28 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C100" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D100" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E100" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F100" t="s">
         <v>25</v>
       </c>
       <c r="G100" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H100" t="s">
         <v>35</v>
       </c>
       <c r="I100" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J100" t="s">
         <v>36</v>
@@ -5972,22 +5957,22 @@
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C101" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D101" t="s">
         <v>36</v>
       </c>
       <c r="E101" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F101" t="s">
         <v>35</v>
       </c>
       <c r="G101" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K101">
         <v>4</v>
@@ -5998,22 +5983,22 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C102" t="s">
         <v>45</v>
       </c>
       <c r="D102" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E102" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F102" t="s">
         <v>25</v>
       </c>
       <c r="G102" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H102" t="s">
         <v>35</v>
@@ -6033,7 +6018,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C103" t="s">
         <v>45</v>
@@ -6042,13 +6027,13 @@
         <v>36</v>
       </c>
       <c r="E103" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F103" t="s">
         <v>35</v>
       </c>
       <c r="G103" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K103">
         <v>4</v>
@@ -6059,22 +6044,22 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C104" t="s">
         <v>52</v>
       </c>
       <c r="D104" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E104" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F104" t="s">
         <v>25</v>
       </c>
       <c r="G104" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H104" t="s">
         <v>35</v>
@@ -6094,7 +6079,7 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C105" t="s">
         <v>52</v>
@@ -6103,13 +6088,13 @@
         <v>36</v>
       </c>
       <c r="E105" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F105" t="s">
         <v>35</v>
       </c>
       <c r="G105" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K105">
         <v>4</v>
@@ -6120,28 +6105,28 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C106" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D106" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E106" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F106" t="s">
         <v>25</v>
       </c>
       <c r="G106" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H106" t="s">
         <v>35</v>
       </c>
       <c r="I106" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J106" t="s">
         <v>36</v>
@@ -6155,22 +6140,22 @@
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C107" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D107" t="s">
         <v>36</v>
       </c>
       <c r="E107" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F107" t="s">
         <v>35</v>
       </c>
       <c r="G107" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -6181,22 +6166,22 @@
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C108" t="s">
         <v>39</v>
       </c>
       <c r="D108" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E108" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F108" t="s">
         <v>25</v>
       </c>
       <c r="G108" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H108" t="s">
         <v>35</v>
@@ -6216,7 +6201,7 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C109" t="s">
         <v>39</v>
@@ -6225,13 +6210,13 @@
         <v>36</v>
       </c>
       <c r="E109" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F109" t="s">
         <v>35</v>
       </c>
       <c r="G109" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K109">
         <v>4</v>
@@ -6251,8 +6236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6315,8 +6300,8 @@
       <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>60</v>
+      <c r="G2" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="H2" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6333,10 +6318,10 @@
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -6344,8 +6329,8 @@
       <c r="F3">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>60</v>
+      <c r="G3" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="H3" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6373,8 +6358,8 @@
       <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>61</v>
+      <c r="G4" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="H4" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6391,10 +6376,10 @@
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -6402,8 +6387,8 @@
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>61</v>
+      <c r="G5" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="H5" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6431,11 +6416,9 @@
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
+      <c r="G6" s="19"/>
       <c r="H6" s="10">
-        <v>0.1646</v>
+        <v>0.15</v>
       </c>
       <c r="I6" s="10">
         <v>0.88</v>
@@ -6460,11 +6443,9 @@
       <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
+      <c r="G7" s="19"/>
       <c r="H7" s="10">
-        <v>0.13189999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="I7" s="10">
         <v>0.88</v>
@@ -6475,7 +6456,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
@@ -6486,11 +6467,9 @@
       <c r="F8">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
-        <v>105</v>
-      </c>
+      <c r="G8" s="19"/>
       <c r="H8" s="10">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="I8" s="10">
         <v>1</v>
@@ -6512,8 +6491,8 @@
       <c r="F9">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
-        <v>64</v>
+      <c r="G9" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="H9" s="10">
         <v>7.4499999999999997E-2</v>
@@ -6541,8 +6520,8 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" t="s">
-        <v>65</v>
+      <c r="G10" s="19" t="s">
+        <v>171</v>
       </c>
       <c r="H10" s="10">
         <v>0.05</v>
@@ -6559,10 +6538,10 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>180</v>
@@ -6570,8 +6549,8 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
-        <v>65</v>
+      <c r="G11" s="19" t="s">
+        <v>171</v>
       </c>
       <c r="H11" s="10">
         <v>0.05</v>
@@ -6599,11 +6578,9 @@
       <c r="F12">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
+      <c r="G12" s="19"/>
       <c r="H12" s="10">
-        <v>5.2999999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="I12" s="10">
         <v>0.88</v>
@@ -6628,11 +6605,9 @@
       <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" t="s">
-        <v>67</v>
-      </c>
+      <c r="G13" s="19"/>
       <c r="H13" s="10">
-        <v>0.1101</v>
+        <v>0.15</v>
       </c>
       <c r="I13" s="10">
         <v>0.88</v>
@@ -6654,8 +6629,8 @@
       <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
-        <v>68</v>
+      <c r="G14" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="H14" s="10">
         <v>2.98E-2</v>
@@ -6698,26 +6673,26 @@
         <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I1" s="3"/>
       <c r="K1" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
@@ -6749,10 +6724,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6785,7 +6760,7 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -6818,7 +6793,7 @@
         <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6851,7 +6826,7 @@
         <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -6859,10 +6834,10 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3">
         <v>50000</v>
@@ -6884,7 +6859,7 @@
         <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -6892,10 +6867,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3">
         <v>10000</v>
@@ -6917,18 +6892,18 @@
         <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3">
         <v>3000</v>
@@ -6947,10 +6922,10 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -6980,10 +6955,10 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -6991,10 +6966,10 @@
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3">
         <v>3000</v>
@@ -7013,15 +6988,15 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -7049,7 +7024,7 @@
         <v>27</v>
       </c>
       <c r="K11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -7082,7 +7057,7 @@
         <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -7090,7 +7065,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>53</v>
@@ -7115,7 +7090,7 @@
         <v>27</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -7148,12 +7123,12 @@
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -7181,18 +7156,18 @@
         <v>27</v>
       </c>
       <c r="K15" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3">
         <v>999999</v>
@@ -7214,7 +7189,7 @@
         <v>27</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -7244,10 +7219,10 @@
       </c>
       <c r="I17" s="3"/>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7307,7 +7282,7 @@
         <v>27</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7315,10 +7290,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D20" s="3">
         <v>25000</v>
@@ -7340,7 +7315,7 @@
         <v>27</v>
       </c>
       <c r="K20" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7373,7 +7348,7 @@
         <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -7381,10 +7356,10 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3">
         <v>3000</v>
@@ -7406,12 +7381,12 @@
         <v>27</v>
       </c>
       <c r="K22" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -7439,12 +7414,12 @@
         <v>27</v>
       </c>
       <c r="K23" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -7472,7 +7447,7 @@
         <v>27</v>
       </c>
       <c r="K24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -7505,7 +7480,7 @@
         <v>27</v>
       </c>
       <c r="K25" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -7538,7 +7513,7 @@
         <v>27</v>
       </c>
       <c r="K26" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -7546,10 +7521,10 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D27" s="9">
         <v>50000</v>
@@ -7601,7 +7576,7 @@
         <v>27</v>
       </c>
       <c r="K28" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7609,10 +7584,10 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D29" s="3">
         <v>20000</v>
@@ -7634,7 +7609,7 @@
         <v>27</v>
       </c>
       <c r="K29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7667,7 +7642,7 @@
         <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7675,7 +7650,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -7700,7 +7675,7 @@
         <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7708,7 +7683,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -7733,18 +7708,18 @@
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D33" s="3">
         <v>3000</v>
@@ -7763,10 +7738,10 @@
       </c>
       <c r="I33" s="3"/>
       <c r="J33" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K33" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -7799,7 +7774,7 @@
         <v>27</v>
       </c>
       <c r="K34" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -7829,10 +7804,10 @@
       </c>
       <c r="I35" s="3"/>
       <c r="J35" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K35" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -7866,13 +7841,13 @@
         <v>10</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7916,10 +7891,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
@@ -7931,13 +7906,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
@@ -7970,10 +7945,10 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
@@ -8060,10 +8035,10 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
@@ -8096,10 +8071,10 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
@@ -8111,7 +8086,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
@@ -8129,7 +8104,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -8186,10 +8161,10 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D19" s="8">
         <f t="shared" si="0"/>
@@ -8207,7 +8182,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" si="0"/>
@@ -8219,13 +8194,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D21" s="8">
         <f t="shared" si="0"/>
@@ -8306,43 +8281,43 @@
         <v>7</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8532,10 +8507,10 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
         <v>33</v>
@@ -8567,22 +8542,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G7">
         <v>30</v>
@@ -8611,22 +8586,22 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -8655,10 +8630,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -8667,10 +8642,10 @@
         <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -8699,10 +8674,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -8711,10 +8686,10 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G10">
         <v>280</v>
@@ -8763,30 +8738,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>120</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8806,7 +8781,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -8823,10 +8798,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -8843,10 +8818,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -8866,7 +8841,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -8881,7 +8856,7 @@
         <v>5000</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -8910,16 +8885,16 @@
         <v>8</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8941,7 +8916,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -8975,7 +8950,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8992,7 +8967,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9043,7 +9018,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -9123,116 +9098,116 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>164</v>
-      </c>
       <c r="O1" s="12" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="J2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="M2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="O2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="P2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="Q2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="R2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B3" s="17">
         <v>1.01</v>
@@ -9288,7 +9263,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -9321,30 +9296,30 @@
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="N4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="P4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="Q4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="R4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -9392,18 +9367,18 @@
         <v>24</v>
       </c>
       <c r="Q5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="R5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -9421,16 +9396,16 @@
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
@@ -9448,15 +9423,15 @@
         <v>26</v>
       </c>
       <c r="Q6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="R6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -9470,21 +9445,21 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -9523,7 +9498,7 @@
         <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="O9" t="s">
         <v>30</v>
@@ -9540,7 +9515,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -9588,18 +9563,18 @@
         <v>24</v>
       </c>
       <c r="Q10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="R10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -9644,15 +9619,15 @@
         <v>46</v>
       </c>
       <c r="Q11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
         <v>53</v>
@@ -9660,7 +9635,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
@@ -9668,21 +9643,21 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
         <v>19</v>
@@ -9690,10 +9665,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
         <v>33</v>
@@ -9701,7 +9676,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -9710,10 +9685,10 @@
         <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J17" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K17" t="s">
         <v>45</v>
@@ -9721,10 +9696,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>53</v>
@@ -9741,10 +9716,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>54</v>
@@ -9761,7 +9736,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -9794,25 +9769,25 @@
         <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="M20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="N20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="O20" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="P20" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="Q20" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="R20" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -9823,6 +9798,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -10077,27 +10072,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10114,23 +10108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
-    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update terminology for ship capacity and payload from hulls to holds
Renames `#Hulls` to `#Holds` and `Payload per Hull` to `Payload per Hold` across Python scripts and constants to match updated data inputs.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 826e8556-5564-485a-a91b-54f571e225fa
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/0xcUuyg
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2ECC71C-8F63-4BD2-BB56-D9D89BFA326B}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E881DB0-A43C-4726-96F2-7C33DDDB17D9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="33870" yWindow="2730" windowWidth="19035" windowHeight="14550" activeTab="6" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="174">
   <si>
     <t>Setting</t>
   </si>
@@ -545,12 +545,6 @@
     <t>Demand Store</t>
   </si>
   <si>
-    <t>#Hulls</t>
-  </si>
-  <si>
-    <t>Payload per Hull</t>
-  </si>
-  <si>
     <t>* Only Applies to SHIPPING</t>
   </si>
   <si>
@@ -588,6 +582,15 @@
   </si>
   <si>
     <t>95-120</t>
+  </si>
+  <si>
+    <t>Route 17</t>
+  </si>
+  <si>
+    <t>#Holds</t>
+  </si>
+  <si>
+    <t>Payload per Hold</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6236,8 +6239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6301,7 +6304,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6330,7 +6333,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H3" s="10">
         <v>3.3000000000000002E-2</v>
@@ -6359,7 +6362,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H4" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6388,7 +6391,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H5" s="10">
         <v>3.7999999999999999E-2</v>
@@ -6492,7 +6495,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H9" s="10">
         <v>7.4499999999999997E-2</v>
@@ -6521,7 +6524,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H10" s="10">
         <v>0.05</v>
@@ -6550,7 +6553,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H11" s="10">
         <v>0.05</v>
@@ -6630,7 +6633,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H14" s="10">
         <v>2.98E-2</v>
@@ -6649,7 +6652,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,7 +6695,7 @@
         <v>89</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
@@ -7642,7 +7645,7 @@
         <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7675,7 +7678,7 @@
         <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7708,7 +7711,7 @@
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -8725,7 +8728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D7C592-8DF8-40A4-9452-62826144206E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8750,10 +8755,10 @@
         <v>112</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -8856,7 +8861,7 @@
         <v>5000</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -9076,8 +9081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9085,12 +9090,7 @@
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
@@ -9140,13 +9140,16 @@
         <v>154</v>
       </c>
       <c r="O1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>167</v>
+      <c r="R1" s="12" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -9798,15 +9801,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
@@ -9817,7 +9811,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -10072,15 +10066,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10091,7 +10086,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10108,4 +10103,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update timestamps to use local time across the project
Adjusts timestamp generation in `supply_chain_viz.py` and `sim_run_report_plot.py` to use local time instead of UTC, ensuring consistent date and time representation in logs and reports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 1feb53c2-f013-4ec4-a2ee-43d0a81c1bfc
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/ZOII0yD
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zephien\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E881DB0-A43C-4726-96F2-7C33DDDB17D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59D5A5-1226-491F-998D-D827940F77E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33870" yWindow="2730" windowWidth="19035" windowHeight="14550" activeTab="6" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="175">
   <si>
     <t>Setting</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>Payload per Hold</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -8729,7 +8732,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8779,6 +8782,9 @@
       </c>
       <c r="F2">
         <v>5000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -9812,6 +9818,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -10066,15 +10081,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
   <ds:schemaRefs>
@@ -10087,6 +10093,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10103,12 +10117,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed output store bug that affected Railton, improved the log for stores, still working on Shipping logic.
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_48038AE7859AA64F7EBA904D5B06B482C9AF219E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B1392B-53A4-4B22-8A38-1481FD7CEAA7}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_48038AE7859AA64F7EBA904D5B06B482C9AF219E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB51D936-76CB-4A49-9B93-C7B566286465}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30090" yWindow="1230" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -6034,7 +6034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6356,7 +6358,7 @@
         <v>25</v>
       </c>
       <c r="E12">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -6382,7 +6384,7 @@
         <v>25</v>
       </c>
       <c r="E13">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="F13">
         <v>10</v>
@@ -8419,7 +8421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
@@ -9827,15 +9829,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
@@ -9846,14 +9839,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FDDD8CB-64BD-4072-8750-C67288F1F719}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FDDD8CB-64BD-4072-8750-C67288F1F719}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F05B2ABF-7AF5-4AFA-A3B1-938588AF40D2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC6AC786-0F8D-4ADC-A468-2F55B748020E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
+    <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC6AC786-0F8D-4ADC-A468-2F55B748020E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F05B2ABF-7AF5-4AFA-A3B1-938588AF40D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Shipping Logic still in progress - Slow Grind - 23 Dec 2025
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F167C78B-2497-4CBA-B117-F509096C3FEF}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D3C9B6-BB61-4D63-9908-ACE6A2E28377}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Deliver!$A$1:$E$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Store!$A$1:$H$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network!$B$1:$K$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Store!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="180">
   <si>
     <t>Setting</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>GBFS_SUPPLY</t>
+  </si>
+  <si>
+    <t>GP_IMP_SILO</t>
+  </si>
+  <si>
+    <t>Existing 7 Silos</t>
+  </si>
+  <si>
+    <t>CONVEYOR</t>
   </si>
 </sst>
 </file>
@@ -1380,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T110"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M89" sqref="M89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2094,7 @@
         <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="K13">
         <v>3</v>
@@ -2099,11 +2108,11 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" si="1"/>
-        <v>Port KemblaStoreGP_STOREGP</v>
+        <v>Port KemblaStoreGP_IMP_SILOGP</v>
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="3"/>
@@ -3226,19 +3235,19 @@
         <v>3</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ref="M34:M67" si="4">C34&amp;F34&amp;D34&amp;E34</f>
+        <f t="shared" ref="M34:M45" si="4">C34&amp;F34&amp;D34&amp;E34</f>
         <v>Import_CLMoveSHIPCL</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" ref="N34:N64" si="5">I34&amp;H34&amp;J34&amp;G34</f>
+        <f t="shared" ref="N34:N45" si="5">I34&amp;H34&amp;J34&amp;G34</f>
         <v>Port KemblaStoreCL_STORE_ICL</v>
       </c>
       <c r="O34">
-        <f t="shared" ref="O34:O65" si="6">COUNTIFS(M:M,N34)</f>
+        <f t="shared" ref="O34:O64" si="6">COUNTIFS(M:M,N34)</f>
         <v>1</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" ref="P34:P68" si="7">C34&amp;F34&amp;G34</f>
+        <f t="shared" ref="P34:P45" si="7">C34&amp;F34&amp;G34</f>
         <v>Import_CLMoveCL</v>
       </c>
     </row>
@@ -3772,8 +3781,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" cm="1">
-        <f t="array" ref="A45">IF(ISNA(_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44)),IF(COUNTIFS($P$2:P45,P45)=1,IF(COUNTIFS($C$2:C44,C45)=0,1,_xlfn.MAXIFS($A$2:A44,$C$2:C44,C45)+1),A44),_xlfn.XLOOKUP(P45,$P$2:P44,$A$2:A44))</f>
+      <c r="A45" s="1">
         <v>2</v>
       </c>
       <c r="B45" t="s">
@@ -3827,9 +3835,8 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" cm="1">
-        <f t="array" ref="A46">IF(ISNA(_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45)),IF(COUNTIFS($P$2:P46,P46)=1,IF(COUNTIFS($C$2:C45,C46)=0,1,_xlfn.MAXIFS($A$2:A45,$C$2:C45,C46)+1),A45),_xlfn.XLOOKUP(P46,$P$2:P45,$A$2:A45))</f>
-        <v>3</v>
+      <c r="A46" s="1">
+        <v>1</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -3838,7 +3845,7 @@
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
@@ -3850,23 +3857,23 @@
         <v>19</v>
       </c>
       <c r="H46" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I46" t="s">
         <v>38</v>
       </c>
       <c r="J46" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="K46">
         <v>2</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M46:M67" si="8">C48&amp;F48&amp;D48&amp;E48</f>
         <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="N46:N64" si="9">I48&amp;H48&amp;J48&amp;G48</f>
         <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="O46">
@@ -3874,14 +3881,13 @@
         <v>3</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="P46:P68" si="10">C48&amp;F48&amp;G48</f>
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" cm="1">
-        <f t="array" ref="A47">IF(ISNA(_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46)),IF(COUNTIFS($P$2:P47,P47)=1,IF(COUNTIFS($C$2:C46,C47)=0,1,_xlfn.MAXIFS($A$2:A46,$C$2:C46,C47)+1),A46),_xlfn.XLOOKUP(P47,$P$2:P46,$A$2:A46))</f>
-        <v>3</v>
+      <c r="A47" s="1">
+        <v>2</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -3890,35 +3896,35 @@
         <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>179</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" t="s">
         <v>25</v>
-      </c>
-      <c r="G47" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" t="s">
-        <v>35</v>
       </c>
       <c r="I47" t="s">
         <v>38</v>
       </c>
       <c r="J47" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Port KemblaStoreGP_STOREGP</v>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>Port KemblaDeliverTRUCKGP</v>
       </c>
       <c r="O47">
@@ -3926,14 +3932,13 @@
         <v>1</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Port KemblaStoreGP</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" cm="1">
-        <f t="array" ref="A48">IF(ISNA(_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47)),IF(COUNTIFS($P$2:P48,P48)=1,IF(COUNTIFS($C$2:C47,C48)=0,1,_xlfn.MAXIFS($A$2:A47,$C$2:C47,C48)+1),A47),_xlfn.XLOOKUP(P48,$P$2:P47,$A$2:A47))</f>
-        <v>4</v>
+      <c r="A48" s="1">
+        <v>3</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -3942,35 +3947,35 @@
         <v>38</v>
       </c>
       <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J48" t="s">
         <v>34</v>
       </c>
-      <c r="E48" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" t="s">
-        <v>19</v>
-      </c>
-      <c r="H48" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" t="s">
-        <v>50</v>
-      </c>
-      <c r="J48" t="s">
-        <v>33</v>
-      </c>
       <c r="K48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>AlburyStoreGP_STOREGP</v>
       </c>
       <c r="O48">
@@ -3978,13 +3983,12 @@
         <v>1</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" cm="1">
-        <f t="array" ref="A49">IF(ISNA(_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48)),IF(COUNTIFS($P$2:P49,P49)=1,IF(COUNTIFS($C$2:C48,C49)=0,1,_xlfn.MAXIFS($A$2:A48,$C$2:C48,C49)+1),A48),_xlfn.XLOOKUP(P49,$P$2:P48,$A$2:A48))</f>
+      <c r="A49" s="1">
         <v>4</v>
       </c>
       <c r="B49" t="s">
@@ -3994,35 +3998,35 @@
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G49" t="s">
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I49" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="J49" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>WaggaStoreGP_STOREGP</v>
       </c>
       <c r="O49">
@@ -4030,14 +4034,13 @@
         <v>1</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" cm="1">
-        <f t="array" ref="A50">IF(ISNA(_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49)),IF(COUNTIFS($P$2:P50,P50)=1,IF(COUNTIFS($C$2:C49,C50)=0,1,_xlfn.MAXIFS($A$2:A49,$C$2:C49,C50)+1),A49),_xlfn.XLOOKUP(P50,$P$2:P49,$A$2:A49))</f>
-        <v>4</v>
+      <c r="A50" s="1">
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
@@ -4061,7 +4064,7 @@
         <v>25</v>
       </c>
       <c r="I50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J50" t="s">
         <v>33</v>
@@ -4070,11 +4073,11 @@
         <v>3</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Port KemblaMoveTRAINGP</v>
       </c>
       <c r="N50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="O50">
@@ -4082,13 +4085,13 @@
         <v>1</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Port KemblaMoveGP</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -4097,26 +4100,35 @@
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E51" t="s">
         <v>19</v>
       </c>
       <c r="F51" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G51" t="s">
         <v>19</v>
       </c>
+      <c r="H51" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" t="s">
+        <v>51</v>
+      </c>
+      <c r="J51" t="s">
+        <v>33</v>
+      </c>
       <c r="K51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Port KemblaDeliverTRUCKGP</v>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O51">
@@ -4124,51 +4136,50 @@
         <v>0</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Port KemblaDeliverGP</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" cm="1">
-        <f t="array" ref="A52">IF(ISNA(_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51)),IF(COUNTIFS($P$2:P52,P52)=1,IF(COUNTIFS($C$2:C51,C52)=0,1,_xlfn.MAXIFS($A$2:A51,$C$2:C51,C52)+1),A51),_xlfn.XLOOKUP(P52,$P$2:P51,$A$2:A51))</f>
-        <v>1</v>
+      <c r="A52" s="1">
+        <v>5</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" t="s">
+        <v>52</v>
+      </c>
+      <c r="J52" t="s">
         <v>33</v>
       </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" t="s">
-        <v>19</v>
-      </c>
-      <c r="H52" t="s">
-        <v>35</v>
-      </c>
-      <c r="I52" t="s">
-        <v>39</v>
-      </c>
-      <c r="J52" t="s">
-        <v>36</v>
-      </c>
       <c r="K52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>NewcastleStoreGP_STOREGP</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>NewcastleDeliverTRUCKGP</v>
       </c>
       <c r="O52">
@@ -4176,20 +4187,19 @@
         <v>1</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>NewcastleStoreGP</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" cm="1">
-        <f t="array" ref="A53">IF(ISNA(_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52)),IF(COUNTIFS($P$2:P53,P53)=1,IF(COUNTIFS($C$2:C52,C53)=0,1,_xlfn.MAXIFS($A$2:A52,$C$2:C52,C53)+1),A52),_xlfn.XLOOKUP(P53,$P$2:P52,$A$2:A52))</f>
-        <v>2</v>
+      <c r="A53" s="1">
+        <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D53" t="s">
         <v>36</v>
@@ -4207,11 +4217,11 @@
         <v>4</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>NewcastleDeliverTRUCKGP</v>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O53">
@@ -4219,20 +4229,19 @@
         <v>0</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>NewcastleDeliverGP</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" cm="1">
-        <f t="array" ref="A54">IF(ISNA(_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53)),IF(COUNTIFS($P$2:P54,P54)=1,IF(COUNTIFS($C$2:C53,C54)=0,1,_xlfn.MAXIFS($A$2:A53,$C$2:C53,C54)+1),A53),_xlfn.XLOOKUP(P54,$P$2:P53,$A$2:A53))</f>
+      <c r="A54" s="1">
         <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
         <v>33</v>
@@ -4250,7 +4259,7 @@
         <v>35</v>
       </c>
       <c r="I54" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J54" t="s">
         <v>36</v>
@@ -4259,11 +4268,11 @@
         <v>2</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>MelbourneStoreGP_STOREGP</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="O54">
@@ -4271,20 +4280,19 @@
         <v>1</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MelbourneStoreGP</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" cm="1">
-        <f t="array" ref="A55">IF(ISNA(_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54)),IF(COUNTIFS($P$2:P55,P55)=1,IF(COUNTIFS($C$2:C54,C55)=0,1,_xlfn.MAXIFS($A$2:A54,$C$2:C54,C55)+1),A54),_xlfn.XLOOKUP(P55,$P$2:P54,$A$2:A54))</f>
+      <c r="A55" s="1">
         <v>2</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
         <v>36</v>
@@ -4302,11 +4310,11 @@
         <v>4</v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>MelbourneDeliverTRUCKGP</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O55">
@@ -4314,20 +4322,19 @@
         <v>0</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MelbourneDeliverGP</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" cm="1">
-        <f t="array" ref="A56">IF(ISNA(_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55)),IF(COUNTIFS($P$2:P56,P56)=1,IF(COUNTIFS($C$2:C55,C56)=0,1,_xlfn.MAXIFS($A$2:A55,$C$2:C55,C56)+1),A55),_xlfn.XLOOKUP(P56,$P$2:P55,$A$2:A55))</f>
+      <c r="A56" s="1">
         <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="D56" t="s">
         <v>33</v>
@@ -4345,7 +4352,7 @@
         <v>35</v>
       </c>
       <c r="I56" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="J56" t="s">
         <v>36</v>
@@ -4354,11 +4361,11 @@
         <v>2</v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>OsborneStoreGP_STOREGP</v>
       </c>
       <c r="N56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OsborneDeliverTRUCKGP</v>
       </c>
       <c r="O56">
@@ -4366,20 +4373,19 @@
         <v>1</v>
       </c>
       <c r="P56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>OsborneStoreGP</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" cm="1">
-        <f t="array" ref="A57">IF(ISNA(_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56)),IF(COUNTIFS($P$2:P57,P57)=1,IF(COUNTIFS($C$2:C56,C57)=0,1,_xlfn.MAXIFS($A$2:A56,$C$2:C56,C57)+1),A56),_xlfn.XLOOKUP(P57,$P$2:P56,$A$2:A56))</f>
+      <c r="A57" s="1">
         <v>2</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
         <v>36</v>
@@ -4397,11 +4403,11 @@
         <v>4</v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>OsborneDeliverTRUCKGP</v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O57">
@@ -4409,20 +4415,19 @@
         <v>0</v>
       </c>
       <c r="P57" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>OsborneDeliverGP</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" cm="1">
-        <f t="array" ref="A58">IF(ISNA(_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57)),IF(COUNTIFS($P$2:P58,P58)=1,IF(COUNTIFS($C$2:C57,C58)=0,1,_xlfn.MAXIFS($A$2:A57,$C$2:C57,C58)+1),A57),_xlfn.XLOOKUP(P58,$P$2:P57,$A$2:A57))</f>
+      <c r="A58" s="1">
         <v>1</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
         <v>33</v>
@@ -4440,7 +4445,7 @@
         <v>35</v>
       </c>
       <c r="I58" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="J58" t="s">
         <v>36</v>
@@ -4449,11 +4454,11 @@
         <v>2</v>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>TownsvilleStoreGP_STOREGP</v>
       </c>
       <c r="N58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="O58">
@@ -4461,20 +4466,19 @@
         <v>1</v>
       </c>
       <c r="P58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>TownsvilleStoreGP</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" cm="1">
-        <f t="array" ref="A59">IF(ISNA(_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58)),IF(COUNTIFS($P$2:P59,P59)=1,IF(COUNTIFS($C$2:C58,C59)=0,1,_xlfn.MAXIFS($A$2:A58,$C$2:C58,C59)+1),A58),_xlfn.XLOOKUP(P59,$P$2:P58,$A$2:A58))</f>
+      <c r="A59" s="1">
         <v>2</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
         <v>36</v>
@@ -4492,11 +4496,11 @@
         <v>4</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>TownsvilleDeliverTRUCKGP</v>
       </c>
       <c r="N59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O59">
@@ -4504,20 +4508,19 @@
         <v>0</v>
       </c>
       <c r="P59" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>TownsvilleDeliverGP</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" cm="1">
-        <f t="array" ref="A60">IF(ISNA(_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59)),IF(COUNTIFS($P$2:P60,P60)=1,IF(COUNTIFS($C$2:C59,C60)=0,1,_xlfn.MAXIFS($A$2:A59,$C$2:C59,C60)+1),A59),_xlfn.XLOOKUP(P60,$P$2:P59,$A$2:A59))</f>
+      <c r="A60" s="1">
         <v>1</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
         <v>33</v>
@@ -4535,7 +4538,7 @@
         <v>35</v>
       </c>
       <c r="I60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J60" t="s">
         <v>36</v>
@@ -4544,11 +4547,11 @@
         <v>2</v>
       </c>
       <c r="M60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>MackayStoreGP_STOREGP</v>
       </c>
       <c r="N60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="O60">
@@ -4556,20 +4559,19 @@
         <v>1</v>
       </c>
       <c r="P60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MackayStoreGP</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" cm="1">
-        <f t="array" ref="A61">IF(ISNA(_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60)),IF(COUNTIFS($P$2:P61,P61)=1,IF(COUNTIFS($C$2:C60,C61)=0,1,_xlfn.MAXIFS($A$2:A60,$C$2:C60,C61)+1),A60),_xlfn.XLOOKUP(P61,$P$2:P60,$A$2:A60))</f>
+      <c r="A61" s="1">
         <v>2</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D61" t="s">
         <v>36</v>
@@ -4587,11 +4589,11 @@
         <v>4</v>
       </c>
       <c r="M61" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>MackayDeliverTRUCKGP</v>
       </c>
       <c r="N61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O61">
@@ -4599,20 +4601,19 @@
         <v>0</v>
       </c>
       <c r="P61" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MackayDeliverGP</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" cm="1">
-        <f t="array" ref="A62">IF(ISNA(_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61)),IF(COUNTIFS($P$2:P62,P62)=1,IF(COUNTIFS($C$2:C61,C62)=0,1,_xlfn.MAXIFS($A$2:A61,$C$2:C61,C62)+1),A61),_xlfn.XLOOKUP(P62,$P$2:P61,$A$2:A61))</f>
+      <c r="A62" s="1">
         <v>1</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D62" t="s">
         <v>33</v>
@@ -4630,7 +4631,7 @@
         <v>35</v>
       </c>
       <c r="I62" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J62" t="s">
         <v>36</v>
@@ -4639,11 +4640,11 @@
         <v>2</v>
       </c>
       <c r="M62" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>WaggaStoreGP_STOREGP</v>
       </c>
       <c r="N62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="O62">
@@ -4651,20 +4652,19 @@
         <v>1</v>
       </c>
       <c r="P62" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>WaggaStoreGP</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" cm="1">
-        <f t="array" ref="A63">IF(ISNA(_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62)),IF(COUNTIFS($P$2:P63,P63)=1,IF(COUNTIFS($C$2:C62,C63)=0,1,_xlfn.MAXIFS($A$2:A62,$C$2:C62,C63)+1),A62),_xlfn.XLOOKUP(P63,$P$2:P62,$A$2:A62))</f>
+      <c r="A63" s="1">
         <v>2</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
         <v>36</v>
@@ -4682,11 +4682,11 @@
         <v>4</v>
       </c>
       <c r="M63" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>WaggaDeliverTRUCKGP</v>
       </c>
       <c r="N63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>GP</v>
       </c>
       <c r="O63">
@@ -4694,20 +4694,19 @@
         <v>0</v>
       </c>
       <c r="P63" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>WaggaDeliverGP</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" cm="1">
-        <f t="array" ref="A64">IF(ISNA(_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63)),IF(COUNTIFS($P$2:P64,P64)=1,IF(COUNTIFS($C$2:C63,C64)=0,1,_xlfn.MAXIFS($A$2:A63,$C$2:C63,C64)+1),A63),_xlfn.XLOOKUP(P64,$P$2:P63,$A$2:A63))</f>
+      <c r="A64" s="1">
         <v>1</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D64" t="s">
         <v>33</v>
@@ -4725,7 +4724,7 @@
         <v>35</v>
       </c>
       <c r="I64" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J64" t="s">
         <v>36</v>
@@ -4734,11 +4733,11 @@
         <v>2</v>
       </c>
       <c r="M64" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>AlburyStoreGP_STOREGP</v>
       </c>
       <c r="N64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="O64">
@@ -4746,20 +4745,19 @@
         <v>1</v>
       </c>
       <c r="P64" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>AlburyStoreGP</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" cm="1">
-        <f t="array" ref="A65">IF(ISNA(_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64)),IF(COUNTIFS($P$2:P65,P65)=1,IF(COUNTIFS($C$2:C64,C65)=0,1,_xlfn.MAXIFS($A$2:A64,$C$2:C64,C65)+1),A64),_xlfn.XLOOKUP(P65,$P$2:P64,$A$2:A64))</f>
+      <c r="A65" s="1">
         <v>2</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D65" t="s">
         <v>36</v>
@@ -4777,24 +4775,23 @@
         <v>4</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>AlburyDeliverTRUCKGP</v>
       </c>
       <c r="P65" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>AlburyDeliverGP</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" cm="1">
-        <f t="array" ref="A66">IF(ISNA(_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65)),IF(COUNTIFS($P$2:P66,P66)=1,IF(COUNTIFS($C$2:C65,C66)=0,1,_xlfn.MAXIFS($A$2:A65,$C$2:C65,C66)+1),A65),_xlfn.XLOOKUP(P66,$P$2:P65,$A$2:A65))</f>
+      <c r="A66" s="1">
         <v>1</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" t="s">
         <v>33</v>
@@ -4812,7 +4809,7 @@
         <v>35</v>
       </c>
       <c r="I66" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J66" t="s">
         <v>36</v>
@@ -4821,24 +4818,23 @@
         <v>2</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>ClydeStoreGP_STOREGP</v>
       </c>
       <c r="P66" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>ClydeStoreGP</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" cm="1">
-        <f t="array" ref="A67">IF(ISNA(_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66)),IF(COUNTIFS($P$2:P67,P67)=1,IF(COUNTIFS($C$2:C66,C67)=0,1,_xlfn.MAXIFS($A$2:A66,$C$2:C66,C67)+1),A66),_xlfn.XLOOKUP(P67,$P$2:P66,$A$2:A66))</f>
+      <c r="A67" s="1">
         <v>2</v>
       </c>
       <c r="B67" t="s">
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D67" t="s">
         <v>36</v>
@@ -4856,11 +4852,11 @@
         <v>4</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>ClydeDeliverTRUCKGP</v>
       </c>
       <c r="P67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>ClydeDeliverGP</v>
       </c>
     </row>
@@ -4869,34 +4865,37 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D68" t="s">
-        <v>95</v>
+        <v>33</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G68" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H68" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I68" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="J68" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="K68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P68" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>GladstoneMakeFA</v>
       </c>
     </row>
@@ -4905,39 +4904,30 @@
         <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D69" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="E69" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G69" t="s">
-        <v>53</v>
-      </c>
-      <c r="H69" t="s">
-        <v>28</v>
-      </c>
-      <c r="I69" t="s">
-        <v>20</v>
-      </c>
-      <c r="J69" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="K69">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B70" t="s">
         <v>53</v>
@@ -4946,13 +4936,10 @@
         <v>20</v>
       </c>
       <c r="D70" t="s">
-        <v>29</v>
-      </c>
-      <c r="E70" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="F70" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G70" t="s">
         <v>53</v>
@@ -4961,18 +4948,18 @@
         <v>25</v>
       </c>
       <c r="I70" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="J70" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="K70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
         <v>53</v>
@@ -4981,28 +4968,28 @@
         <v>20</v>
       </c>
       <c r="D71" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="E71" t="s">
         <v>53</v>
       </c>
       <c r="F71" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G71" t="s">
         <v>53</v>
       </c>
       <c r="H71" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I71" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J71" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="K71">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -5031,7 +5018,7 @@
         <v>25</v>
       </c>
       <c r="I72" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="J72" t="s">
         <v>54</v>
@@ -5042,72 +5029,72 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B73" t="s">
         <v>53</v>
       </c>
       <c r="C73" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D73" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E73" t="s">
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G73" t="s">
         <v>53</v>
       </c>
       <c r="H73" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I73" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J73" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="K73">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
         <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E74" t="s">
         <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G74" t="s">
         <v>53</v>
       </c>
       <c r="H74" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I74" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="J74" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="K74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -5118,7 +5105,7 @@
         <v>53</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="D75" t="s">
         <v>54</v>
@@ -5136,7 +5123,7 @@
         <v>35</v>
       </c>
       <c r="I75" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="J75" t="s">
         <v>36</v>
@@ -5147,54 +5134,72 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
         <v>53</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D76" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G76" t="s">
         <v>53</v>
       </c>
+      <c r="H76" t="s">
+        <v>35</v>
+      </c>
+      <c r="I76" t="s">
+        <v>38</v>
+      </c>
+      <c r="J76" t="s">
+        <v>36</v>
+      </c>
       <c r="K76">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B77" t="s">
         <v>53</v>
       </c>
       <c r="C77" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="D77" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E77" t="s">
         <v>53</v>
       </c>
       <c r="F77" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G77" t="s">
         <v>53</v>
       </c>
+      <c r="H77" t="s">
+        <v>35</v>
+      </c>
+      <c r="I77" t="s">
+        <v>146</v>
+      </c>
+      <c r="J77" t="s">
+        <v>36</v>
+      </c>
       <c r="K77">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -5205,7 +5210,7 @@
         <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="D78" t="s">
         <v>36</v>
@@ -5225,37 +5230,28 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C79" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="D79" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="E79" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F79" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>65</v>
-      </c>
-      <c r="H79" t="s">
-        <v>28</v>
-      </c>
-      <c r="I79" t="s">
-        <v>148</v>
-      </c>
-      <c r="J79" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="K79">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -5263,39 +5259,30 @@
         <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C80" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D80" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E80" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F80" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G80" t="s">
-        <v>65</v>
-      </c>
-      <c r="H80" t="s">
-        <v>25</v>
-      </c>
-      <c r="I80" t="s">
-        <v>38</v>
-      </c>
-      <c r="J80" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="K80">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B81" t="s">
         <v>63</v>
@@ -5304,45 +5291,48 @@
         <v>148</v>
       </c>
       <c r="D81" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E81" t="s">
         <v>65</v>
       </c>
       <c r="F81" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G81" t="s">
         <v>65</v>
       </c>
       <c r="H81" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I81" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="J81" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="K81">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
         <v>63</v>
       </c>
       <c r="C82" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="D82" t="s">
-        <v>176</v>
+        <v>29</v>
+      </c>
+      <c r="E82" t="s">
+        <v>65</v>
       </c>
       <c r="F82" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G82" t="s">
         <v>65</v>
@@ -5351,18 +5341,18 @@
         <v>25</v>
       </c>
       <c r="I82" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J82" t="s">
         <v>64</v>
       </c>
       <c r="K82">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B83" t="s">
         <v>63</v>
@@ -5371,33 +5361,30 @@
         <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="F83" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G83" t="s">
         <v>65</v>
       </c>
       <c r="H83" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I83" t="s">
         <v>38</v>
       </c>
       <c r="J83" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="K83">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B84" t="s">
         <v>63</v>
@@ -5406,33 +5393,33 @@
         <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E84" t="s">
         <v>65</v>
       </c>
       <c r="F84" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" t="s">
+        <v>65</v>
+      </c>
+      <c r="H84" t="s">
         <v>23</v>
-      </c>
-      <c r="G84" t="s">
-        <v>63</v>
-      </c>
-      <c r="H84" t="s">
-        <v>25</v>
       </c>
       <c r="I84" t="s">
         <v>38</v>
       </c>
       <c r="J84" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="K84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
         <v>63</v>
@@ -5441,33 +5428,33 @@
         <v>38</v>
       </c>
       <c r="D85" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E85" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F85" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" t="s">
+        <v>63</v>
+      </c>
+      <c r="H85" t="s">
         <v>25</v>
-      </c>
-      <c r="G85" t="s">
-        <v>63</v>
-      </c>
-      <c r="H85" t="s">
-        <v>35</v>
       </c>
       <c r="I85" t="s">
         <v>38</v>
       </c>
       <c r="J85" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K85">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
         <v>63</v>
@@ -5476,24 +5463,33 @@
         <v>38</v>
       </c>
       <c r="D86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E86" t="s">
+        <v>63</v>
+      </c>
+      <c r="F86" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" t="s">
+        <v>63</v>
+      </c>
+      <c r="H86" t="s">
+        <v>35</v>
+      </c>
+      <c r="I86" t="s">
+        <v>38</v>
+      </c>
+      <c r="J86" t="s">
         <v>36</v>
       </c>
-      <c r="E86" t="s">
-        <v>63</v>
-      </c>
-      <c r="F86" t="s">
-        <v>35</v>
-      </c>
-      <c r="G86" t="s">
-        <v>63</v>
-      </c>
       <c r="K86">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
         <v>63</v>
@@ -5502,28 +5498,19 @@
         <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E87" t="s">
         <v>63</v>
       </c>
       <c r="F87" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G87" t="s">
         <v>63</v>
       </c>
-      <c r="H87" t="s">
-        <v>28</v>
-      </c>
-      <c r="I87" t="s">
-        <v>38</v>
-      </c>
-      <c r="J87" t="s">
-        <v>29</v>
-      </c>
       <c r="K87">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -5555,7 +5542,7 @@
         <v>38</v>
       </c>
       <c r="J88" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K88">
         <v>2</v>
@@ -5563,7 +5550,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
         <v>63</v>
@@ -5572,28 +5559,28 @@
         <v>38</v>
       </c>
       <c r="D89" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E89" t="s">
         <v>63</v>
       </c>
       <c r="F89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" t="s">
+        <v>63</v>
+      </c>
+      <c r="H89" t="s">
         <v>28</v>
       </c>
-      <c r="G89" t="s">
-        <v>63</v>
-      </c>
-      <c r="H89" t="s">
-        <v>25</v>
-      </c>
       <c r="I89" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J89" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="K89">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -5607,7 +5594,7 @@
         <v>38</v>
       </c>
       <c r="D90" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E90" t="s">
         <v>63</v>
@@ -5622,7 +5609,7 @@
         <v>25</v>
       </c>
       <c r="I90" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J90" t="s">
         <v>66</v>
@@ -5657,7 +5644,7 @@
         <v>25</v>
       </c>
       <c r="I91" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="J91" t="s">
         <v>66</v>
@@ -5692,7 +5679,7 @@
         <v>25</v>
       </c>
       <c r="I92" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="J92" t="s">
         <v>66</v>
@@ -5703,37 +5690,37 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B93" t="s">
         <v>63</v>
       </c>
       <c r="C93" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D93" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E93" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F93" t="s">
+        <v>28</v>
+      </c>
+      <c r="G93" t="s">
+        <v>63</v>
+      </c>
+      <c r="H93" t="s">
         <v>25</v>
       </c>
-      <c r="G93" t="s">
-        <v>65</v>
-      </c>
-      <c r="H93" t="s">
-        <v>23</v>
-      </c>
       <c r="I93" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J93" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="K93">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -5765,7 +5752,7 @@
         <v>30</v>
       </c>
       <c r="J94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K94">
         <v>2</v>
@@ -5773,7 +5760,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B95" t="s">
         <v>63</v>
@@ -5782,28 +5769,28 @@
         <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E95" t="s">
         <v>65</v>
       </c>
       <c r="F95" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" t="s">
+        <v>65</v>
+      </c>
+      <c r="H95" t="s">
         <v>23</v>
-      </c>
-      <c r="G95" t="s">
-        <v>63</v>
-      </c>
-      <c r="H95" t="s">
-        <v>25</v>
       </c>
       <c r="I95" t="s">
         <v>30</v>
       </c>
       <c r="J95" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="K95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -5817,7 +5804,7 @@
         <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s">
         <v>65</v>
@@ -5843,7 +5830,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
         <v>63</v>
@@ -5852,28 +5839,28 @@
         <v>30</v>
       </c>
       <c r="D97" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E97" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F97" t="s">
+        <v>23</v>
+      </c>
+      <c r="G97" t="s">
+        <v>63</v>
+      </c>
+      <c r="H97" t="s">
         <v>25</v>
-      </c>
-      <c r="G97" t="s">
-        <v>63</v>
-      </c>
-      <c r="H97" t="s">
-        <v>28</v>
       </c>
       <c r="I97" t="s">
         <v>30</v>
       </c>
       <c r="J97" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="K97">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -5899,13 +5886,13 @@
         <v>63</v>
       </c>
       <c r="H98" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I98" t="s">
         <v>30</v>
       </c>
       <c r="J98" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K98">
         <v>2</v>
@@ -5913,7 +5900,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B99" t="s">
         <v>63</v>
@@ -5922,28 +5909,28 @@
         <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E99" t="s">
         <v>63</v>
       </c>
       <c r="F99" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G99" t="s">
         <v>63</v>
       </c>
       <c r="H99" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I99" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="J99" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="K99">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -5957,59 +5944,59 @@
         <v>30</v>
       </c>
       <c r="D100" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E100" t="s">
         <v>63</v>
       </c>
       <c r="F100" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G100" t="s">
         <v>63</v>
       </c>
+      <c r="H100" t="s">
+        <v>25</v>
+      </c>
+      <c r="I100" t="s">
+        <v>67</v>
+      </c>
+      <c r="J100" t="s">
+        <v>66</v>
+      </c>
       <c r="K100">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B101" t="s">
         <v>63</v>
       </c>
       <c r="C101" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E101" t="s">
         <v>63</v>
       </c>
       <c r="F101" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G101" t="s">
         <v>63</v>
       </c>
-      <c r="H101" t="s">
-        <v>35</v>
-      </c>
-      <c r="I101" t="s">
-        <v>67</v>
-      </c>
-      <c r="J101" t="s">
-        <v>36</v>
-      </c>
       <c r="K101">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B102" t="s">
         <v>63</v>
@@ -6018,59 +6005,59 @@
         <v>67</v>
       </c>
       <c r="D102" t="s">
+        <v>66</v>
+      </c>
+      <c r="E102" t="s">
+        <v>63</v>
+      </c>
+      <c r="F102" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" t="s">
+        <v>63</v>
+      </c>
+      <c r="H102" t="s">
+        <v>35</v>
+      </c>
+      <c r="I102" t="s">
+        <v>67</v>
+      </c>
+      <c r="J102" t="s">
         <v>36</v>
       </c>
-      <c r="E102" t="s">
-        <v>63</v>
-      </c>
-      <c r="F102" t="s">
-        <v>35</v>
-      </c>
-      <c r="G102" t="s">
-        <v>63</v>
-      </c>
       <c r="K102">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
         <v>63</v>
       </c>
       <c r="C103" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="D103" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E103" t="s">
         <v>63</v>
       </c>
       <c r="F103" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G103" t="s">
         <v>63</v>
       </c>
-      <c r="H103" t="s">
-        <v>35</v>
-      </c>
-      <c r="I103" t="s">
-        <v>45</v>
-      </c>
-      <c r="J103" t="s">
-        <v>36</v>
-      </c>
       <c r="K103">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B104" t="s">
         <v>63</v>
@@ -6079,59 +6066,59 @@
         <v>45</v>
       </c>
       <c r="D104" t="s">
+        <v>66</v>
+      </c>
+      <c r="E104" t="s">
+        <v>63</v>
+      </c>
+      <c r="F104" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" t="s">
+        <v>63</v>
+      </c>
+      <c r="H104" t="s">
+        <v>35</v>
+      </c>
+      <c r="I104" t="s">
+        <v>45</v>
+      </c>
+      <c r="J104" t="s">
         <v>36</v>
       </c>
-      <c r="E104" t="s">
-        <v>63</v>
-      </c>
-      <c r="F104" t="s">
-        <v>35</v>
-      </c>
-      <c r="G104" t="s">
-        <v>63</v>
-      </c>
       <c r="K104">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
         <v>63</v>
       </c>
       <c r="C105" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D105" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E105" t="s">
         <v>63</v>
       </c>
       <c r="F105" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G105" t="s">
         <v>63</v>
       </c>
-      <c r="H105" t="s">
-        <v>35</v>
-      </c>
-      <c r="I105" t="s">
-        <v>52</v>
-      </c>
-      <c r="J105" t="s">
-        <v>36</v>
-      </c>
       <c r="K105">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B106" t="s">
         <v>63</v>
@@ -6140,59 +6127,59 @@
         <v>52</v>
       </c>
       <c r="D106" t="s">
+        <v>66</v>
+      </c>
+      <c r="E106" t="s">
+        <v>63</v>
+      </c>
+      <c r="F106" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" t="s">
+        <v>63</v>
+      </c>
+      <c r="H106" t="s">
+        <v>35</v>
+      </c>
+      <c r="I106" t="s">
+        <v>52</v>
+      </c>
+      <c r="J106" t="s">
         <v>36</v>
       </c>
-      <c r="E106" t="s">
-        <v>63</v>
-      </c>
-      <c r="F106" t="s">
-        <v>35</v>
-      </c>
-      <c r="G106" t="s">
-        <v>63</v>
-      </c>
       <c r="K106">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
         <v>63</v>
       </c>
       <c r="C107" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D107" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E107" t="s">
         <v>63</v>
       </c>
       <c r="F107" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G107" t="s">
         <v>63</v>
       </c>
-      <c r="H107" t="s">
-        <v>35</v>
-      </c>
-      <c r="I107" t="s">
-        <v>68</v>
-      </c>
-      <c r="J107" t="s">
-        <v>36</v>
-      </c>
       <c r="K107">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B108" t="s">
         <v>63</v>
@@ -6201,59 +6188,59 @@
         <v>68</v>
       </c>
       <c r="D108" t="s">
+        <v>66</v>
+      </c>
+      <c r="E108" t="s">
+        <v>63</v>
+      </c>
+      <c r="F108" t="s">
+        <v>25</v>
+      </c>
+      <c r="G108" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108" t="s">
+        <v>35</v>
+      </c>
+      <c r="I108" t="s">
+        <v>68</v>
+      </c>
+      <c r="J108" t="s">
         <v>36</v>
       </c>
-      <c r="E108" t="s">
-        <v>63</v>
-      </c>
-      <c r="F108" t="s">
-        <v>35</v>
-      </c>
-      <c r="G108" t="s">
-        <v>63</v>
-      </c>
       <c r="K108">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
         <v>63</v>
       </c>
       <c r="C109" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D109" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E109" t="s">
         <v>63</v>
       </c>
       <c r="F109" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G109" t="s">
         <v>63</v>
       </c>
-      <c r="H109" t="s">
-        <v>35</v>
-      </c>
-      <c r="I109" t="s">
-        <v>39</v>
-      </c>
-      <c r="J109" t="s">
-        <v>36</v>
-      </c>
       <c r="K109">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B110" t="s">
         <v>63</v>
@@ -6262,23 +6249,58 @@
         <v>39</v>
       </c>
       <c r="D110" t="s">
+        <v>66</v>
+      </c>
+      <c r="E110" t="s">
+        <v>63</v>
+      </c>
+      <c r="F110" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" t="s">
+        <v>63</v>
+      </c>
+      <c r="H110" t="s">
+        <v>35</v>
+      </c>
+      <c r="I110" t="s">
+        <v>39</v>
+      </c>
+      <c r="J110" t="s">
         <v>36</v>
       </c>
-      <c r="E110" t="s">
-        <v>63</v>
-      </c>
-      <c r="F110" t="s">
+      <c r="K110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>2</v>
+      </c>
+      <c r="B111" t="s">
+        <v>63</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="s">
+        <v>36</v>
+      </c>
+      <c r="E111" t="s">
+        <v>63</v>
+      </c>
+      <c r="F111" t="s">
         <v>35</v>
       </c>
-      <c r="G110" t="s">
-        <v>63</v>
-      </c>
-      <c r="K110">
+      <c r="G111" t="s">
+        <v>63</v>
+      </c>
+      <c r="K111">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K110" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:K111" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="M1:N1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -6289,10 +6311,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I10" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6561,13 +6583,16 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -6575,7 +6600,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="19">
         <v>1</v>
       </c>
     </row>
@@ -6584,28 +6609,22 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="E11">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="H11" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="I11" s="10">
-        <v>0.88</v>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6616,13 +6635,13 @@
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E12">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -6634,34 +6653,36 @@
         <v>0.05</v>
       </c>
       <c r="I12" s="10">
-        <v>1</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E13">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="H13" s="10">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="I13" s="10">
-        <v>0.88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6669,7 +6690,7 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -6678,7 +6699,7 @@
         <v>19</v>
       </c>
       <c r="E14">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -6696,24 +6717,51 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E15">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H16" s="10">
         <v>2.98E-2</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I16" s="10">
         <v>1</v>
       </c>
     </row>
@@ -6724,10 +6772,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H35"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7635,10 +7683,10 @@
         <v>19</v>
       </c>
       <c r="D28" s="9">
-        <v>30000</v>
+        <v>14500</v>
       </c>
       <c r="E28" s="3">
-        <v>30000</v>
+        <v>14500</v>
       </c>
       <c r="F28" s="3">
         <v>5000</v>
@@ -7647,14 +7695,14 @@
         <v>0</v>
       </c>
       <c r="H28" s="3">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" t="s">
         <v>27</v>
       </c>
       <c r="K28" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7662,55 +7710,55 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="3">
-        <v>20000</v>
+        <v>19</v>
+      </c>
+      <c r="D29" s="9">
+        <v>30000</v>
       </c>
       <c r="E29" s="3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F29" s="3">
         <v>5000</v>
       </c>
       <c r="G29" s="3">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" t="s">
         <v>27</v>
       </c>
       <c r="K29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="D30" s="3">
-        <v>115000</v>
+        <v>20000</v>
       </c>
       <c r="E30" s="3">
-        <v>115000</v>
+        <v>20000</v>
       </c>
       <c r="F30" s="3">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H30" s="3">
         <v>0</v>
@@ -7720,7 +7768,7 @@
         <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7728,19 +7776,19 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3">
-        <v>1500</v>
+        <v>115000</v>
       </c>
       <c r="E31" s="3">
-        <v>1500</v>
+        <v>115000</v>
       </c>
       <c r="F31" s="3">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -7753,7 +7801,7 @@
         <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7761,16 +7809,16 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="3">
-        <v>3600</v>
+        <v>1500</v>
       </c>
       <c r="E32" s="3">
-        <v>3600</v>
+        <v>1500</v>
       </c>
       <c r="F32" s="3">
         <v>500</v>
@@ -7786,24 +7834,24 @@
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="D33" s="3">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="E33" s="3">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="F33" s="3">
         <v>500</v>
@@ -7816,48 +7864,48 @@
       </c>
       <c r="I33" s="3"/>
       <c r="J33" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="K33" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D34" s="3">
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="E34" s="3">
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="F34" s="3">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
       </c>
       <c r="H34" s="3">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="K34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -7866,34 +7914,67 @@
         <v>19</v>
       </c>
       <c r="D35" s="3">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="E35" s="3">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="F35" s="3">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
       </c>
       <c r="H35" s="3">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3000</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3000</v>
+      </c>
+      <c r="F36" s="3">
+        <v>500</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" t="s">
         <v>74</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K36" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H35" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L35">
-    <sortCondition ref="A2:A35"/>
-    <sortCondition ref="B2:B35"/>
-    <sortCondition ref="C2:C35"/>
+  <autoFilter ref="A1:H36" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L36">
+    <sortCondition ref="A2:A36"/>
+    <sortCondition ref="B2:B36"/>
+    <sortCondition ref="C2:C36"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7903,8 +7984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8339,7 +8420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA5544C-34DA-4E23-978C-2BA3091E3A4F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8809,7 +8892,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8889,16 +8972,16 @@
         <v>149</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>5000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8915,10 +8998,10 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>5000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9161,8 +9244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344567A9-6C72-4B48-AD7D-7F7718ACFC30}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:T20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9714,13 +9797,13 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="H11" t="s">
         <v>54</v>
@@ -9977,6 +10060,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
@@ -9987,7 +10079,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E219A9FF51DF7F40A2797E30E842AF22" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14cd91dac819157c91b1d14f281b7de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef0ff67e-9087-4832-8b9d-0b53066cc775" xmlns:ns3="89e87ded-6359-4f8b-890f-4b93e2ce9d62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59d8e09582726c96a64897b0d147333a" ns2:_="" ns3:_="">
     <xsd:import namespace="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
@@ -10242,16 +10334,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACAF3F0-A2CA-497B-8705-2777094C916D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10262,7 +10353,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109886AA-45CB-43C9-9308-75A4553674A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10279,12 +10370,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1FDA4F6-8237-4AAA-84B8-AECFD549038D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Shipping Logic still in progress - Slow Grind - 24 Dec 2025. Expanded multi store supply to Delivery and Train Movements.
</commit_message>
<xml_diff>
--- a/Model Inputs.xlsx
+++ b/Model Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F5EE4BD-4B17-401B-9CD0-67BAF3D46223}"/>
+  <xr:revisionPtr revIDLastSave="360" documentId="13_ncr:1_{2588B9DF-2B1B-45CC-AAB1-3FBB567B5864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9D16FE-5941-43A3-A03B-45F99E49E991}"/>
   <bookViews>
-    <workbookView xWindow="31890" yWindow="870" windowWidth="28770" windowHeight="15450" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{1AEEAFBB-14E9-4895-ADA0-281549BC4509}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="SHIP_BERTHS" sheetId="11" r:id="rId8"/>
     <sheet name="SHIP_ROUTES" sheetId="12" r:id="rId9"/>
     <sheet name="SHIP_DISTANCES" sheetId="13" r:id="rId10"/>
+    <sheet name="Move_CONVEYOR" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Deliver!$A$1:$E$23</definedName>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="223">
   <si>
     <t>Value</t>
   </si>
@@ -593,9 +594,6 @@
     <t>Existing 7 Silos</t>
   </si>
   <si>
-    <t>CONVEYOR</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -732,6 +730,15 @@
   </si>
   <si>
     <t>Output Controls</t>
+  </si>
+  <si>
+    <t>conveyor_speed</t>
+  </si>
+  <si>
+    <t>The speed at which a conveyor can move product from one store to another.</t>
+  </si>
+  <si>
+    <t>Speed (tons/hr)</t>
   </si>
 </sst>
 </file>
@@ -779,6 +786,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1241,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,262 +1264,276 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>365</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>180</v>
       </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>181</v>
-      </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>217</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" t="s">
-        <v>202</v>
+      <c r="A9" s="19" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>185</v>
       </c>
-      <c r="D10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>218</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>181</v>
-      </c>
-      <c r="D13" t="s">
-        <v>204</v>
+      <c r="A13" s="19" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14">
+        <v>186</v>
+      </c>
+      <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B16">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>219</v>
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>185</v>
-      </c>
-      <c r="D19" t="s">
-        <v>208</v>
+      <c r="A19" s="19" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" t="s">
-        <v>215</v>
+        <v>190</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
+        <v>214</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>220</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>195</v>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D24" t="s">
-        <v>211</v>
+      <c r="A24" s="19" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B26" t="s">
-        <v>216</v>
+        <v>195</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D26" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1748,12 +1770,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E675B-CAFA-4298-B424-A8167AFF830C}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4262,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
@@ -4218,13 +4283,13 @@
         <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I46" t="s">
         <v>33</v>
       </c>
       <c r="J46" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
       <c r="K46">
         <v>2</v>
@@ -4248,7 +4313,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
@@ -4257,25 +4322,25 @@
         <v>33</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
       <c r="F47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I47" t="s">
         <v>33</v>
       </c>
       <c r="J47" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -4350,7 +4415,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
         <v>14</v>
@@ -4401,7 +4466,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
@@ -4452,7 +4517,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -4503,7 +4568,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -4554,7 +4619,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
@@ -6672,10 +6737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I11"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6944,16 +7009,13 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E10">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -6970,22 +7032,28 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E11">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18">
-        <v>1</v>
+      <c r="G11" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.88</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6996,13 +7064,13 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E12">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -7014,36 +7082,34 @@
         <v>0.05</v>
       </c>
       <c r="I12" s="9">
-        <v>0.88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="E13">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" s="17" t="s">
-        <v>163</v>
-      </c>
+      <c r="G13" s="17"/>
       <c r="H13" s="9">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="I13" s="9">
-        <v>1</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -7051,7 +7117,7 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -7060,7 +7126,7 @@
         <v>14</v>
       </c>
       <c r="E14">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -7078,51 +7144,24 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
       <c r="E15">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="H15" s="9">
-        <v>0.15</v>
+        <v>2.98E-2</v>
       </c>
       <c r="I15" s="9">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>150</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="H16" s="9">
-        <v>2.98E-2</v>
-      </c>
-      <c r="I16" s="9">
         <v>1</v>
       </c>
     </row>
@@ -7135,7 +7174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>

</xml_diff>